<commit_message>
Add study specific growth rates assumptions
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1971013-3190-4C86-8914-9840BE2B0209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C743D129-2A02-4E47-B28B-4AAEF28F8E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="5565" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -1155,7 +1155,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B2A03571-7FFC-4A97-87EA-3B1CB5DB6A9D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1199,7 +1199,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF4C7E08-57B7-4B69-AA5B-8D8B8B7B8102}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1248,7 +1248,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9755C22-D338-4CCC-8602-285159403FCB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1298,7 +1298,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38BB12B9-6384-42D9-8624-A816371DA3AE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1348,7 +1348,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B857065-E7A8-4C06-9763-F4026263D97D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1397,7 +1397,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E41843CB-8CDF-441F-83B4-D48634C7A4F9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
               <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{B1489C0F-1609-4587-A5BA-D0B99739EA08}"/>
@@ -1807,25 +1807,25 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B20" sqref="B20:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" style="3" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" style="3" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="3" customWidth="1"/>
+    <col min="1" max="4" width="21.73046875" style="3" customWidth="1"/>
+    <col min="5" max="6" width="14.1328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.1328125" style="3" customWidth="1"/>
+    <col min="8" max="10" width="8.1328125" style="3" customWidth="1"/>
+    <col min="11" max="11" width="9.73046875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="8.1328125" style="3" customWidth="1"/>
     <col min="13" max="13" width="10" style="3" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" style="3" customWidth="1"/>
-    <col min="16" max="16384" width="8.85546875" style="3"/>
+    <col min="14" max="14" width="11.3984375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="13.3984375" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="8.86328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
       <c r="C1" s="38"/>
@@ -1853,7 +1853,7 @@
       <c r="Y1" s="39"/>
       <c r="Z1" s="39"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A2" s="38"/>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
@@ -1881,7 +1881,7 @@
       <c r="Y2" s="39"/>
       <c r="Z2" s="39"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A3" s="38"/>
       <c r="B3" s="38"/>
       <c r="C3" s="38"/>
@@ -1909,7 +1909,7 @@
       <c r="Y3" s="39"/>
       <c r="Z3" s="39"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A4" s="38"/>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
@@ -1937,7 +1937,7 @@
       <c r="Y4" s="39"/>
       <c r="Z4" s="39"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A5" s="38"/>
       <c r="B5" s="38"/>
       <c r="C5" s="38"/>
@@ -1965,7 +1965,7 @@
       <c r="Y5" s="39"/>
       <c r="Z5" s="39"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A6" s="38"/>
       <c r="B6" s="38"/>
       <c r="C6" s="38"/>
@@ -1993,7 +1993,7 @@
       <c r="Y6" s="39"/>
       <c r="Z6" s="39"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A7" s="38"/>
       <c r="B7" s="38"/>
       <c r="C7" s="38"/>
@@ -2021,7 +2021,7 @@
       <c r="Y7" s="39"/>
       <c r="Z7" s="39"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A8" s="38"/>
       <c r="B8" s="38"/>
       <c r="C8" s="38"/>
@@ -2049,7 +2049,7 @@
       <c r="Y8" s="39"/>
       <c r="Z8" s="39"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A9" s="38"/>
       <c r="B9" s="38"/>
       <c r="C9" s="38"/>
@@ -2077,7 +2077,7 @@
       <c r="Y9" s="39"/>
       <c r="Z9" s="39"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A10" s="38"/>
       <c r="B10" s="38"/>
       <c r="C10" s="38"/>
@@ -2105,7 +2105,7 @@
       <c r="Y10" s="39"/>
       <c r="Z10" s="39"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A11" s="38"/>
       <c r="B11" s="38"/>
       <c r="C11" s="38"/>
@@ -2133,7 +2133,7 @@
       <c r="Y11" s="39"/>
       <c r="Z11" s="39"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A12" s="38"/>
       <c r="B12" s="38"/>
       <c r="C12" s="38"/>
@@ -2161,7 +2161,7 @@
       <c r="Y12" s="39"/>
       <c r="Z12" s="39"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A13" s="38"/>
       <c r="B13" s="38"/>
       <c r="C13" s="38"/>
@@ -2189,7 +2189,7 @@
       <c r="Y13" s="39"/>
       <c r="Z13" s="39"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A14" s="38"/>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
@@ -2217,7 +2217,7 @@
       <c r="Y14" s="39"/>
       <c r="Z14" s="39"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
@@ -2245,7 +2245,7 @@
       <c r="Y15" s="39"/>
       <c r="Z15" s="39"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="54" t="s">
         <v>169</v>
       </c>
@@ -2275,7 +2275,7 @@
       <c r="Y16" s="39"/>
       <c r="Z16" s="39"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="42"/>
       <c r="B17" s="42"/>
       <c r="C17" s="42"/>
@@ -2303,7 +2303,7 @@
       <c r="Y17" s="39"/>
       <c r="Z17" s="39"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
       <c r="C18" s="42"/>
@@ -2331,7 +2331,7 @@
       <c r="Y18" s="39"/>
       <c r="Z18" s="39"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="45" t="s">
         <v>170</v>
       </c>
@@ -2363,7 +2363,7 @@
       <c r="Y19" s="39"/>
       <c r="Z19" s="39"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="45" t="s">
         <v>171</v>
       </c>
@@ -2395,7 +2395,7 @@
       <c r="Y20" s="39"/>
       <c r="Z20" s="39"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="45" t="s">
         <v>172</v>
       </c>
@@ -2427,7 +2427,7 @@
       <c r="Y21" s="39"/>
       <c r="Z21" s="39"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="45"/>
       <c r="B22" s="48"/>
       <c r="C22" s="48"/>
@@ -2455,7 +2455,7 @@
       <c r="Y22" s="39"/>
       <c r="Z22" s="39"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="45" t="s">
         <v>173</v>
       </c>
@@ -2487,7 +2487,7 @@
       <c r="Y23" s="39"/>
       <c r="Z23" s="39"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="45"/>
       <c r="B24" s="53" t="s">
         <v>182</v>
@@ -2517,7 +2517,7 @@
       <c r="Y24" s="39"/>
       <c r="Z24" s="39"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="45"/>
       <c r="B25" s="48" t="s">
         <v>183</v>
@@ -2547,7 +2547,7 @@
       <c r="Y25" s="39"/>
       <c r="Z25" s="39"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="45" t="s">
         <v>174</v>
       </c>
@@ -2579,7 +2579,7 @@
       <c r="Y26" s="39"/>
       <c r="Z26" s="39"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="45"/>
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
@@ -2607,7 +2607,7 @@
       <c r="Y27" s="39"/>
       <c r="Z27" s="39"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="45"/>
       <c r="B28" s="48"/>
       <c r="C28" s="48"/>
@@ -2635,7 +2635,7 @@
       <c r="Y28" s="39"/>
       <c r="Z28" s="39"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="45" t="s">
         <v>175</v>
       </c>
@@ -2667,7 +2667,7 @@
       <c r="Y29" s="39"/>
       <c r="Z29" s="39"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="45" t="s">
         <v>176</v>
       </c>
@@ -2699,7 +2699,7 @@
       <c r="Y30" s="39"/>
       <c r="Z30" s="39"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A31" s="45" t="s">
         <v>178</v>
       </c>
@@ -2731,7 +2731,7 @@
       <c r="Y31" s="39"/>
       <c r="Z31" s="39"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A32" s="51"/>
       <c r="B32" s="52" t="s">
         <v>180</v>
@@ -2761,7 +2761,7 @@
       <c r="Y32" s="39"/>
       <c r="Z32" s="39"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A33" s="38"/>
       <c r="B33" s="38"/>
       <c r="C33" s="38"/>
@@ -2789,7 +2789,7 @@
       <c r="Y33" s="39"/>
       <c r="Z33" s="39"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A34" s="38"/>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
@@ -2817,7 +2817,7 @@
       <c r="Y34" s="39"/>
       <c r="Z34" s="39"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A35" s="38"/>
       <c r="B35" s="38"/>
       <c r="C35" s="38"/>
@@ -2845,7 +2845,7 @@
       <c r="Y35" s="39"/>
       <c r="Z35" s="39"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A36" s="38"/>
       <c r="B36" s="38"/>
       <c r="C36" s="38"/>
@@ -2873,7 +2873,7 @@
       <c r="Y36" s="39"/>
       <c r="Z36" s="39"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A37" s="38"/>
       <c r="B37" s="38"/>
       <c r="C37" s="38"/>
@@ -2901,7 +2901,7 @@
       <c r="Y37" s="39"/>
       <c r="Z37" s="39"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A38" s="38"/>
       <c r="B38" s="38"/>
       <c r="C38" s="38"/>
@@ -2929,7 +2929,7 @@
       <c r="Y38" s="39"/>
       <c r="Z38" s="39"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A39" s="38"/>
       <c r="B39" s="38"/>
       <c r="C39" s="38"/>
@@ -2957,7 +2957,7 @@
       <c r="Y39" s="39"/>
       <c r="Z39" s="39"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A40" s="38"/>
       <c r="B40" s="38"/>
       <c r="C40" s="38"/>
@@ -2985,7 +2985,7 @@
       <c r="Y40" s="39"/>
       <c r="Z40" s="39"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A41" s="38"/>
       <c r="B41" s="38"/>
       <c r="C41" s="38"/>
@@ -3013,7 +3013,7 @@
       <c r="Y41" s="39"/>
       <c r="Z41" s="39"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A42" s="38"/>
       <c r="B42" s="38"/>
       <c r="C42" s="38"/>
@@ -3041,7 +3041,7 @@
       <c r="Y42" s="39"/>
       <c r="Z42" s="39"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A43" s="39"/>
       <c r="B43" s="39"/>
       <c r="C43" s="39"/>
@@ -3069,7 +3069,7 @@
       <c r="Y43" s="39"/>
       <c r="Z43" s="39"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A44" s="39"/>
       <c r="B44" s="39"/>
       <c r="C44" s="39"/>
@@ -3097,7 +3097,7 @@
       <c r="Y44" s="39"/>
       <c r="Z44" s="39"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A45" s="39"/>
       <c r="B45" s="39"/>
       <c r="C45" s="39"/>
@@ -3125,7 +3125,7 @@
       <c r="Y45" s="39"/>
       <c r="Z45" s="39"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A46" s="39"/>
       <c r="B46" s="39"/>
       <c r="C46" s="39"/>
@@ -3153,7 +3153,7 @@
       <c r="Y46" s="39"/>
       <c r="Z46" s="39"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A47" s="39"/>
       <c r="B47" s="39"/>
       <c r="C47" s="39"/>
@@ -3181,7 +3181,7 @@
       <c r="Y47" s="39"/>
       <c r="Z47" s="39"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A48" s="39"/>
       <c r="B48" s="39"/>
       <c r="C48" s="39"/>
@@ -3209,7 +3209,7 @@
       <c r="Y48" s="39"/>
       <c r="Z48" s="39"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A49" s="39"/>
       <c r="B49" s="39"/>
       <c r="C49" s="39"/>
@@ -3237,7 +3237,7 @@
       <c r="Y49" s="39"/>
       <c r="Z49" s="39"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A50" s="39"/>
       <c r="B50" s="39"/>
       <c r="C50" s="39"/>
@@ -3265,7 +3265,7 @@
       <c r="Y50" s="39"/>
       <c r="Z50" s="39"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A51" s="39"/>
       <c r="B51" s="39"/>
       <c r="C51" s="39"/>
@@ -3293,7 +3293,7 @@
       <c r="Y51" s="39"/>
       <c r="Z51" s="39"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A52" s="39"/>
       <c r="B52" s="39"/>
       <c r="C52" s="39"/>
@@ -3321,7 +3321,7 @@
       <c r="Y52" s="39"/>
       <c r="Z52" s="39"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A53" s="39"/>
       <c r="B53" s="39"/>
       <c r="C53" s="39"/>
@@ -3349,7 +3349,7 @@
       <c r="Y53" s="39"/>
       <c r="Z53" s="39"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A54" s="39"/>
       <c r="B54" s="39"/>
       <c r="C54" s="39"/>
@@ -3377,7 +3377,7 @@
       <c r="Y54" s="39"/>
       <c r="Z54" s="39"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A55" s="39"/>
       <c r="B55" s="39"/>
       <c r="C55" s="39"/>
@@ -3405,7 +3405,7 @@
       <c r="Y55" s="39"/>
       <c r="Z55" s="39"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A56" s="39"/>
       <c r="B56" s="39"/>
       <c r="C56" s="39"/>
@@ -3433,7 +3433,7 @@
       <c r="Y56" s="39"/>
       <c r="Z56" s="39"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A57" s="39"/>
       <c r="B57" s="39"/>
       <c r="C57" s="39"/>
@@ -3461,7 +3461,7 @@
       <c r="Y57" s="39"/>
       <c r="Z57" s="39"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A58" s="39"/>
       <c r="B58" s="39"/>
       <c r="C58" s="39"/>
@@ -3489,7 +3489,7 @@
       <c r="Y58" s="39"/>
       <c r="Z58" s="39"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A59" s="39"/>
       <c r="B59" s="39"/>
       <c r="C59" s="39"/>
@@ -3517,7 +3517,7 @@
       <c r="Y59" s="39"/>
       <c r="Z59" s="39"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A60" s="39"/>
       <c r="B60" s="39"/>
       <c r="C60" s="39"/>
@@ -3545,7 +3545,7 @@
       <c r="Y60" s="39"/>
       <c r="Z60" s="39"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A61" s="39"/>
       <c r="B61" s="39"/>
       <c r="C61" s="39"/>
@@ -3573,7 +3573,7 @@
       <c r="Y61" s="39"/>
       <c r="Z61" s="39"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A62" s="39"/>
       <c r="B62" s="39"/>
       <c r="C62" s="39"/>
@@ -3601,7 +3601,7 @@
       <c r="Y62" s="39"/>
       <c r="Z62" s="39"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A63" s="39"/>
       <c r="B63" s="39"/>
       <c r="C63" s="39"/>
@@ -3629,7 +3629,7 @@
       <c r="Y63" s="39"/>
       <c r="Z63" s="39"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A64" s="39"/>
       <c r="B64" s="39"/>
       <c r="C64" s="39"/>
@@ -3657,7 +3657,7 @@
       <c r="Y64" s="39"/>
       <c r="Z64" s="39"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A65" s="39"/>
       <c r="B65" s="39"/>
       <c r="C65" s="39"/>
@@ -3685,7 +3685,7 @@
       <c r="Y65" s="39"/>
       <c r="Z65" s="39"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A66" s="39"/>
       <c r="B66" s="39"/>
       <c r="C66" s="39"/>
@@ -3713,7 +3713,7 @@
       <c r="Y66" s="39"/>
       <c r="Z66" s="39"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A67" s="39"/>
       <c r="B67" s="39"/>
       <c r="C67" s="39"/>
@@ -3741,7 +3741,7 @@
       <c r="Y67" s="39"/>
       <c r="Z67" s="39"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A68" s="39"/>
       <c r="B68" s="39"/>
       <c r="C68" s="39"/>
@@ -3769,7 +3769,7 @@
       <c r="Y68" s="39"/>
       <c r="Z68" s="39"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A69" s="39"/>
       <c r="B69" s="39"/>
       <c r="C69" s="39"/>
@@ -3797,7 +3797,7 @@
       <c r="Y69" s="39"/>
       <c r="Z69" s="39"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A70" s="39"/>
       <c r="B70" s="39"/>
       <c r="C70" s="39"/>
@@ -3825,7 +3825,7 @@
       <c r="Y70" s="39"/>
       <c r="Z70" s="39"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A71" s="39"/>
       <c r="B71" s="39"/>
       <c r="C71" s="39"/>
@@ -3853,7 +3853,7 @@
       <c r="Y71" s="39"/>
       <c r="Z71" s="39"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" s="39"/>
       <c r="B72" s="39"/>
       <c r="C72" s="39"/>
@@ -3881,7 +3881,7 @@
       <c r="Y72" s="39"/>
       <c r="Z72" s="39"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A73" s="39"/>
       <c r="B73" s="39"/>
       <c r="C73" s="39"/>
@@ -3909,7 +3909,7 @@
       <c r="Y73" s="39"/>
       <c r="Z73" s="39"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A74" s="39"/>
       <c r="B74" s="39"/>
       <c r="C74" s="39"/>
@@ -3937,7 +3937,7 @@
       <c r="Y74" s="39"/>
       <c r="Z74" s="39"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A75" s="39"/>
       <c r="B75" s="39"/>
       <c r="C75" s="39"/>
@@ -3965,7 +3965,7 @@
       <c r="Y75" s="39"/>
       <c r="Z75" s="39"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A76" s="39"/>
       <c r="B76" s="39"/>
       <c r="C76" s="39"/>
@@ -3993,7 +3993,7 @@
       <c r="Y76" s="39"/>
       <c r="Z76" s="39"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A77" s="39"/>
       <c r="B77" s="39"/>
       <c r="C77" s="39"/>
@@ -4021,7 +4021,7 @@
       <c r="Y77" s="39"/>
       <c r="Z77" s="39"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A78" s="39"/>
       <c r="B78" s="39"/>
       <c r="C78" s="39"/>
@@ -4049,7 +4049,7 @@
       <c r="Y78" s="39"/>
       <c r="Z78" s="39"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A79" s="39"/>
       <c r="B79" s="39"/>
       <c r="C79" s="39"/>
@@ -4077,7 +4077,7 @@
       <c r="Y79" s="39"/>
       <c r="Z79" s="39"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A80" s="39"/>
       <c r="B80" s="39"/>
       <c r="C80" s="39"/>
@@ -4105,7 +4105,7 @@
       <c r="Y80" s="39"/>
       <c r="Z80" s="39"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A81" s="39"/>
       <c r="B81" s="39"/>
       <c r="C81" s="39"/>
@@ -4133,7 +4133,7 @@
       <c r="Y81" s="39"/>
       <c r="Z81" s="39"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A82" s="39"/>
       <c r="B82" s="39"/>
       <c r="C82" s="39"/>
@@ -4161,7 +4161,7 @@
       <c r="Y82" s="39"/>
       <c r="Z82" s="39"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A83" s="39"/>
       <c r="B83" s="39"/>
       <c r="C83" s="39"/>
@@ -4189,7 +4189,7 @@
       <c r="Y83" s="39"/>
       <c r="Z83" s="39"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A84" s="39"/>
       <c r="B84" s="39"/>
       <c r="C84" s="39"/>
@@ -4217,7 +4217,7 @@
       <c r="Y84" s="39"/>
       <c r="Z84" s="39"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A85" s="39"/>
       <c r="B85" s="39"/>
       <c r="C85" s="39"/>
@@ -4245,7 +4245,7 @@
       <c r="Y85" s="39"/>
       <c r="Z85" s="39"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A86" s="39"/>
       <c r="B86" s="39"/>
       <c r="C86" s="39"/>
@@ -4273,7 +4273,7 @@
       <c r="Y86" s="39"/>
       <c r="Z86" s="39"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A87" s="39"/>
       <c r="B87" s="39"/>
       <c r="C87" s="39"/>
@@ -4301,7 +4301,7 @@
       <c r="Y87" s="39"/>
       <c r="Z87" s="39"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A88" s="39"/>
       <c r="B88" s="39"/>
       <c r="C88" s="39"/>
@@ -4329,7 +4329,7 @@
       <c r="Y88" s="39"/>
       <c r="Z88" s="39"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A89" s="39"/>
       <c r="B89" s="39"/>
       <c r="C89" s="39"/>
@@ -4357,7 +4357,7 @@
       <c r="Y89" s="39"/>
       <c r="Z89" s="39"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A90" s="39"/>
       <c r="B90" s="39"/>
       <c r="C90" s="39"/>
@@ -4385,7 +4385,7 @@
       <c r="Y90" s="39"/>
       <c r="Z90" s="39"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A91" s="39"/>
       <c r="B91" s="39"/>
       <c r="C91" s="39"/>
@@ -4413,7 +4413,7 @@
       <c r="Y91" s="39"/>
       <c r="Z91" s="39"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A92" s="39"/>
       <c r="B92" s="39"/>
       <c r="C92" s="39"/>
@@ -4441,7 +4441,7 @@
       <c r="Y92" s="39"/>
       <c r="Z92" s="39"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A93" s="39"/>
       <c r="B93" s="39"/>
       <c r="C93" s="39"/>
@@ -4469,7 +4469,7 @@
       <c r="Y93" s="39"/>
       <c r="Z93" s="39"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A94" s="39"/>
       <c r="B94" s="39"/>
       <c r="C94" s="39"/>
@@ -4497,7 +4497,7 @@
       <c r="Y94" s="39"/>
       <c r="Z94" s="39"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A95" s="39"/>
       <c r="B95" s="39"/>
       <c r="C95" s="39"/>
@@ -4525,7 +4525,7 @@
       <c r="Y95" s="39"/>
       <c r="Z95" s="39"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A96" s="39"/>
       <c r="B96" s="39"/>
       <c r="C96" s="39"/>
@@ -4553,7 +4553,7 @@
       <c r="Y96" s="39"/>
       <c r="Z96" s="39"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A97" s="39"/>
       <c r="B97" s="39"/>
       <c r="C97" s="39"/>
@@ -4581,7 +4581,7 @@
       <c r="Y97" s="39"/>
       <c r="Z97" s="39"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A98" s="39"/>
       <c r="B98" s="39"/>
       <c r="C98" s="39"/>
@@ -4609,7 +4609,7 @@
       <c r="Y98" s="39"/>
       <c r="Z98" s="39"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A99" s="39"/>
       <c r="B99" s="39"/>
       <c r="C99" s="39"/>
@@ -4667,39 +4667,39 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1328125" customWidth="1"/>
+    <col min="2" max="2" width="11.73046875" customWidth="1"/>
+    <col min="3" max="3" width="3.1328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.86328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.86328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.59765625" customWidth="1"/>
+    <col min="25" max="25" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.1328125" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.73046875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.45">
       <c r="C3" s="23" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -4813,12 +4813,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5050,7 +5050,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -5167,7 +5167,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A10" s="25" t="s">
         <v>56</v>
       </c>
@@ -5175,7 +5175,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A11" s="26" t="s">
         <v>58</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A12" s="27" t="s">
         <v>60</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A13" s="27" t="s">
         <v>62</v>
       </c>
@@ -5199,7 +5199,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A14" s="27" t="s">
         <v>64</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A15" s="27" t="s">
         <v>66</v>
       </c>
@@ -5215,7 +5215,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.45">
       <c r="A16" s="27" t="s">
         <v>68</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A17" s="27" t="s">
         <v>70</v>
       </c>
@@ -5231,7 +5231,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A18" s="27" t="s">
         <v>72</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A19" s="27" t="s">
         <v>74</v>
       </c>
@@ -5247,7 +5247,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="27" t="s">
         <v>76</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" s="27" t="s">
         <v>78</v>
       </c>
@@ -5263,7 +5263,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A22" s="27" t="s">
         <v>80</v>
       </c>
@@ -5271,7 +5271,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="27" t="s">
         <v>82</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="27" t="s">
         <v>84</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="27" t="s">
         <v>86</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="27" t="s">
         <v>88</v>
       </c>
@@ -5303,7 +5303,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="27" t="s">
         <v>90</v>
       </c>
@@ -5311,7 +5311,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="27" t="s">
         <v>92</v>
       </c>
@@ -5319,7 +5319,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="27" t="s">
         <v>94</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="27" t="s">
         <v>96</v>
       </c>
@@ -5335,7 +5335,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A31" s="27" t="s">
         <v>98</v>
       </c>
@@ -5343,7 +5343,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A32" s="27" t="s">
         <v>100</v>
       </c>
@@ -5351,7 +5351,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A33" s="27" t="s">
         <v>102</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A34" s="27" t="s">
         <v>104</v>
       </c>
@@ -5367,7 +5367,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A35" s="27" t="s">
         <v>106</v>
       </c>
@@ -5375,7 +5375,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A36" s="27" t="s">
         <v>108</v>
       </c>
@@ -5383,7 +5383,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A37" s="28" t="s">
         <v>110</v>
       </c>
@@ -5428,20 +5428,20 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -5459,7 +5459,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5476,7 +5476,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -5493,7 +5493,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -5534,7 +5534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6:B11" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
@@ -5573,7 +5573,7 @@
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_Wave</v>
@@ -5609,7 +5609,7 @@
         <v>PWR maximum growth rate of Wave</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_Tidal</v>
@@ -5645,7 +5645,7 @@
         <v>PWR maximum growth rate of Tidal</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_H2GT</v>
@@ -5684,7 +5684,7 @@
         <v>PWR maximum growth rate of H2GT</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_WON</v>
@@ -5720,7 +5720,7 @@
         <v>PWR maximum growth rate of WON</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_WOF</v>
@@ -5756,7 +5756,7 @@
         <v>PWR maximum growth rate of WOF</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="str">
         <f t="shared" ref="B12:B13" si="8">_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
         <v>UC_PWR_MaxGrowth_PV</v>
@@ -5792,7 +5792,7 @@
         <v>PWR maximum growth rate of PV</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="str">
         <f t="shared" si="8"/>
         <v>UC_PWR_MaxGrowth_CSP</v>
@@ -5828,7 +5828,7 @@
         <v>PWR maximum growth rate of CSP</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="C15" t="s">
         <v>117</v>
       </c>
@@ -5836,7 +5836,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>129</v>
       </c>
@@ -5850,7 +5850,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -5864,7 +5864,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>129</v>
       </c>
@@ -5878,7 +5878,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>129</v>
       </c>
@@ -5892,7 +5892,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>129</v>
       </c>
@@ -5906,7 +5906,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>129</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>129</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>129</v>
       </c>
@@ -5958,27 +5958,27 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:P53"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.3984375" customWidth="1"/>
+    <col min="3" max="3" width="14.265625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.1328125" customWidth="1"/>
+    <col min="7" max="7" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.59765625" customWidth="1"/>
+    <col min="14" max="14" width="13.59765625" customWidth="1"/>
+    <col min="15" max="15" width="10.73046875" customWidth="1"/>
+    <col min="16" max="16" width="11.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3,Regions!E3:AD3)</f>
         <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
@@ -5997,7 +5997,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -6015,7 +6015,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -6033,7 +6033,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -6074,7 +6074,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B6" s="18" t="str">
         <f t="shared" ref="B6:B23" si="0">IF(H27="*","*",_xlfn.TEXTJOIN("",TRUE,"UC-",I27,"_MaxGrowth",J27))</f>
         <v>UC-CAR_MaxGrowthBEV</v>
@@ -6105,7 +6105,7 @@
       </c>
       <c r="L6" s="19">
         <f t="shared" ref="L6:L8" si="2">-$B$53*L27/1000</f>
-        <v>-18.168149999999997</v>
+        <v>-27.252225000000003</v>
       </c>
       <c r="M6" s="18">
         <v>5</v>
@@ -6115,7 +6115,7 @@
         <v>CARs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B7" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthPHEV</v>
@@ -6146,7 +6146,7 @@
       </c>
       <c r="L7" s="19">
         <f t="shared" si="2"/>
-        <v>-18.168149999999997</v>
+        <v>-27.252225000000003</v>
       </c>
       <c r="M7" s="18">
         <v>5</v>
@@ -6156,7 +6156,7 @@
         <v>CARs maximum growth rate of PHEVs</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B8" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthNG-ICE</v>
@@ -6197,7 +6197,7 @@
         <v>CARs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B9" s="21" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthFCV</v>
@@ -6238,7 +6238,7 @@
         <v>CARs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B10" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthBEV</v>
@@ -6279,7 +6279,7 @@
         <v>LGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B11" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthPHEV</v>
@@ -6320,7 +6320,7 @@
         <v>LGTs maximum growth rate of PHEVs</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B12" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthNG-ICE</v>
@@ -6361,7 +6361,7 @@
         <v>LGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B13" s="21" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthFCV</v>
@@ -6402,7 +6402,7 @@
         <v>LGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B14" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthBEV</v>
@@ -6443,7 +6443,7 @@
         <v>MGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B15" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthNG-ICE</v>
@@ -6484,7 +6484,7 @@
         <v>MGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.45">
       <c r="B16" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthLNG-ICE</v>
@@ -6525,7 +6525,7 @@
         <v>MGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B17" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthHEV</v>
@@ -6566,7 +6566,7 @@
         <v>MGTs maximum growth rate of HEVs</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B18" s="21" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthFCV</v>
@@ -6607,7 +6607,7 @@
         <v>MGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B19" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthBEV</v>
@@ -6648,7 +6648,7 @@
         <v>HGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B20" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthNG-ICE</v>
@@ -6689,7 +6689,7 @@
         <v>HGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B21" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthLNG-ICE</v>
@@ -6730,7 +6730,7 @@
         <v>HGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B22" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthHEV</v>
@@ -6772,7 +6772,7 @@
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B23" s="21" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthFCV</v>
@@ -6813,7 +6813,7 @@
         <v>HGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="H26" t="s">
         <v>158</v>
       </c>
@@ -6830,7 +6830,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="I27" t="s">
         <v>153</v>
       </c>
@@ -6841,10 +6841,10 @@
         <v>0.8</v>
       </c>
       <c r="L27" s="13">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
@@ -6858,10 +6858,10 @@
         <v>0.8</v>
       </c>
       <c r="L28" s="13">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="10" t="s">
@@ -6886,7 +6886,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" s="56" t="s">
         <v>27</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" s="56"/>
       <c r="B31" s="3" t="s">
         <v>25</v>
@@ -6944,7 +6944,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" s="56"/>
       <c r="B32" s="3" t="s">
         <v>24</v>
@@ -6972,7 +6972,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A33" s="56"/>
       <c r="B33" s="3" t="s">
         <v>23</v>
@@ -7000,7 +7000,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A34" s="56"/>
       <c r="B34" s="3" t="s">
         <v>22</v>
@@ -7028,7 +7028,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A35" s="56"/>
       <c r="B35" s="3" t="s">
         <v>21</v>
@@ -7056,7 +7056,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B36" s="3" t="s">
         <v>20</v>
       </c>
@@ -7083,7 +7083,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B37" s="3" t="s">
         <v>19</v>
       </c>
@@ -7110,7 +7110,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B38" s="3" t="s">
         <v>18</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A39" s="6"/>
       <c r="B39" s="7" t="s">
         <v>17</v>
@@ -7165,7 +7165,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -7182,7 +7182,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.45">
       <c r="I41" t="s">
         <v>141</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.45">
       <c r="I42" t="s">
         <v>141</v>
       </c>
@@ -7210,7 +7210,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.45">
       <c r="I43" t="s">
         <v>141</v>
       </c>
@@ -7224,7 +7224,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.45">
       <c r="I44" t="s">
         <v>141</v>
       </c>
@@ -7238,12 +7238,12 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B46" t="s">
         <v>33</v>
       </c>
@@ -7251,15 +7251,15 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B47" s="13">
         <v>0.5</v>
       </c>
       <c r="C47" s="13">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.45">
       <c r="C48">
         <v>2018</v>
       </c>
@@ -7303,7 +7303,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B49" t="s">
         <v>34</v>
       </c>
@@ -7347,7 +7347,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -7357,62 +7357,62 @@
       </c>
       <c r="C50" s="14">
         <f>B50*$C$47</f>
-        <v>303.60000000000002</v>
+        <v>227.7</v>
       </c>
       <c r="D50" s="14">
         <f>C50*(1+$B$47)</f>
-        <v>455.40000000000003</v>
+        <v>341.54999999999995</v>
       </c>
       <c r="E50" s="20">
         <f t="shared" ref="E50:H50" si="12">D50*(1+$B$47)</f>
-        <v>683.1</v>
+        <v>512.32499999999993</v>
       </c>
       <c r="F50" s="14">
         <f t="shared" si="12"/>
-        <v>1024.6500000000001</v>
+        <v>768.48749999999995</v>
       </c>
       <c r="G50" s="14">
         <f t="shared" si="12"/>
-        <v>1536.9750000000001</v>
+        <v>1152.7312499999998</v>
       </c>
       <c r="H50" s="14">
         <f t="shared" si="12"/>
-        <v>2305.4625000000001</v>
+        <v>1729.0968749999997</v>
       </c>
       <c r="I50" s="14">
         <f t="shared" ref="I50" si="13">H50*(1+$B$47)</f>
-        <v>3458.1937500000004</v>
+        <v>2593.6453124999998</v>
       </c>
       <c r="J50" s="14">
         <f t="shared" ref="J50" si="14">I50*(1+$B$47)</f>
-        <v>5187.2906250000005</v>
+        <v>3890.4679687499997</v>
       </c>
       <c r="K50" s="14">
         <f t="shared" ref="K50" si="15">J50*(1+$B$47)</f>
-        <v>7780.9359375000004</v>
+        <v>5835.7019531249998</v>
       </c>
       <c r="L50" s="14">
         <f t="shared" ref="L50" si="16">K50*(1+$B$47)</f>
-        <v>11671.403906250001</v>
+        <v>8753.5529296874993</v>
       </c>
       <c r="M50" s="14">
         <f t="shared" ref="M50" si="17">L50*(1+$B$47)</f>
-        <v>17507.105859375002</v>
+        <v>13130.329394531249</v>
       </c>
       <c r="N50" s="14">
         <f t="shared" ref="N50" si="18">M50*(1+$B$47)</f>
-        <v>26260.658789062501</v>
+        <v>19695.494091796874</v>
       </c>
       <c r="O50" s="31">
         <f>N50*(1+$B$47)</f>
-        <v>39390.988183593756</v>
+        <v>29543.24113769531</v>
       </c>
       <c r="P50" s="15">
         <f>C35+C34</f>
         <v>22797</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -7422,62 +7422,62 @@
       </c>
       <c r="C51" s="14">
         <f>B51*$C$47</f>
-        <v>106</v>
+        <v>79.5</v>
       </c>
       <c r="D51" s="14">
         <f t="shared" ref="D51:L51" si="19">C51*(1+$B$47)</f>
-        <v>159</v>
+        <v>119.25</v>
       </c>
       <c r="E51" s="20">
         <f t="shared" si="19"/>
-        <v>238.5</v>
+        <v>178.875</v>
       </c>
       <c r="F51" s="14">
         <f t="shared" si="19"/>
-        <v>357.75</v>
+        <v>268.3125</v>
       </c>
       <c r="G51" s="14">
         <f t="shared" si="19"/>
-        <v>536.625</v>
+        <v>402.46875</v>
       </c>
       <c r="H51" s="14">
         <f t="shared" si="19"/>
-        <v>804.9375</v>
+        <v>603.703125</v>
       </c>
       <c r="I51" s="14">
         <f t="shared" si="19"/>
-        <v>1207.40625</v>
+        <v>905.5546875</v>
       </c>
       <c r="J51" s="14">
         <f t="shared" si="19"/>
-        <v>1811.109375</v>
+        <v>1358.33203125</v>
       </c>
       <c r="K51" s="14">
         <f t="shared" si="19"/>
-        <v>2716.6640625</v>
+        <v>2037.498046875</v>
       </c>
       <c r="L51" s="14">
         <f t="shared" si="19"/>
-        <v>4074.99609375</v>
+        <v>3056.2470703125</v>
       </c>
       <c r="M51" s="14">
         <f t="shared" ref="M51:M53" si="20">L51*(1+$B$47)</f>
-        <v>6112.494140625</v>
+        <v>4584.37060546875</v>
       </c>
       <c r="N51" s="14">
         <f t="shared" ref="N51:N53" si="21">M51*(1+$B$47)</f>
-        <v>9168.7412109375</v>
+        <v>6876.555908203125</v>
       </c>
       <c r="O51" s="31">
         <f t="shared" ref="O51:O53" si="22">N51*(1+$B$47)</f>
-        <v>13753.11181640625</v>
+        <v>10314.833862304688</v>
       </c>
       <c r="P51" s="15">
         <f>C33+C32</f>
         <v>11207</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -7487,62 +7487,62 @@
       </c>
       <c r="C52" s="14">
         <f>B52*$C$47</f>
-        <v>3307.8</v>
+        <v>2480.85</v>
       </c>
       <c r="D52" s="14">
         <f>C52*(1+$B$47)</f>
-        <v>4961.7000000000007</v>
+        <v>3721.2749999999996</v>
       </c>
       <c r="E52" s="20">
         <f t="shared" ref="E52:L52" si="23">D52*(1+$B$47)</f>
-        <v>7442.5500000000011</v>
+        <v>5581.9124999999995</v>
       </c>
       <c r="F52" s="14">
         <f t="shared" si="23"/>
-        <v>11163.825000000001</v>
+        <v>8372.8687499999996</v>
       </c>
       <c r="G52" s="14">
         <f t="shared" si="23"/>
-        <v>16745.737500000003</v>
+        <v>12559.303124999999</v>
       </c>
       <c r="H52" s="14">
         <f t="shared" si="23"/>
-        <v>25118.606250000004</v>
+        <v>18838.954687499998</v>
       </c>
       <c r="I52" s="14">
         <f t="shared" si="23"/>
-        <v>37677.909375000003</v>
+        <v>28258.432031249999</v>
       </c>
       <c r="J52" s="14">
         <f t="shared" si="23"/>
-        <v>56516.864062500004</v>
+        <v>42387.648046874994</v>
       </c>
       <c r="K52" s="14">
         <f t="shared" si="23"/>
-        <v>84775.296093750003</v>
+        <v>63581.472070312491</v>
       </c>
       <c r="L52" s="14">
         <f t="shared" si="23"/>
-        <v>127162.94414062501</v>
+        <v>95372.208105468744</v>
       </c>
       <c r="M52" s="14">
         <f t="shared" si="20"/>
-        <v>190744.41621093752</v>
+        <v>143058.3121582031</v>
       </c>
       <c r="N52" s="14">
         <f t="shared" si="21"/>
-        <v>286116.62431640626</v>
+        <v>214587.46823730465</v>
       </c>
       <c r="O52" s="31">
         <f t="shared" si="22"/>
-        <v>429174.93647460942</v>
+        <v>321881.20235595701</v>
       </c>
       <c r="P52" s="15">
         <f>C31+C30</f>
         <v>328695</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -7552,55 +7552,55 @@
       </c>
       <c r="C53" s="14">
         <f>B53*$C$47</f>
-        <v>24224.2</v>
+        <v>18168.149999999998</v>
       </c>
       <c r="D53" s="14">
         <f t="shared" ref="D53:L53" si="24">C53*(1+$B$47)</f>
-        <v>36336.300000000003</v>
+        <v>27252.224999999999</v>
       </c>
       <c r="E53" s="20">
         <f t="shared" si="24"/>
-        <v>54504.450000000004</v>
+        <v>40878.337499999994</v>
       </c>
       <c r="F53" s="14">
         <f t="shared" si="24"/>
-        <v>81756.675000000003</v>
+        <v>61317.506249999991</v>
       </c>
       <c r="G53" s="14">
         <f t="shared" si="24"/>
-        <v>122635.01250000001</v>
+        <v>91976.259374999994</v>
       </c>
       <c r="H53" s="14">
         <f t="shared" si="24"/>
-        <v>183952.51875000002</v>
+        <v>137964.38906249998</v>
       </c>
       <c r="I53" s="14">
         <f t="shared" si="24"/>
-        <v>275928.77812500001</v>
+        <v>206946.58359374997</v>
       </c>
       <c r="J53" s="14">
         <f t="shared" si="24"/>
-        <v>413893.16718750005</v>
+        <v>310419.87539062498</v>
       </c>
       <c r="K53" s="14">
         <f t="shared" si="24"/>
-        <v>620839.75078125007</v>
+        <v>465629.81308593747</v>
       </c>
       <c r="L53" s="14">
         <f t="shared" si="24"/>
-        <v>931259.62617187505</v>
+        <v>698444.71962890623</v>
       </c>
       <c r="M53" s="14">
         <f t="shared" si="20"/>
-        <v>1396889.4392578127</v>
+        <v>1047667.0794433593</v>
       </c>
       <c r="N53" s="14">
         <f t="shared" si="21"/>
-        <v>2095334.158886719</v>
+        <v>1571500.6191650389</v>
       </c>
       <c r="O53" s="31">
         <f t="shared" si="22"/>
-        <v>3143001.2383300783</v>
+        <v>2357250.9287475585</v>
       </c>
       <c r="P53" s="15">
         <f>C36</f>
@@ -7623,21 +7623,21 @@
   <dimension ref="A2:N18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="14" max="14" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.86328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.1328125" customWidth="1"/>
+    <col min="14" max="14" width="34.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -7655,7 +7655,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7672,7 +7672,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7689,7 +7689,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -7730,7 +7730,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
         <v>UC_SRV-PU_MaxGrowth_HPs</v>
@@ -7771,7 +7771,7 @@
         <v>SRV-PU maximum growth rate of HPs</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
         <v>UC_SRV-CS_MaxGrowth_HPs</v>
@@ -7812,7 +7812,7 @@
         <v>SRV-CS maximum growth rate of HPs</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -7827,7 +7827,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -7844,7 +7844,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
@@ -7885,7 +7885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A17,"MaxGrowth",B17)</f>
         <v>UC_SRV_MaxGrowth_Biomass</v>
@@ -7915,7 +7915,7 @@
       </c>
       <c r="L11" s="33">
         <f>-D17</f>
-        <v>-0.3</v>
+        <v>-0.1</v>
       </c>
       <c r="M11" s="2">
         <v>5</v>
@@ -7925,7 +7925,7 @@
         <v>SRV maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_SRV_MaxGrowth_Biogas</v>
@@ -7955,7 +7955,7 @@
       </c>
       <c r="L12" s="33">
         <f>-D18</f>
-        <v>-0.3</v>
+        <v>-0.1</v>
       </c>
       <c r="M12" s="2">
         <v>5</v>
@@ -7965,7 +7965,7 @@
         <v>SRV maximum growth rate of Biogas</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="C14" t="s">
         <v>117</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>130</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>131</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -8012,10 +8012,10 @@
         <v>0.05</v>
       </c>
       <c r="D17">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>145</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>0.05</v>
       </c>
       <c r="D18">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -8035,6 +8035,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -8245,22 +8260,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8277,21 +8294,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Increase max WON NCAP for 2019 to reflect historical development
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882AECD3-2F96-4390-8CE7-FD1D0215A59A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3588191-9619-4780-96B7-57F33141E806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="192">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -5432,10 +5432,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:N25"/>
+  <dimension ref="A2:N26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5554,14 +5554,14 @@
         <v>1</v>
       </c>
       <c r="I6" s="16">
-        <f>-D14</f>
+        <f t="shared" ref="I6:I11" si="2">-D14</f>
         <v>-0.4</v>
       </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
       <c r="K6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
+        <f t="shared" ref="K6:K11" si="3">_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
@@ -5590,14 +5590,14 @@
         <v>1</v>
       </c>
       <c r="I7" s="16">
-        <f>-D15</f>
+        <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
       <c r="J7" s="2">
         <v>5</v>
       </c>
       <c r="K7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
+        <f t="shared" si="3"/>
         <v>PWR maximum growth rate of Wave</v>
       </c>
     </row>
@@ -5626,14 +5626,14 @@
         <v>1</v>
       </c>
       <c r="I8" s="16">
-        <f>-D16</f>
+        <f t="shared" si="2"/>
         <v>-0.1</v>
       </c>
       <c r="J8" s="2">
         <v>5</v>
       </c>
       <c r="K8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A16, "maximum growth rate of",B16)</f>
+        <f t="shared" si="3"/>
         <v>PWR maximum growth rate of Tidal</v>
       </c>
     </row>
@@ -5662,20 +5662,20 @@
         <v>1</v>
       </c>
       <c r="I9" s="16">
-        <f>-D17</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="J9" s="2">
         <v>5</v>
       </c>
       <c r="K9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A17, "maximum growth rate of",B17)</f>
+        <f t="shared" si="3"/>
         <v>PWR maximum growth rate of H2GT</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
-        <f t="shared" ref="B10:B11" si="2">_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
+        <f t="shared" ref="B10:B11" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_PWR_MaxGrowth_PV</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -5691,27 +5691,27 @@
         <v>15</v>
       </c>
       <c r="G10" s="26">
-        <f t="shared" ref="G10:J11" si="3">1+$C18</f>
+        <f t="shared" ref="G10:G11" si="5">1+$C18</f>
         <v>1.2</v>
       </c>
       <c r="H10" s="2">
         <v>1</v>
       </c>
       <c r="I10" s="16">
-        <f>-D18</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="J10" s="2">
         <v>5</v>
       </c>
       <c r="K10" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A18, "maximum growth rate of",B18)</f>
+        <f t="shared" si="3"/>
         <v>PWR maximum growth rate of PV</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>UC_PWR_MaxGrowth_CSP</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -5727,21 +5727,21 @@
         <v>15</v>
       </c>
       <c r="G11" s="26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2</v>
       </c>
       <c r="H11" s="2">
         <v>1</v>
       </c>
       <c r="I11" s="16">
-        <f>-D19</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="J11" s="2">
         <v>5</v>
       </c>
       <c r="K11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A19, "maximum growth rate of",B19)</f>
+        <f t="shared" si="3"/>
         <v>PWR maximum growth rate of CSP</v>
       </c>
     </row>
@@ -5889,17 +5889,17 @@
         <v>160</v>
       </c>
       <c r="E24" s="2">
-        <v>2023</v>
+        <v>2019</v>
       </c>
       <c r="F24" s="2" t="s">
         <v>191</v>
       </c>
       <c r="G24" s="26">
-        <f>1+$C28</f>
+        <f>1+$C29</f>
         <v>1</v>
       </c>
       <c r="H24" s="16">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="I24" s="2">
         <v>3</v>
@@ -5909,30 +5909,52 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>186</v>
-      </c>
+      <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="E25">
-        <v>2026</v>
+        <v>160</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2020</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>191</v>
       </c>
       <c r="G25" s="26">
-        <f>1+$C29</f>
+        <f>1+$C30</f>
         <v>1</v>
       </c>
       <c r="H25" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E26">
+        <v>2026</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G26" s="26">
+        <f>1+$C30</f>
         <v>1</v>
       </c>
-      <c r="I25" s="2">
+      <c r="H26" s="16">
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
         <v>3</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J26" s="2" t="s">
         <v>190</v>
       </c>
     </row>
@@ -8023,6 +8045,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -8233,15 +8264,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -8249,6 +8271,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8267,14 +8297,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Increase maximum new WOF to 2 GW/yr from 2027
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3588191-9619-4780-96B7-57F33141E806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59D4D74-4A5E-484F-814D-02BABDBBFC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="192">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -5432,10 +5432,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:N26"/>
+  <dimension ref="A2:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5956,6 +5956,18 @@
       </c>
       <c r="J26" s="2" t="s">
         <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D27" s="2"/>
+      <c r="E27">
+        <v>2027</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="H27" s="16">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -8054,6 +8066,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -8264,12 +8282,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
@@ -8279,6 +8291,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8295,13 +8316,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add a maximum growth rate for biogas production
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B59D4D74-4A5E-484F-814D-02BABDBBFC75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC93D19-71AC-4D3D-AFCA-1FD32AD79421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
     <sheet name="Regions" sheetId="2" r:id="rId2"/>
-    <sheet name="PWR" sheetId="4" r:id="rId3"/>
-    <sheet name="TRA" sheetId="1" r:id="rId4"/>
-    <sheet name="SRV" sheetId="5" r:id="rId5"/>
+    <sheet name="SUP" sheetId="7" r:id="rId3"/>
+    <sheet name="PWR" sheetId="4" r:id="rId4"/>
+    <sheet name="TRA" sheetId="1" r:id="rId5"/>
+    <sheet name="SRV" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
+    <definedName name="__123Graph_AEUMILKPN" localSheetId="3" hidden="1">#REF!</definedName>
+    <definedName name="__123Graph_AEUMILKPN" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="2" hidden="1">#REF!</definedName>
-    <definedName name="__123Graph_AEUMILKPN" localSheetId="4" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
     <definedName name="_AtRisk_SimSetting_AutomaticResultsDisplayMode" hidden="1">2</definedName>
@@ -43,28 +45,34 @@
     <definedName name="_AtRisk_SimSetting_StdRecalcBehavior" hidden="1">1</definedName>
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStatic" hidden="1">0</definedName>
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
+    <definedName name="_Regression_Y" localSheetId="3" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_Y" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" localSheetId="2" hidden="1">#REF!</definedName>
-    <definedName name="_Regression_Y" localSheetId="4" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
     <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="aa" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec2" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elec3" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="elecc" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
     <definedName name="IQ_FWD_CY1" hidden="1">10002</definedName>
@@ -103,12 +111,14 @@
     <definedName name="RiskUseFixedSeed" hidden="1">TRUE</definedName>
     <definedName name="RiskUseMultipleCPUs" hidden="1">FALSE</definedName>
     <definedName name="table6" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="table6" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
-    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -152,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="196">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -748,6 +758,18 @@
   </si>
   <si>
     <t>UP</t>
+  </si>
+  <si>
+    <t>SUP</t>
+  </si>
+  <si>
+    <t>BIOGAS</t>
+  </si>
+  <si>
+    <t>SBIORGAS*</t>
+  </si>
+  <si>
+    <t>Starting value (PJ)</t>
   </si>
 </sst>
 </file>
@@ -5430,12 +5452,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:N27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89417C8F-9D07-4311-9372-0B0C534E50C4}">
+  <dimension ref="A2:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5514,6 +5535,186 @@
         <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="str">
+        <f t="shared" ref="B6" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A10,"MaxGrowth",B10)</f>
+        <v>UC_SUP_MaxGrowth_BIOGAS</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="26">
+        <f t="shared" ref="G6" si="1">1+$C10</f>
+        <v>1.4</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="16">
+        <f t="shared" ref="I6" si="2">-D10</f>
+        <v>-0.2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2" t="str">
+        <f t="shared" ref="K6" si="3">_xlfn.TEXTJOIN(" ",TRUE,A10, "maximum growth rate of",B10)</f>
+        <v>SUP maximum growth rate of BIOGAS</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="H11" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A2:N27"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -5975,7 +6176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:P53"/>
@@ -7639,7 +7840,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N18"/>
@@ -8066,12 +8267,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -8282,6 +8477,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
@@ -8291,15 +8492,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8316,4 +8508,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add max growth constraints for ambient and district heat in SRV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC93D19-71AC-4D3D-AFCA-1FD32AD79421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5CF401-9EC6-48E1-8520-ADB61A93FBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="199">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -770,6 +770,15 @@
   </si>
   <si>
     <t>Starting value (PJ)</t>
+  </si>
+  <si>
+    <t>AmbientHeat</t>
+  </si>
+  <si>
+    <t>DistrictHeat</t>
+  </si>
+  <si>
+    <t>SRVHET</t>
   </si>
 </sst>
 </file>
@@ -5455,8 +5464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89417C8F-9D07-4311-9372-0B0C534E50C4}">
   <dimension ref="A2:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7843,10 +7852,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:N18"/>
+  <dimension ref="A2:N25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7856,11 +7865,12 @@
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" customWidth="1"/>
-    <col min="14" max="14" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -7878,7 +7888,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7895,7 +7905,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7912,7 +7922,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -7944,7 +7954,7 @@
         <v>10</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>11</v>
@@ -7953,9 +7963,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_SRV-PU_MaxGrowth_HPs</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -7976,27 +7986,27 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f>1+C15</f>
+        <f>1+C18</f>
         <v>1.05</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="16">
-        <f>-D15</f>
+        <f>-D18</f>
         <v>-0.3</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A18, "maximum growth rate of",B18)</f>
         <v>SRV-PU maximum growth rate of HPs</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A19,"MaxGrowth",B19)</f>
         <v>UC_SRV-CS_MaxGrowth_HPs</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -8017,25 +8027,25 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f>1+C16</f>
+        <f>1+C19</f>
         <v>1.05</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="16">
-        <f>-D16</f>
+        <f>-D19</f>
         <v>-0.3</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A16, "maximum growth rate of",B16)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A19, "maximum growth rate of",B19)</f>
         <v>SRV-CS maximum growth rate of HPs</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -8050,7 +8060,7 @@
       <c r="M8" s="2"/>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -8067,7 +8077,7 @@
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
@@ -8099,7 +8109,7 @@
         <v>152</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>43</v>
+        <v>188</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>11</v>
@@ -8108,9 +8118,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A17,"MaxGrowth",B17)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
         <v>UC_SRV_MaxGrowth_Biomass</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -8130,27 +8140,27 @@
         <v>15</v>
       </c>
       <c r="J11" s="29">
-        <f>1+C17</f>
+        <f>1+C22</f>
         <v>1.05</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
       </c>
       <c r="L11" s="16">
-        <f>-D17</f>
+        <f>-D22</f>
         <v>-0.3</v>
       </c>
       <c r="M11" s="2">
         <v>5</v>
       </c>
       <c r="N11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A17, "maximum growth rate of",B17)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
         <v>SRV maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
         <v>UC_SRV_MaxGrowth_Biogas</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -8170,85 +8180,218 @@
         <v>15</v>
       </c>
       <c r="J12" s="29">
-        <f>1+C18</f>
+        <f>1+C23</f>
         <v>1.05</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
       </c>
       <c r="L12" s="16">
-        <f>-D18</f>
+        <f>-D23</f>
         <v>-0.3</v>
       </c>
       <c r="M12" s="2">
         <v>5</v>
       </c>
       <c r="N12" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A18, "maximum growth rate of",B18)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
         <v>SRV maximum growth rate of Biogas</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A24,"MaxGrowth",B24)</f>
+        <v>UC_SRV_MaxGrowth_AmbientHeat</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="29">
+        <f>1+C24</f>
+        <v>1.05</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="16">
+        <f>-D24</f>
+        <v>-0.3</v>
+      </c>
+      <c r="M13" s="2">
+        <v>5</v>
+      </c>
+      <c r="N13" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
+        <v>SRV maximum growth rate of AmbientHeat</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A25,"MaxGrowth",B25)</f>
+        <v>UC_SRV_MaxGrowth_DistrictHeat</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="29">
+        <f>1+C25</f>
+        <v>1.05</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="16">
+        <f>-D25</f>
+        <v>-0.3</v>
+      </c>
+      <c r="M14" s="2">
+        <v>5</v>
+      </c>
+      <c r="N14" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A25, "maximum growth rate of",B25)</f>
+        <v>SRV maximum growth rate of DistrictHeat</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="2"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
         <v>117</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" t="s">
-        <v>128</v>
-      </c>
-      <c r="C15" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D15">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" t="s">
-        <v>128</v>
-      </c>
-      <c r="C16" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D16">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>145</v>
-      </c>
-      <c r="B17" t="s">
-        <v>143</v>
-      </c>
-      <c r="C17" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D17">
-        <v>0.3</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C18" s="11">
         <v>0.05</v>
       </c>
       <c r="D18">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C19" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D19">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="11"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22" t="s">
+        <v>143</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D22">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>145</v>
+      </c>
+      <c r="B23" t="s">
+        <v>144</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D23">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>145</v>
+      </c>
+      <c r="B24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D24">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>145</v>
+      </c>
+      <c r="B25" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D25">
         <v>0.3</v>
       </c>
     </row>
@@ -8267,6 +8410,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -8477,12 +8626,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
@@ -8492,6 +8635,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8508,13 +8660,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove capacity-based growth rate for HPs in SRV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5CF401-9EC6-48E1-8520-ADB61A93FBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC91B870-24A1-463E-957D-E6E320C9904C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -162,7 +162,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="194">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -568,25 +568,10 @@
     <t>National</t>
   </si>
   <si>
-    <t>HPs</t>
-  </si>
-  <si>
     <t>PWR</t>
   </si>
   <si>
-    <t>SRV-PU</t>
-  </si>
-  <si>
-    <t>SRV-CS</t>
-  </si>
-  <si>
     <t>SRVAHT</t>
-  </si>
-  <si>
-    <t>S-SH*PU*</t>
-  </si>
-  <si>
-    <t>S-SH*CS*</t>
   </si>
   <si>
     <t>BEV</t>
@@ -2284,7 +2269,7 @@
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="46" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B16" s="46"/>
       <c r="C16" s="46"/>
@@ -2370,10 +2355,10 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B19" s="45" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C19" s="45"/>
       <c r="D19" s="45"/>
@@ -2402,10 +2387,10 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B20" s="45" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C20" s="45"/>
       <c r="D20" s="45"/>
@@ -2434,10 +2419,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
@@ -2494,10 +2479,10 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B23" s="45" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C23" s="45"/>
       <c r="D23" s="45"/>
@@ -2527,7 +2512,7 @@
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="37"/>
       <c r="B24" s="45" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C24" s="45"/>
       <c r="D24" s="45"/>
@@ -2557,7 +2542,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="40" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="40"/>
@@ -2586,10 +2571,10 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C26" s="45"/>
       <c r="D26" s="45"/>
@@ -2674,7 +2659,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B29" s="41">
         <v>1</v>
@@ -2706,10 +2691,10 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B30" s="47" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C30" s="45"/>
       <c r="D30" s="45"/>
@@ -2738,10 +2723,10 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B31" s="45" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C31" s="45"/>
       <c r="D31" s="45"/>
@@ -2771,7 +2756,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="43"/>
       <c r="B32" s="44" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C32" s="43"/>
       <c r="D32" s="43"/>
@@ -5544,10 +5529,10 @@
         <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="I5" s="4" t="s">
         <v>43</v>
@@ -5565,10 +5550,10 @@
         <v>UC_SUP_MaxGrowth_BIOGAS</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E6" s="2">
         <v>2018</v>
@@ -5612,15 +5597,15 @@
         <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="C10" s="11">
         <v>0.4</v>
@@ -5856,7 +5841,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="E9" s="2">
         <v>2020</v>
@@ -5892,7 +5877,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E10">
         <v>2018</v>
@@ -5928,7 +5913,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E11">
         <v>2018</v>
@@ -5965,7 +5950,7 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B14" t="s">
         <v>124</v>
@@ -5979,7 +5964,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
         <v>125</v>
@@ -5993,7 +5978,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
         <v>126</v>
@@ -6007,10 +5992,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C17" s="11">
         <v>0.2</v>
@@ -6021,10 +6006,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C18" s="11">
         <v>0.2</v>
@@ -6035,10 +6020,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B19" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C19" s="11">
         <v>0.2</v>
@@ -6078,10 +6063,10 @@
         <v>8</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>11</v>
@@ -6092,17 +6077,17 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E24" s="2">
         <v>2019</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G24" s="26">
         <f>1+$C29</f>
@@ -6115,20 +6100,20 @@
         <v>3</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E25" s="2">
         <v>2020</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G25" s="26">
         <f>1+$C30</f>
@@ -6142,17 +6127,17 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E26">
         <v>2026</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="G26" s="26">
         <f>1+$C30</f>
@@ -6165,7 +6150,7 @@
         <v>3</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -6174,7 +6159,7 @@
         <v>2027</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="H27" s="16">
         <v>2</v>
@@ -7047,27 +7032,27 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="I26" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J26" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="K26" t="s">
         <v>117</v>
       </c>
       <c r="L26" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J27" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K27" s="11">
         <v>0.8</v>
@@ -7081,10 +7066,10 @@
         <v>29</v>
       </c>
       <c r="I28" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J28" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K28" s="11">
         <v>0.8</v>
@@ -7106,10 +7091,10 @@
         <v>32</v>
       </c>
       <c r="I29" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J29" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K29" s="11">
         <v>0.5</v>
@@ -7136,10 +7121,10 @@
         <v>4.3671013742841359E-2</v>
       </c>
       <c r="I30" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="J30" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K30" s="11">
         <v>0.5</v>
@@ -7164,10 +7149,10 @@
         <v>6.5375711631511485E-2</v>
       </c>
       <c r="I31" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="J31" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K31" s="11">
         <v>0.5</v>
@@ -7192,10 +7177,10 @@
         <v>4.4214694236691596E-2</v>
       </c>
       <c r="I32" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="J32" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="K32" s="11">
         <v>0.5</v>
@@ -7220,10 +7205,10 @@
         <v>4.9391983185707852E-2</v>
       </c>
       <c r="I33" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="J33" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K33" s="11">
         <v>0.5</v>
@@ -7248,10 +7233,10 @@
         <v>5.7573599240265907E-2</v>
       </c>
       <c r="I34" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="J34" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K34" s="11">
         <v>0.5</v>
@@ -7276,10 +7261,10 @@
         <v>7.187086899046824E-2</v>
       </c>
       <c r="I35" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="J35" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K35" s="11">
         <v>0.5</v>
@@ -7303,10 +7288,10 @@
         <v>5.5865068892149296E-2</v>
       </c>
       <c r="I36" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="J36" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K36" s="11">
         <v>0.5</v>
@@ -7330,10 +7315,10 @@
         <v>6.1874562947601935E-2</v>
       </c>
       <c r="I37" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="J37" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="K37" s="11">
         <v>0.5</v>
@@ -7357,10 +7342,10 @@
         <v>5.7044321200540614E-2</v>
       </c>
       <c r="I38" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="J38" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="K38" s="11">
         <v>0.5</v>
@@ -7385,10 +7370,10 @@
         <v>4.9170087453150095E-2</v>
       </c>
       <c r="I39" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="J39" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K39" s="11">
         <v>0.5</v>
@@ -7402,10 +7387,10 @@
         <v>28</v>
       </c>
       <c r="I40" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J40" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="K40" s="11">
         <v>0.5</v>
@@ -7416,10 +7401,10 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J41" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="K41" s="11">
         <v>0.5</v>
@@ -7430,10 +7415,10 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I42" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J42" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="K42" s="11">
         <v>0.5</v>
@@ -7444,10 +7429,10 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J43" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="K43" s="11">
         <v>0.5</v>
@@ -7458,10 +7443,10 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="J44" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="K44" s="11">
         <v>0.5</v>
@@ -7472,7 +7457,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -7852,10 +7837,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:N25"/>
+  <dimension ref="A2:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M29" sqref="M29"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7870,7 +7855,7 @@
     <col min="14" max="14" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -7888,7 +7873,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7905,7 +7890,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7922,7 +7907,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -7948,13 +7933,13 @@
         <v>8</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>9</v>
+        <v>146</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>10</v>
+        <v>147</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>11</v>
@@ -7963,21 +7948,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
-        <v>UC_SRV-PU_MaxGrowth_HPs</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A13,"MaxGrowth",B13)</f>
+        <v>UC_SRV_MaxGrowth_Biomass</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>13</v>
+        <v>145</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>141</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
@@ -7986,39 +7970,38 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f>1+C18</f>
+        <f>1+C13</f>
         <v>1.05</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="16">
-        <f>-D18</f>
+        <f>-D13</f>
         <v>-0.3</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A18, "maximum growth rate of",B18)</f>
-        <v>SRV-PU maximum growth rate of HPs</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A13, "maximum growth rate of",B13)</f>
+        <v>SRV maximum growth rate of Biomass</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A19,"MaxGrowth",B19)</f>
-        <v>UC_SRV-CS_MaxGrowth_HPs</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
+        <v>UC_SRV_MaxGrowth_Biogas</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>145</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="G7" s="2" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="H7" s="2">
         <v>2018</v>
@@ -8027,371 +8010,179 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f>1+C19</f>
+        <f>1+C14</f>
         <v>1.05</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="16">
-        <f>-D19</f>
+        <f>-D14</f>
         <v>-0.3</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A19, "maximum growth rate of",B19)</f>
-        <v>SRV-CS maximum growth rate of HPs</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
+        <v>SRV maximum growth rate of Biogas</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
+        <v>UC_SRV_MaxGrowth_AmbientHeat</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="29"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="29">
+        <f>1+C15</f>
+        <v>1.05</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="16">
+        <f>-D15</f>
+        <v>-0.3</v>
+      </c>
+      <c r="M8" s="2">
+        <v>5</v>
+      </c>
+      <c r="N8" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
+        <v>SRV maximum growth rate of AmbientHeat</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
+        <v>UC_SRV_MaxGrowth_DistrictHeat</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>145</v>
+      </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2021</v>
+      </c>
       <c r="I9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-    </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="29">
+        <f>1+C16</f>
+        <v>1.05</v>
+      </c>
+      <c r="K9" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="14" t="s">
+      <c r="L9" s="16">
+        <f>-D16</f>
+        <v>-0.3</v>
+      </c>
+      <c r="M9" s="2">
         <v>5</v>
       </c>
-      <c r="G10" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="K10" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="M10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
-        <v>UC_SRV_MaxGrowth_Biomass</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H11" s="2">
-        <v>2018</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="29">
-        <f>1+C22</f>
-        <v>1.05</v>
-      </c>
-      <c r="K11" s="2">
-        <v>1</v>
-      </c>
-      <c r="L11" s="16">
-        <f>-D22</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M11" s="2">
-        <v>5</v>
-      </c>
-      <c r="N11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
-        <v>SRV maximum growth rate of Biomass</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
-        <v>UC_SRV_MaxGrowth_Biogas</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H12" s="2">
-        <v>2018</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="29">
-        <f>1+C23</f>
-        <v>1.05</v>
-      </c>
-      <c r="K12" s="2">
-        <v>1</v>
-      </c>
-      <c r="L12" s="16">
-        <f>-D23</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M12" s="2">
-        <v>5</v>
-      </c>
-      <c r="N12" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
-        <v>SRV maximum growth rate of Biogas</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A24,"MaxGrowth",B24)</f>
-        <v>UC_SRV_MaxGrowth_AmbientHeat</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H13" s="2">
-        <v>2021</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="29">
-        <f>1+C24</f>
-        <v>1.05</v>
-      </c>
-      <c r="K13" s="2">
-        <v>1</v>
-      </c>
-      <c r="L13" s="16">
-        <f>-D24</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M13" s="2">
-        <v>5</v>
-      </c>
-      <c r="N13" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
-        <v>SRV maximum growth rate of AmbientHeat</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A25,"MaxGrowth",B25)</f>
-        <v>UC_SRV_MaxGrowth_DistrictHeat</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="H14" s="2">
-        <v>2021</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J14" s="29">
-        <f>1+C25</f>
-        <v>1.05</v>
-      </c>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="16">
-        <f>-D25</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M14" s="2">
-        <v>5</v>
-      </c>
-      <c r="N14" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A25, "maximum growth rate of",B25)</f>
+      <c r="N9" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A16, "maximum growth rate of",B16)</f>
         <v>SRV maximum growth rate of DistrictHeat</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
         <v>117</v>
       </c>
-      <c r="D17" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="11">
+      <c r="D12" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" s="11">
         <v>0.05</v>
       </c>
-      <c r="D18">
+      <c r="D13">
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>131</v>
-      </c>
-      <c r="B19" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="11">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="11">
         <v>0.05</v>
       </c>
-      <c r="D19">
+      <c r="D14">
         <v>0.3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="11"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>117</v>
-      </c>
-      <c r="D21" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B22" t="s">
-        <v>143</v>
-      </c>
-      <c r="C22" s="11">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" t="s">
+        <v>191</v>
+      </c>
+      <c r="C15" s="11">
         <v>0.05</v>
       </c>
-      <c r="D22">
+      <c r="D15">
         <v>0.3</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>145</v>
-      </c>
-      <c r="B23" t="s">
-        <v>144</v>
-      </c>
-      <c r="C23" s="11">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" t="s">
+        <v>192</v>
+      </c>
+      <c r="C16" s="11">
         <v>0.05</v>
       </c>
-      <c r="D23">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>145</v>
-      </c>
-      <c r="B24" t="s">
-        <v>196</v>
-      </c>
-      <c r="C24" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D24">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>145</v>
-      </c>
-      <c r="B25" t="s">
-        <v>197</v>
-      </c>
-      <c r="C25" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D25">
+      <c r="D16">
         <v>0.3</v>
       </c>
     </row>
@@ -8401,18 +8192,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8627,18 +8418,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Use max growth rates in RSD instead of annual bounds
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E26547-6CCC-4450-AE0D-D23C32DA0108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12547C9-8D0B-49E7-BB28-B1E07F376044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
     <sheet name="Regions" sheetId="2" r:id="rId2"/>
     <sheet name="SUP" sheetId="7" r:id="rId3"/>
     <sheet name="PWR" sheetId="4" r:id="rId4"/>
-    <sheet name="TRA" sheetId="1" r:id="rId5"/>
+    <sheet name="RSD" sheetId="8" r:id="rId5"/>
     <sheet name="SRV" sheetId="5" r:id="rId6"/>
+    <sheet name="TRA" sheetId="1" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="3" hidden="1">#REF!</definedName>
+    <definedName name="__123Graph_AEUMILKPN" localSheetId="4" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -46,31 +48,37 @@
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStatic" hidden="1">0</definedName>
     <definedName name="_AtRisk_SimSetting_StdRecalcWithoutRiskStaticPercentile" hidden="1">0.5</definedName>
     <definedName name="_Regression_Y" localSheetId="3" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_Y" localSheetId="4" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
     <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -112,11 +120,13 @@
     <definedName name="RiskUseMultipleCPUs" hidden="1">FALSE</definedName>
     <definedName name="table6" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
@@ -162,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="217">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -770,6 +780,69 @@
   </si>
   <si>
     <t>SRVGAS</t>
+  </si>
+  <si>
+    <t>RSD</t>
+  </si>
+  <si>
+    <t>RSDBDL</t>
+  </si>
+  <si>
+    <t>Biodiesel</t>
+  </si>
+  <si>
+    <t>Coal</t>
+  </si>
+  <si>
+    <t>Peat</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Ethanol</t>
+  </si>
+  <si>
+    <t>LPG</t>
+  </si>
+  <si>
+    <t>Kerosene</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>RSDAHT</t>
+  </si>
+  <si>
+    <t>RSDWOO</t>
+  </si>
+  <si>
+    <t>RSDCOA</t>
+  </si>
+  <si>
+    <t>RSDPEA</t>
+  </si>
+  <si>
+    <t>RSDELC</t>
+  </si>
+  <si>
+    <t>RSDETH</t>
+  </si>
+  <si>
+    <t>RSDGAS</t>
+  </si>
+  <si>
+    <t>RSDHET</t>
+  </si>
+  <si>
+    <t>RSDLPG</t>
+  </si>
+  <si>
+    <t>RSDKER</t>
+  </si>
+  <si>
+    <t>RSDSOL</t>
   </si>
 </sst>
 </file>
@@ -6177,6 +6250,1201 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
+  <dimension ref="A2:N32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A21,"MaxGrowth",B21)</f>
+        <v>UC_RSD_MaxGrowth_AmbientHeat</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="29">
+        <f>1+C22</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="16">
+        <f>-D22</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5</v>
+      </c>
+      <c r="N6" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
+        <v>RSD maximum growth rate of Biodiesel</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="str">
+        <f t="shared" ref="B7:B17" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
+        <v>UC_RSD_MaxGrowth_Biodiesel</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="F7" t="s">
+        <v>197</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="29">
+        <f>1+C23</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="16">
+        <f>-D23</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5</v>
+      </c>
+      <c r="N7" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
+        <v>RSD maximum growth rate of Biomass</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_Biomass</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="F8" t="s">
+        <v>207</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="29">
+        <f>1+C23</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="16">
+        <f>-D23</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M8" s="2">
+        <v>5</v>
+      </c>
+      <c r="N8" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
+        <v>RSD maximum growth rate of Biomass</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_Coal</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="F9" t="s">
+        <v>208</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="29">
+        <f>1+C24</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="16">
+        <f>-D24</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M9" s="2">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
+        <v>RSD maximum growth rate of Coal</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_Peat</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="F10" t="s">
+        <v>209</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="29">
+        <f>1+C25</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="16">
+        <f>-D25</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A25, "maximum growth rate of",B25)</f>
+        <v>RSD maximum growth rate of Peat</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_Electricity</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="F11" t="s">
+        <v>210</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="29">
+        <f>1+C26</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
+      <c r="L11" s="16">
+        <f>-D26</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M11" s="2">
+        <v>5</v>
+      </c>
+      <c r="N11" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
+        <v>RSD maximum growth rate of Electricity</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_Ethanol</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="F12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="29">
+        <f t="shared" ref="J12:J17" si="1">1+C27</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+      <c r="L12" s="16">
+        <f t="shared" ref="L12:L17" si="2">-D27</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M12" s="2">
+        <v>5</v>
+      </c>
+      <c r="N12" s="2" t="str">
+        <f t="shared" ref="N12:N17" si="3">_xlfn.TEXTJOIN(" ",TRUE,A27, "maximum growth rate of",B27)</f>
+        <v>RSD maximum growth rate of Ethanol</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_Gas</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="F13" t="s">
+        <v>212</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H13" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="29">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1</v>
+      </c>
+      <c r="L13" s="16">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="M13" s="2">
+        <v>5</v>
+      </c>
+      <c r="N13" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>RSD maximum growth rate of Gas</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_DistrictHeat</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="F14" t="s">
+        <v>213</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H14" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J14" s="29">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1</v>
+      </c>
+      <c r="L14" s="16">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="M14" s="2">
+        <v>5</v>
+      </c>
+      <c r="N14" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>RSD maximum growth rate of DistrictHeat</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_LPG</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="2"/>
+      <c r="F15" t="s">
+        <v>214</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H15" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" s="29">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+      <c r="L15" s="16">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="M15" s="2">
+        <v>5</v>
+      </c>
+      <c r="N15" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>RSD maximum growth rate of LPG</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_Kerosene</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="F16" t="s">
+        <v>215</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H16" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" s="29">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+      <c r="L16" s="16">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="M16" s="2">
+        <v>5</v>
+      </c>
+      <c r="N16" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>RSD maximum growth rate of Kerosene</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_Solar</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="F17" t="s">
+        <v>216</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H17" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J17" s="29">
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K17" s="2">
+        <v>1</v>
+      </c>
+      <c r="L17" s="16">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="M17" s="2">
+        <v>5</v>
+      </c>
+      <c r="N17" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>RSD maximum growth rate of Solar</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="16"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B21" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D22">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>196</v>
+      </c>
+      <c r="B23" t="s">
+        <v>138</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>196</v>
+      </c>
+      <c r="B24" t="s">
+        <v>199</v>
+      </c>
+      <c r="C24" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D24">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>196</v>
+      </c>
+      <c r="B25" t="s">
+        <v>200</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>196</v>
+      </c>
+      <c r="B26" t="s">
+        <v>201</v>
+      </c>
+      <c r="C26" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27" t="s">
+        <v>202</v>
+      </c>
+      <c r="C27" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>196</v>
+      </c>
+      <c r="B28" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>196</v>
+      </c>
+      <c r="B29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>196</v>
+      </c>
+      <c r="B30" t="s">
+        <v>203</v>
+      </c>
+      <c r="C30" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B31" t="s">
+        <v>204</v>
+      </c>
+      <c r="C31" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>196</v>
+      </c>
+      <c r="B32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C32" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D32">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A2:N18"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="40" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
+        <v>UC_SRV_MaxGrowth_Biomass</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="29">
+        <f>1+C14</f>
+        <v>1.05</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="16">
+        <f>-D14</f>
+        <v>-0.3</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5</v>
+      </c>
+      <c r="N6" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
+        <v>SRV maximum growth rate of Biomass</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
+        <v>UC_SRV_MaxGrowth_Biogas</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H7" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" s="29">
+        <f>1+C15</f>
+        <v>1.05</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="16">
+        <f>-D15</f>
+        <v>-0.3</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5</v>
+      </c>
+      <c r="N7" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
+        <v>SRV maximum growth rate of Biogas</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
+        <v>UC_SRV_MaxGrowth_AmbientHeat</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H8" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J8" s="29">
+        <f>1+C16</f>
+        <v>1.05</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="16">
+        <f>-D16</f>
+        <v>-0.3</v>
+      </c>
+      <c r="M8" s="2">
+        <v>5</v>
+      </c>
+      <c r="N8" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A16, "maximum growth rate of",B16)</f>
+        <v>SRV maximum growth rate of AmbientHeat</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A17,"MaxGrowth",B17)</f>
+        <v>UC_SRV_MaxGrowth_DistrictHeat</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="29">
+        <f>1+C17</f>
+        <v>1.05</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1</v>
+      </c>
+      <c r="L9" s="16">
+        <f>-D17</f>
+        <v>-0.3</v>
+      </c>
+      <c r="M9" s="2">
+        <v>5</v>
+      </c>
+      <c r="N9" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A17, "maximum growth rate of",B17)</f>
+        <v>SRV maximum growth rate of DistrictHeat</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
+        <v>UC_SRV_MaxGrowth_Gas</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="H10" s="2">
+        <v>2018</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="29">
+        <f>1+C18</f>
+        <v>1.08</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+      <c r="L10" s="16">
+        <f>-D18</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M10" s="2">
+        <v>5</v>
+      </c>
+      <c r="N10" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A18, "maximum growth rate of",B18)</f>
+        <v>SRV maximum growth rate of Gas</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D14">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>140</v>
+      </c>
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D15">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" t="s">
+        <v>191</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D16">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>140</v>
+      </c>
+      <c r="B17" t="s">
+        <v>192</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D17">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" t="s">
+        <v>194</v>
+      </c>
+      <c r="C18" s="11">
+        <v>0.08</v>
+      </c>
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:P53"/>
@@ -7840,417 +9108,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:N18"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="40" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="str">
-        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
-        <v>~UC_Sets: R_E: IE,National</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
-        <v>UC_SRV_MaxGrowth_Biomass</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H6" s="2">
-        <v>2018</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J6" s="29">
-        <f>1+C14</f>
-        <v>1.05</v>
-      </c>
-      <c r="K6" s="2">
-        <v>1</v>
-      </c>
-      <c r="L6" s="16">
-        <f>-D14</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M6" s="2">
-        <v>5</v>
-      </c>
-      <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
-        <v>SRV maximum growth rate of Biomass</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
-        <v>UC_SRV_MaxGrowth_Biogas</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="F7" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H7" s="2">
-        <v>2018</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="29">
-        <f>1+C15</f>
-        <v>1.05</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1</v>
-      </c>
-      <c r="L7" s="16">
-        <f>-D15</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M7" s="2">
-        <v>5</v>
-      </c>
-      <c r="N7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
-        <v>SRV maximum growth rate of Biogas</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
-        <v>UC_SRV_MaxGrowth_AmbientHeat</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="F8" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H8" s="2">
-        <v>2021</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J8" s="29">
-        <f>1+C16</f>
-        <v>1.05</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1</v>
-      </c>
-      <c r="L8" s="16">
-        <f>-D16</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M8" s="2">
-        <v>5</v>
-      </c>
-      <c r="N8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A16, "maximum growth rate of",B16)</f>
-        <v>SRV maximum growth rate of AmbientHeat</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A17,"MaxGrowth",B17)</f>
-        <v>UC_SRV_MaxGrowth_DistrictHeat</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H9" s="2">
-        <v>2021</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="29">
-        <f>1+C17</f>
-        <v>1.05</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1</v>
-      </c>
-      <c r="L9" s="16">
-        <f>-D17</f>
-        <v>-0.3</v>
-      </c>
-      <c r="M9" s="2">
-        <v>5</v>
-      </c>
-      <c r="N9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A17, "maximum growth rate of",B17)</f>
-        <v>SRV maximum growth rate of DistrictHeat</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
-        <v>UC_SRV_MaxGrowth_Gas</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>195</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="H10" s="2">
-        <v>2018</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="29">
-        <f>1+C18</f>
-        <v>1.08</v>
-      </c>
-      <c r="K10" s="2">
-        <v>1</v>
-      </c>
-      <c r="L10" s="16">
-        <f>-D18</f>
-        <v>-0.5</v>
-      </c>
-      <c r="M10" s="2">
-        <v>5</v>
-      </c>
-      <c r="N10" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A18, "maximum growth rate of",B18)</f>
-        <v>SRV maximum growth rate of Gas</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="29"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>117</v>
-      </c>
-      <c r="D13" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>140</v>
-      </c>
-      <c r="B14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D14">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D15">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" t="s">
-        <v>191</v>
-      </c>
-      <c r="C16" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D16">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B17" t="s">
-        <v>192</v>
-      </c>
-      <c r="C17" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D17">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>140</v>
-      </c>
-      <c r="B18" t="s">
-        <v>194</v>
-      </c>
-      <c r="C18" s="11">
-        <v>0.08</v>
-      </c>
-      <c r="D18">
-        <v>0.5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -8258,15 +9115,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -8477,6 +9325,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
@@ -8487,14 +9344,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8511,4 +9360,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add a tax on net amount of commodities bound by max growth rates
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12547C9-8D0B-49E7-BB28-B1E07F376044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7955A760-D012-47BC-8449-3B3431D6552A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -21,6 +21,9 @@
     <sheet name="SRV" sheetId="5" r:id="rId6"/>
     <sheet name="TRA" sheetId="1" r:id="rId7"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId8"/>
+  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="3" hidden="1">#REF!</definedName>
@@ -172,7 +175,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="223">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -581,9 +584,6 @@
     <t>PWR</t>
   </si>
   <si>
-    <t>SRVAHT</t>
-  </si>
-  <si>
     <t>BEV</t>
   </si>
   <si>
@@ -812,9 +812,6 @@
     <t>Solar</t>
   </si>
   <si>
-    <t>RSDAHT</t>
-  </si>
-  <si>
     <t>RSDWOO</t>
   </si>
   <si>
@@ -843,6 +840,30 @@
   </si>
   <si>
     <t>RSDSOL</t>
+  </si>
+  <si>
+    <t>~TFM_INS</t>
+  </si>
+  <si>
+    <t>TimeSlice</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Cset_CN</t>
+  </si>
+  <si>
+    <t>RSDAHT,RSDAHT2</t>
+  </si>
+  <si>
+    <t>SRVAHT,SRVAHT2</t>
+  </si>
+  <si>
+    <t>BIOGAS1G,BIOGAS2G</t>
+  </si>
+  <si>
+    <t>COM_TAXNET</t>
   </si>
 </sst>
 </file>
@@ -855,7 +876,7 @@
     <numFmt numFmtId="166" formatCode="0.000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -985,8 +1006,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1038,6 +1066,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="44"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1117,7 +1157,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1200,6 +1240,13 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1609,6 +1656,48 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Cover"/>
+      <sheetName val="Regions"/>
+      <sheetName val="PWR"/>
+      <sheetName val="SYS"/>
+      <sheetName val="SUP"/>
+      <sheetName val="SRV"/>
+      <sheetName val="RSD"/>
+      <sheetName val="TRA"/>
+      <sheetName val="DataFill"/>
+      <sheetName val="RSDAFC"/>
+      <sheetName val="RSDAFA"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="3">
+          <cell r="C3" t="str">
+            <v>IE</v>
+          </cell>
+          <cell r="D3" t="str">
+            <v>National</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2347,12 +2436,12 @@
       <c r="Z15" s="31"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
+      <c r="A16" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="32"/>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -2434,13 +2523,13 @@
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
-        <v>163</v>
-      </c>
-      <c r="B19" s="45" t="s">
-        <v>174</v>
-      </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
+        <v>162</v>
+      </c>
+      <c r="B19" s="50" t="s">
+        <v>173</v>
+      </c>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
       <c r="G19" s="39"/>
@@ -2466,13 +2555,13 @@
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
-        <v>164</v>
-      </c>
-      <c r="B20" s="45" t="s">
-        <v>177</v>
-      </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
+        <v>163</v>
+      </c>
+      <c r="B20" s="50" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
       <c r="G20" s="39"/>
@@ -2498,10 +2587,10 @@
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C21" s="40"/>
       <c r="D21" s="40"/>
@@ -2558,13 +2647,13 @@
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
-        <v>166</v>
-      </c>
-      <c r="B23" s="45" t="s">
-        <v>179</v>
-      </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
+        <v>165</v>
+      </c>
+      <c r="B23" s="50" t="s">
+        <v>178</v>
+      </c>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
@@ -2590,11 +2679,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="37"/>
-      <c r="B24" s="45" t="s">
-        <v>175</v>
-      </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
+      <c r="B24" s="50" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
@@ -2621,7 +2710,7 @@
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="40" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C25" s="40"/>
       <c r="D25" s="40"/>
@@ -2650,13 +2739,13 @@
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>167</v>
-      </c>
-      <c r="B26" s="45" t="s">
-        <v>176</v>
-      </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
+        <v>166</v>
+      </c>
+      <c r="B26" s="50" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
@@ -2738,7 +2827,7 @@
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B29" s="41">
         <v>1</v>
@@ -2770,13 +2859,13 @@
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="B30" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="B30" s="47" t="s">
-        <v>170</v>
-      </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="42"/>
       <c r="F30" s="42"/>
       <c r="G30" s="31"/>
@@ -2802,13 +2891,13 @@
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="B31" s="45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
       <c r="E31" s="42"/>
       <c r="F31" s="42"/>
       <c r="G31" s="31"/>
@@ -2835,7 +2924,7 @@
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="43"/>
       <c r="B32" s="44" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C32" s="43"/>
       <c r="D32" s="43"/>
@@ -5526,10 +5615,240 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89417C8F-9D07-4311-9372-0B0C534E50C4}">
-  <dimension ref="A2:N11"/>
+  <dimension ref="A2:N17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="str">
+        <f t="shared" ref="B6" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A10,"MaxGrowth",B10)</f>
+        <v>UC_SUP_MaxGrowth_BIOGAS</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="26">
+        <f t="shared" ref="G6" si="1">1+$C10</f>
+        <v>1.4</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="16">
+        <f t="shared" ref="I6" si="2">-D10</f>
+        <v>-0.2</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2" t="str">
+        <f t="shared" ref="K6" si="3">_xlfn.TEXTJOIN(" ",TRUE,A10, "maximum growth rate of",B10)</f>
+        <v>SUP maximum growth rate of BIOGAS</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>186</v>
+      </c>
+      <c r="B10" t="s">
+        <v>187</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="H15" s="46"/>
+    </row>
+    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="E16" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="48" t="str">
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G16" s="48" t="str">
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H16" s="49" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>222</v>
+      </c>
+      <c r="E17">
+        <v>2018</v>
+      </c>
+      <c r="F17">
+        <v>2222</v>
+      </c>
+      <c r="G17">
+        <f>F17</f>
+        <v>2222</v>
+      </c>
+      <c r="H17" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
+  <sheetPr codeName="Sheet2"/>
+  <dimension ref="A2:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5608,186 +5927,6 @@
         <v>8</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A10,"MaxGrowth",B10)</f>
-        <v>UC_SUP_MaxGrowth_BIOGAS</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2018</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="26">
-        <f t="shared" ref="G6" si="1">1+$C10</f>
-        <v>1.4</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="16">
-        <f t="shared" ref="I6" si="2">-D10</f>
-        <v>-0.2</v>
-      </c>
-      <c r="J6" s="2">
-        <v>5</v>
-      </c>
-      <c r="K6" s="2" t="str">
-        <f t="shared" ref="K6" si="3">_xlfn.TEXTJOIN(" ",TRUE,A10, "maximum growth rate of",B10)</f>
-        <v>SUP maximum growth rate of BIOGAS</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>117</v>
-      </c>
-      <c r="D9" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>187</v>
-      </c>
-      <c r="B10" t="s">
-        <v>188</v>
-      </c>
-      <c r="C10" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="D10">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="H11" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:N27"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="str">
-        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
-        <v>~UC_Sets: R_E: IE,National</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -5920,7 +6059,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E9" s="2">
         <v>2020</v>
@@ -5956,7 +6095,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E10">
         <v>2018</v>
@@ -5992,7 +6131,7 @@
         <v>13</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E11">
         <v>2018</v>
@@ -6074,7 +6213,7 @@
         <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C17" s="11">
         <v>0.2</v>
@@ -6088,7 +6227,7 @@
         <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" s="11">
         <v>0.2</v>
@@ -6102,7 +6241,7 @@
         <v>128</v>
       </c>
       <c r="B19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C19" s="11">
         <v>0.2</v>
@@ -6142,10 +6281,10 @@
         <v>8</v>
       </c>
       <c r="G23" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>182</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>183</v>
       </c>
       <c r="I23" s="4" t="s">
         <v>11</v>
@@ -6156,17 +6295,17 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E24" s="2">
         <v>2019</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G24" s="26">
         <f>1+$C29</f>
@@ -6179,20 +6318,20 @@
         <v>3</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E25" s="2">
         <v>2020</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G25" s="26">
         <f>1+$C30</f>
@@ -6206,17 +6345,17 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E26">
         <v>2026</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G26" s="26">
         <f>1+$C30</f>
@@ -6229,7 +6368,7 @@
         <v>3</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -6238,7 +6377,7 @@
         <v>2027</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H27" s="16">
         <v>2</v>
@@ -6251,10 +6390,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
-  <dimension ref="A2:N32"/>
+  <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6262,7 +6401,8 @@
     <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
@@ -6350,13 +6490,13 @@
         <v>8</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>11</v>
@@ -6371,14 +6511,14 @@
         <v>UC_RSD_MaxGrowth_AmbientHeat</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H6" s="2">
         <v>2021</v>
@@ -6411,14 +6551,14 @@
         <v>UC_RSD_MaxGrowth_Biodiesel</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="2"/>
       <c r="F7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H7" s="2">
         <v>2021</v>
@@ -6451,14 +6591,14 @@
         <v>UC_RSD_MaxGrowth_Biomass</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D8" s="2"/>
       <c r="F8" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H8" s="2">
         <v>2021</v>
@@ -6491,14 +6631,14 @@
         <v>UC_RSD_MaxGrowth_Coal</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D9" s="2"/>
       <c r="F9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H9" s="2">
         <v>2021</v>
@@ -6531,14 +6671,14 @@
         <v>UC_RSD_MaxGrowth_Peat</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="2"/>
       <c r="F10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H10" s="2">
         <v>2021</v>
@@ -6571,14 +6711,14 @@
         <v>UC_RSD_MaxGrowth_Electricity</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D11" s="2"/>
       <c r="F11" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H11" s="2">
         <v>2021</v>
@@ -6611,14 +6751,14 @@
         <v>UC_RSD_MaxGrowth_Ethanol</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D12" s="2"/>
       <c r="F12" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H12" s="2">
         <v>2021</v>
@@ -6651,14 +6791,14 @@
         <v>UC_RSD_MaxGrowth_Gas</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D13" s="2"/>
       <c r="F13" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H13" s="2">
         <v>2021</v>
@@ -6691,14 +6831,14 @@
         <v>UC_RSD_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D14" s="2"/>
       <c r="F14" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H14" s="2">
         <v>2021</v>
@@ -6731,14 +6871,14 @@
         <v>UC_RSD_MaxGrowth_LPG</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D15" s="2"/>
       <c r="F15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H15" s="2">
         <v>2021</v>
@@ -6771,14 +6911,14 @@
         <v>UC_RSD_MaxGrowth_Kerosene</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D16" s="2"/>
       <c r="F16" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H16" s="2">
         <v>2021</v>
@@ -6811,14 +6951,14 @@
         <v>UC_RSD_MaxGrowth_Solar</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D17" s="2"/>
       <c r="F17" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H17" s="2">
         <v>2021</v>
@@ -6863,23 +7003,23 @@
         <v>117</v>
       </c>
       <c r="D20" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B22" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C22" s="11">
         <v>0.1</v>
@@ -6890,10 +7030,10 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B23" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C23" s="11">
         <v>0.1</v>
@@ -6904,10 +7044,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C24" s="11">
         <v>0.1</v>
@@ -6918,10 +7058,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B25" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C25" s="11">
         <v>0.1</v>
@@ -6932,10 +7072,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C26" s="11">
         <v>0.1</v>
@@ -6946,10 +7086,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B27" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C27" s="11">
         <v>0.1</v>
@@ -6960,10 +7100,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C28" s="11">
         <v>0.1</v>
@@ -6974,10 +7114,10 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B29" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C29" s="11">
         <v>0.1</v>
@@ -6988,10 +7128,10 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B30" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C30" s="11">
         <v>0.1</v>
@@ -7002,10 +7142,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B31" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C31" s="11">
         <v>0.1</v>
@@ -7016,16 +7156,67 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C32" s="11">
         <v>0.1</v>
       </c>
       <c r="D32">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
+    </row>
+    <row r="36" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="E36" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F36" s="48" t="str">
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G36" s="48" t="str">
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H36" s="49" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>222</v>
+      </c>
+      <c r="E37">
+        <v>2018</v>
+      </c>
+      <c r="F37">
+        <v>2222</v>
+      </c>
+      <c r="G37">
+        <f>F37</f>
+        <v>2222</v>
+      </c>
+      <c r="H37" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F17)</f>
+        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET,RSDLPG,RSDKER,RSDSOL</v>
       </c>
     </row>
   </sheetData>
@@ -7036,18 +7227,19 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:N18"/>
+  <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -7132,13 +7324,13 @@
         <v>8</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>147</v>
-      </c>
       <c r="L5" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>11</v>
@@ -7153,14 +7345,14 @@
         <v>UC_SRV_MaxGrowth_Biomass</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H6" s="2">
         <v>2018</v>
@@ -7193,14 +7385,14 @@
         <v>UC_SRV_MaxGrowth_Biogas</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="2"/>
       <c r="F7" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="H7" s="2">
         <v>2018</v>
@@ -7233,14 +7425,14 @@
         <v>UC_SRV_MaxGrowth_AmbientHeat</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>129</v>
+        <v>220</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H8" s="2">
         <v>2021</v>
@@ -7273,14 +7465,14 @@
         <v>UC_SRV_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H9" s="2">
         <v>2021</v>
@@ -7313,14 +7505,14 @@
         <v>UC_SRV_MaxGrowth_Gas</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H10" s="2">
         <v>2018</v>
@@ -7366,15 +7558,15 @@
         <v>117</v>
       </c>
       <c r="D13" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C14" s="11">
         <v>0.05</v>
@@ -7385,10 +7577,10 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C15" s="11">
         <v>0.05</v>
@@ -7399,10 +7591,10 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C16" s="11">
         <v>0.05</v>
@@ -7411,12 +7603,12 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C17" s="11">
         <v>0.05</v>
@@ -7425,18 +7617,68 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C18" s="11">
         <v>0.08</v>
       </c>
       <c r="D18">
         <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="H22" s="46"/>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="47" t="s">
+        <v>217</v>
+      </c>
+      <c r="E23" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" s="48" t="str">
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!C$3,"*")</f>
+        <v>IE</v>
+      </c>
+      <c r="G23" s="48" t="str">
+        <f>IF([1]Regions!C$3&lt;&gt;"",[1]Regions!D$3,"*")</f>
+        <v>National</v>
+      </c>
+      <c r="H23" s="49" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>222</v>
+      </c>
+      <c r="E24">
+        <v>2018</v>
+      </c>
+      <c r="F24">
+        <v>2222</v>
+      </c>
+      <c r="G24">
+        <f>F24</f>
+        <v>2222</v>
+      </c>
+      <c r="H24" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F10)</f>
+        <v>SRVBIO,SRVBGS,SRVAHT,SRVAHT2,SRVHET,SRVGAS</v>
       </c>
     </row>
   </sheetData>
@@ -7449,9 +7691,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:P53"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8306,27 +8546,27 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I26" t="s">
+        <v>150</v>
+      </c>
+      <c r="J26" t="s">
         <v>151</v>
-      </c>
-      <c r="J26" t="s">
-        <v>152</v>
       </c>
       <c r="K26" t="s">
         <v>117</v>
       </c>
       <c r="L26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K27" s="11">
         <v>0.8</v>
@@ -8340,10 +8580,10 @@
         <v>29</v>
       </c>
       <c r="I28" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J28" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K28" s="11">
         <v>0.8</v>
@@ -8365,10 +8605,10 @@
         <v>32</v>
       </c>
       <c r="I29" t="s">
+        <v>147</v>
+      </c>
+      <c r="J29" t="s">
         <v>148</v>
-      </c>
-      <c r="J29" t="s">
-        <v>149</v>
       </c>
       <c r="K29" s="11">
         <v>0.5</v>
@@ -8378,7 +8618,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="53" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
@@ -8395,10 +8635,10 @@
         <v>4.3671013742841359E-2</v>
       </c>
       <c r="I30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K30" s="11">
         <v>0.5</v>
@@ -8408,7 +8648,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
+      <c r="A31" s="53"/>
       <c r="B31" t="s">
         <v>25</v>
       </c>
@@ -8423,10 +8663,10 @@
         <v>6.5375711631511485E-2</v>
       </c>
       <c r="I31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K31" s="11">
         <v>0.5</v>
@@ -8436,7 +8676,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
+      <c r="A32" s="53"/>
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -8451,10 +8691,10 @@
         <v>4.4214694236691596E-2</v>
       </c>
       <c r="I32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J32" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K32" s="11">
         <v>0.5</v>
@@ -8464,7 +8704,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
+      <c r="A33" s="53"/>
       <c r="B33" t="s">
         <v>23</v>
       </c>
@@ -8479,10 +8719,10 @@
         <v>4.9391983185707852E-2</v>
       </c>
       <c r="I33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K33" s="11">
         <v>0.5</v>
@@ -8492,7 +8732,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
+      <c r="A34" s="53"/>
       <c r="B34" t="s">
         <v>22</v>
       </c>
@@ -8507,10 +8747,10 @@
         <v>5.7573599240265907E-2</v>
       </c>
       <c r="I34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K34" s="11">
         <v>0.5</v>
@@ -8520,7 +8760,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
+      <c r="A35" s="53"/>
       <c r="B35" t="s">
         <v>21</v>
       </c>
@@ -8535,10 +8775,10 @@
         <v>7.187086899046824E-2</v>
       </c>
       <c r="I35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K35" s="11">
         <v>0.5</v>
@@ -8562,10 +8802,10 @@
         <v>5.5865068892149296E-2</v>
       </c>
       <c r="I36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J36" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K36" s="11">
         <v>0.5</v>
@@ -8589,10 +8829,10 @@
         <v>6.1874562947601935E-2</v>
       </c>
       <c r="I37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J37" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K37" s="11">
         <v>0.5</v>
@@ -8616,10 +8856,10 @@
         <v>5.7044321200540614E-2</v>
       </c>
       <c r="I38" t="s">
+        <v>133</v>
+      </c>
+      <c r="J38" t="s">
         <v>134</v>
-      </c>
-      <c r="J38" t="s">
-        <v>135</v>
       </c>
       <c r="K38" s="11">
         <v>0.5</v>
@@ -8644,10 +8884,10 @@
         <v>4.9170087453150095E-2</v>
       </c>
       <c r="I39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J39" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K39" s="11">
         <v>0.5</v>
@@ -8661,10 +8901,10 @@
         <v>28</v>
       </c>
       <c r="I40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J40" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K40" s="11">
         <v>0.5</v>
@@ -8675,10 +8915,10 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K41" s="11">
         <v>0.5</v>
@@ -8689,10 +8929,10 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I42" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K42" s="11">
         <v>0.5</v>
@@ -8703,10 +8943,10 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J43" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K43" s="11">
         <v>0.5</v>
@@ -8717,10 +8957,10 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J44" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K44" s="11">
         <v>0.5</v>
@@ -8731,7 +8971,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -9109,12 +9349,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9325,7 +9559,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9334,16 +9568,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9362,10 +9593,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust the load factor of the freight vehicles Modify CNG/BioCNG delivery costs Modify the stock retirement for freight vehicles
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bcf850925e8c42cd/Desktop/times-ireland-model/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D12547C9-8D0B-49E7-BB28-B1E07F376044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D12547C9-8D0B-49E7-BB28-B1E07F376044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4CA94C66-CC8B-47EE-8BB4-69C443DDFA2E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -1913,20 +1913,20 @@
       <selection activeCell="B20" sqref="B20:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="1" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="8" max="10" width="8.109375" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.109375" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1954,7 +1954,7 @@
       <c r="Y1" s="31"/>
       <c r="Z1" s="31"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -1982,7 +1982,7 @@
       <c r="Y2" s="31"/>
       <c r="Z2" s="31"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -2010,7 +2010,7 @@
       <c r="Y3" s="31"/>
       <c r="Z3" s="31"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="30"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -2038,7 +2038,7 @@
       <c r="Y4" s="31"/>
       <c r="Z4" s="31"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
@@ -2066,7 +2066,7 @@
       <c r="Y5" s="31"/>
       <c r="Z5" s="31"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -2094,7 +2094,7 @@
       <c r="Y6" s="31"/>
       <c r="Z6" s="31"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
@@ -2122,7 +2122,7 @@
       <c r="Y7" s="31"/>
       <c r="Z7" s="31"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
@@ -2150,7 +2150,7 @@
       <c r="Y8" s="31"/>
       <c r="Z8" s="31"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
@@ -2178,7 +2178,7 @@
       <c r="Y9" s="31"/>
       <c r="Z9" s="31"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
@@ -2206,7 +2206,7 @@
       <c r="Y10" s="31"/>
       <c r="Z10" s="31"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
@@ -2234,7 +2234,7 @@
       <c r="Y11" s="31"/>
       <c r="Z11" s="31"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
@@ -2262,7 +2262,7 @@
       <c r="Y12" s="31"/>
       <c r="Z12" s="31"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
@@ -2290,7 +2290,7 @@
       <c r="Y13" s="31"/>
       <c r="Z13" s="31"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
@@ -2318,7 +2318,7 @@
       <c r="Y14" s="31"/>
       <c r="Z14" s="31"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="30"/>
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
@@ -2346,7 +2346,7 @@
       <c r="Y15" s="31"/>
       <c r="Z15" s="31"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="46" t="s">
         <v>162</v>
       </c>
@@ -2376,7 +2376,7 @@
       <c r="Y16" s="31"/>
       <c r="Z16" s="31"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34"/>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
@@ -2404,7 +2404,7 @@
       <c r="Y17" s="31"/>
       <c r="Z17" s="31"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="34"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
@@ -2432,7 +2432,7 @@
       <c r="Y18" s="31"/>
       <c r="Z18" s="31"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>163</v>
       </c>
@@ -2464,7 +2464,7 @@
       <c r="Y19" s="31"/>
       <c r="Z19" s="31"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>164</v>
       </c>
@@ -2496,7 +2496,7 @@
       <c r="Y20" s="31"/>
       <c r="Z20" s="31"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>165</v>
       </c>
@@ -2528,7 +2528,7 @@
       <c r="Y21" s="31"/>
       <c r="Z21" s="31"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37"/>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -2556,7 +2556,7 @@
       <c r="Y22" s="31"/>
       <c r="Z22" s="31"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>166</v>
       </c>
@@ -2588,7 +2588,7 @@
       <c r="Y23" s="31"/>
       <c r="Z23" s="31"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
       <c r="B24" s="45" t="s">
         <v>175</v>
@@ -2618,7 +2618,7 @@
       <c r="Y24" s="31"/>
       <c r="Z24" s="31"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" s="40" t="s">
         <v>176</v>
@@ -2648,7 +2648,7 @@
       <c r="Y25" s="31"/>
       <c r="Z25" s="31"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>167</v>
       </c>
@@ -2680,7 +2680,7 @@
       <c r="Y26" s="31"/>
       <c r="Z26" s="31"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37"/>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
@@ -2708,7 +2708,7 @@
       <c r="Y27" s="31"/>
       <c r="Z27" s="31"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -2736,7 +2736,7 @@
       <c r="Y28" s="31"/>
       <c r="Z28" s="31"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="37" t="s">
         <v>168</v>
       </c>
@@ -2768,7 +2768,7 @@
       <c r="Y29" s="31"/>
       <c r="Z29" s="31"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="37" t="s">
         <v>169</v>
       </c>
@@ -2800,7 +2800,7 @@
       <c r="Y30" s="31"/>
       <c r="Z30" s="31"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37" t="s">
         <v>171</v>
       </c>
@@ -2832,7 +2832,7 @@
       <c r="Y31" s="31"/>
       <c r="Z31" s="31"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="43"/>
       <c r="B32" s="44" t="s">
         <v>173</v>
@@ -2862,7 +2862,7 @@
       <c r="Y32" s="31"/>
       <c r="Z32" s="31"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
@@ -2890,7 +2890,7 @@
       <c r="Y33" s="31"/>
       <c r="Z33" s="31"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="30"/>
       <c r="B34" s="30"/>
       <c r="C34" s="30"/>
@@ -2918,7 +2918,7 @@
       <c r="Y34" s="31"/>
       <c r="Z34" s="31"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="30"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -2946,7 +2946,7 @@
       <c r="Y35" s="31"/>
       <c r="Z35" s="31"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="30"/>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
@@ -2974,7 +2974,7 @@
       <c r="Y36" s="31"/>
       <c r="Z36" s="31"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="30"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
@@ -3002,7 +3002,7 @@
       <c r="Y37" s="31"/>
       <c r="Z37" s="31"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="30"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -3030,7 +3030,7 @@
       <c r="Y38" s="31"/>
       <c r="Z38" s="31"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="30"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -3058,7 +3058,7 @@
       <c r="Y39" s="31"/>
       <c r="Z39" s="31"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="30"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
@@ -3086,7 +3086,7 @@
       <c r="Y40" s="31"/>
       <c r="Z40" s="31"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -3114,7 +3114,7 @@
       <c r="Y41" s="31"/>
       <c r="Z41" s="31"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="30"/>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
@@ -3142,7 +3142,7 @@
       <c r="Y42" s="31"/>
       <c r="Z42" s="31"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" s="31"/>
       <c r="B43" s="31"/>
       <c r="C43" s="31"/>
@@ -3170,7 +3170,7 @@
       <c r="Y43" s="31"/>
       <c r="Z43" s="31"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="31"/>
       <c r="B44" s="31"/>
       <c r="C44" s="31"/>
@@ -3198,7 +3198,7 @@
       <c r="Y44" s="31"/>
       <c r="Z44" s="31"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="31"/>
       <c r="B45" s="31"/>
       <c r="C45" s="31"/>
@@ -3226,7 +3226,7 @@
       <c r="Y45" s="31"/>
       <c r="Z45" s="31"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="31"/>
       <c r="B46" s="31"/>
       <c r="C46" s="31"/>
@@ -3254,7 +3254,7 @@
       <c r="Y46" s="31"/>
       <c r="Z46" s="31"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="31"/>
       <c r="B47" s="31"/>
       <c r="C47" s="31"/>
@@ -3282,7 +3282,7 @@
       <c r="Y47" s="31"/>
       <c r="Z47" s="31"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="31"/>
       <c r="B48" s="31"/>
       <c r="C48" s="31"/>
@@ -3310,7 +3310,7 @@
       <c r="Y48" s="31"/>
       <c r="Z48" s="31"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="31"/>
       <c r="B49" s="31"/>
       <c r="C49" s="31"/>
@@ -3338,7 +3338,7 @@
       <c r="Y49" s="31"/>
       <c r="Z49" s="31"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="31"/>
       <c r="B50" s="31"/>
       <c r="C50" s="31"/>
@@ -3366,7 +3366,7 @@
       <c r="Y50" s="31"/>
       <c r="Z50" s="31"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="31"/>
       <c r="B51" s="31"/>
       <c r="C51" s="31"/>
@@ -3394,7 +3394,7 @@
       <c r="Y51" s="31"/>
       <c r="Z51" s="31"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="31"/>
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
@@ -3422,7 +3422,7 @@
       <c r="Y52" s="31"/>
       <c r="Z52" s="31"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="31"/>
       <c r="B53" s="31"/>
       <c r="C53" s="31"/>
@@ -3450,7 +3450,7 @@
       <c r="Y53" s="31"/>
       <c r="Z53" s="31"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="31"/>
       <c r="B54" s="31"/>
       <c r="C54" s="31"/>
@@ -3478,7 +3478,7 @@
       <c r="Y54" s="31"/>
       <c r="Z54" s="31"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="31"/>
       <c r="B55" s="31"/>
       <c r="C55" s="31"/>
@@ -3506,7 +3506,7 @@
       <c r="Y55" s="31"/>
       <c r="Z55" s="31"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="31"/>
       <c r="B56" s="31"/>
       <c r="C56" s="31"/>
@@ -3534,7 +3534,7 @@
       <c r="Y56" s="31"/>
       <c r="Z56" s="31"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" s="31"/>
       <c r="B57" s="31"/>
       <c r="C57" s="31"/>
@@ -3562,7 +3562,7 @@
       <c r="Y57" s="31"/>
       <c r="Z57" s="31"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" s="31"/>
       <c r="B58" s="31"/>
       <c r="C58" s="31"/>
@@ -3590,7 +3590,7 @@
       <c r="Y58" s="31"/>
       <c r="Z58" s="31"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" s="31"/>
       <c r="B59" s="31"/>
       <c r="C59" s="31"/>
@@ -3618,7 +3618,7 @@
       <c r="Y59" s="31"/>
       <c r="Z59" s="31"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="31"/>
       <c r="B60" s="31"/>
       <c r="C60" s="31"/>
@@ -3646,7 +3646,7 @@
       <c r="Y60" s="31"/>
       <c r="Z60" s="31"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" s="31"/>
       <c r="B61" s="31"/>
       <c r="C61" s="31"/>
@@ -3674,7 +3674,7 @@
       <c r="Y61" s="31"/>
       <c r="Z61" s="31"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="31"/>
       <c r="B62" s="31"/>
       <c r="C62" s="31"/>
@@ -3702,7 +3702,7 @@
       <c r="Y62" s="31"/>
       <c r="Z62" s="31"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" s="31"/>
       <c r="B63" s="31"/>
       <c r="C63" s="31"/>
@@ -3730,7 +3730,7 @@
       <c r="Y63" s="31"/>
       <c r="Z63" s="31"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="31"/>
       <c r="B64" s="31"/>
       <c r="C64" s="31"/>
@@ -3758,7 +3758,7 @@
       <c r="Y64" s="31"/>
       <c r="Z64" s="31"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="31"/>
       <c r="B65" s="31"/>
       <c r="C65" s="31"/>
@@ -3786,7 +3786,7 @@
       <c r="Y65" s="31"/>
       <c r="Z65" s="31"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="31"/>
       <c r="B66" s="31"/>
       <c r="C66" s="31"/>
@@ -3814,7 +3814,7 @@
       <c r="Y66" s="31"/>
       <c r="Z66" s="31"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="31"/>
       <c r="B67" s="31"/>
       <c r="C67" s="31"/>
@@ -3842,7 +3842,7 @@
       <c r="Y67" s="31"/>
       <c r="Z67" s="31"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" s="31"/>
       <c r="B68" s="31"/>
       <c r="C68" s="31"/>
@@ -3870,7 +3870,7 @@
       <c r="Y68" s="31"/>
       <c r="Z68" s="31"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" s="31"/>
       <c r="B69" s="31"/>
       <c r="C69" s="31"/>
@@ -3898,7 +3898,7 @@
       <c r="Y69" s="31"/>
       <c r="Z69" s="31"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="31"/>
       <c r="B70" s="31"/>
       <c r="C70" s="31"/>
@@ -3926,7 +3926,7 @@
       <c r="Y70" s="31"/>
       <c r="Z70" s="31"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="31"/>
       <c r="B71" s="31"/>
       <c r="C71" s="31"/>
@@ -3954,7 +3954,7 @@
       <c r="Y71" s="31"/>
       <c r="Z71" s="31"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="31"/>
       <c r="B72" s="31"/>
       <c r="C72" s="31"/>
@@ -3982,7 +3982,7 @@
       <c r="Y72" s="31"/>
       <c r="Z72" s="31"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" s="31"/>
       <c r="B73" s="31"/>
       <c r="C73" s="31"/>
@@ -4010,7 +4010,7 @@
       <c r="Y73" s="31"/>
       <c r="Z73" s="31"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74" s="31"/>
       <c r="B74" s="31"/>
       <c r="C74" s="31"/>
@@ -4038,7 +4038,7 @@
       <c r="Y74" s="31"/>
       <c r="Z74" s="31"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" s="31"/>
       <c r="B75" s="31"/>
       <c r="C75" s="31"/>
@@ -4066,7 +4066,7 @@
       <c r="Y75" s="31"/>
       <c r="Z75" s="31"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="31"/>
       <c r="B76" s="31"/>
       <c r="C76" s="31"/>
@@ -4094,7 +4094,7 @@
       <c r="Y76" s="31"/>
       <c r="Z76" s="31"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" s="31"/>
       <c r="B77" s="31"/>
       <c r="C77" s="31"/>
@@ -4122,7 +4122,7 @@
       <c r="Y77" s="31"/>
       <c r="Z77" s="31"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" s="31"/>
       <c r="B78" s="31"/>
       <c r="C78" s="31"/>
@@ -4150,7 +4150,7 @@
       <c r="Y78" s="31"/>
       <c r="Z78" s="31"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" s="31"/>
       <c r="B79" s="31"/>
       <c r="C79" s="31"/>
@@ -4178,7 +4178,7 @@
       <c r="Y79" s="31"/>
       <c r="Z79" s="31"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" s="31"/>
       <c r="B80" s="31"/>
       <c r="C80" s="31"/>
@@ -4206,7 +4206,7 @@
       <c r="Y80" s="31"/>
       <c r="Z80" s="31"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="31"/>
       <c r="B81" s="31"/>
       <c r="C81" s="31"/>
@@ -4234,7 +4234,7 @@
       <c r="Y81" s="31"/>
       <c r="Z81" s="31"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="31"/>
       <c r="B82" s="31"/>
       <c r="C82" s="31"/>
@@ -4262,7 +4262,7 @@
       <c r="Y82" s="31"/>
       <c r="Z82" s="31"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="31"/>
       <c r="B83" s="31"/>
       <c r="C83" s="31"/>
@@ -4290,7 +4290,7 @@
       <c r="Y83" s="31"/>
       <c r="Z83" s="31"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84" s="31"/>
       <c r="B84" s="31"/>
       <c r="C84" s="31"/>
@@ -4318,7 +4318,7 @@
       <c r="Y84" s="31"/>
       <c r="Z84" s="31"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85" s="31"/>
       <c r="B85" s="31"/>
       <c r="C85" s="31"/>
@@ -4346,7 +4346,7 @@
       <c r="Y85" s="31"/>
       <c r="Z85" s="31"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86" s="31"/>
       <c r="B86" s="31"/>
       <c r="C86" s="31"/>
@@ -4374,7 +4374,7 @@
       <c r="Y86" s="31"/>
       <c r="Z86" s="31"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A87" s="31"/>
       <c r="B87" s="31"/>
       <c r="C87" s="31"/>
@@ -4402,7 +4402,7 @@
       <c r="Y87" s="31"/>
       <c r="Z87" s="31"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A88" s="31"/>
       <c r="B88" s="31"/>
       <c r="C88" s="31"/>
@@ -4430,7 +4430,7 @@
       <c r="Y88" s="31"/>
       <c r="Z88" s="31"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A89" s="31"/>
       <c r="B89" s="31"/>
       <c r="C89" s="31"/>
@@ -4458,7 +4458,7 @@
       <c r="Y89" s="31"/>
       <c r="Z89" s="31"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A90" s="31"/>
       <c r="B90" s="31"/>
       <c r="C90" s="31"/>
@@ -4486,7 +4486,7 @@
       <c r="Y90" s="31"/>
       <c r="Z90" s="31"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A91" s="31"/>
       <c r="B91" s="31"/>
       <c r="C91" s="31"/>
@@ -4514,7 +4514,7 @@
       <c r="Y91" s="31"/>
       <c r="Z91" s="31"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A92" s="31"/>
       <c r="B92" s="31"/>
       <c r="C92" s="31"/>
@@ -4542,7 +4542,7 @@
       <c r="Y92" s="31"/>
       <c r="Z92" s="31"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A93" s="31"/>
       <c r="B93" s="31"/>
       <c r="C93" s="31"/>
@@ -4570,7 +4570,7 @@
       <c r="Y93" s="31"/>
       <c r="Z93" s="31"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A94" s="31"/>
       <c r="B94" s="31"/>
       <c r="C94" s="31"/>
@@ -4598,7 +4598,7 @@
       <c r="Y94" s="31"/>
       <c r="Z94" s="31"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A95" s="31"/>
       <c r="B95" s="31"/>
       <c r="C95" s="31"/>
@@ -4626,7 +4626,7 @@
       <c r="Y95" s="31"/>
       <c r="Z95" s="31"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A96" s="31"/>
       <c r="B96" s="31"/>
       <c r="C96" s="31"/>
@@ -4654,7 +4654,7 @@
       <c r="Y96" s="31"/>
       <c r="Z96" s="31"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A97" s="31"/>
       <c r="B97" s="31"/>
       <c r="C97" s="31"/>
@@ -4682,7 +4682,7 @@
       <c r="Y97" s="31"/>
       <c r="Z97" s="31"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A98" s="31"/>
       <c r="B98" s="31"/>
       <c r="C98" s="31"/>
@@ -4710,7 +4710,7 @@
       <c r="Y98" s="31"/>
       <c r="Z98" s="31"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A99" s="31"/>
       <c r="B99" s="31"/>
       <c r="C99" s="31"/>
@@ -4768,39 +4768,39 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C3" s="20" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -4914,12 +4914,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -5034,7 +5034,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5151,7 +5151,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>56</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>58</v>
       </c>
@@ -5284,7 +5284,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>60</v>
       </c>
@@ -5292,7 +5292,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>62</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>64</v>
       </c>
@@ -5308,7 +5308,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>66</v>
       </c>
@@ -5316,7 +5316,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>68</v>
       </c>
@@ -5324,7 +5324,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>70</v>
       </c>
@@ -5332,7 +5332,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>72</v>
       </c>
@@ -5340,7 +5340,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>74</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>76</v>
       </c>
@@ -5356,7 +5356,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>78</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>80</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>82</v>
       </c>
@@ -5380,7 +5380,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>84</v>
       </c>
@@ -5388,7 +5388,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>86</v>
       </c>
@@ -5396,7 +5396,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>88</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>90</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>92</v>
       </c>
@@ -5420,7 +5420,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>94</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
         <v>96</v>
       </c>
@@ -5436,7 +5436,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>98</v>
       </c>
@@ -5444,7 +5444,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>100</v>
       </c>
@@ -5452,7 +5452,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>102</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>104</v>
       </c>
@@ -5468,7 +5468,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>106</v>
       </c>
@@ -5476,7 +5476,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
         <v>108</v>
       </c>
@@ -5484,7 +5484,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
         <v>110</v>
       </c>
@@ -5532,17 +5532,17 @@
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -5560,7 +5560,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5577,7 +5577,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -5591,7 +5591,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -5623,7 +5623,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A10,"MaxGrowth",B10)</f>
         <v>UC_SUP_MaxGrowth_BIOGAS</v>
@@ -5659,7 +5659,7 @@
         <v>SUP maximum growth rate of BIOGAS</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -5671,7 +5671,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>117</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>187</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" s="16"/>
@@ -5712,17 +5712,17 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -5740,7 +5740,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5757,7 +5757,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -5771,7 +5771,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6:B9" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
@@ -5839,7 +5839,7 @@
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_Wave</v>
@@ -5875,7 +5875,7 @@
         <v>PWR maximum growth rate of Wave</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_Tidal</v>
@@ -5911,7 +5911,7 @@
         <v>PWR maximum growth rate of Tidal</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_H2GT</v>
@@ -5947,7 +5947,7 @@
         <v>PWR maximum growth rate of H2GT</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="str">
         <f t="shared" ref="B10:B11" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_PWR_MaxGrowth_PV</v>
@@ -5983,7 +5983,7 @@
         <v>PWR maximum growth rate of PV</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="str">
         <f t="shared" si="4"/>
         <v>UC_PWR_MaxGrowth_CSP</v>
@@ -6019,7 +6019,7 @@
         <v>PWR maximum growth rate of CSP</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>117</v>
       </c>
@@ -6027,7 +6027,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -6055,7 +6055,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -6083,7 +6083,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -6097,7 +6097,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -6111,7 +6111,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -6125,7 +6125,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>1</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>180</v>
       </c>
@@ -6182,7 +6182,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
@@ -6204,7 +6204,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>181</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D27" s="2"/>
       <c r="E27">
         <v>2027</v>
@@ -6253,26 +6253,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -6290,7 +6290,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -6307,7 +6307,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -6324,7 +6324,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -6365,7 +6365,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A21,"MaxGrowth",B21)</f>
         <v>UC_RSD_MaxGrowth_AmbientHeat</v>
@@ -6405,7 +6405,7 @@
         <v>RSD maximum growth rate of Biodiesel</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
         <f t="shared" ref="B7:B17" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
         <v>UC_RSD_MaxGrowth_Biodiesel</v>
@@ -6445,7 +6445,7 @@
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Biomass</v>
@@ -6485,7 +6485,7 @@
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Coal</v>
@@ -6525,7 +6525,7 @@
         <v>RSD maximum growth rate of Coal</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Peat</v>
@@ -6565,7 +6565,7 @@
         <v>RSD maximum growth rate of Peat</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Electricity</v>
@@ -6605,7 +6605,7 @@
         <v>RSD maximum growth rate of Electricity</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Ethanol</v>
@@ -6645,7 +6645,7 @@
         <v>RSD maximum growth rate of Ethanol</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Gas</v>
@@ -6685,7 +6685,7 @@
         <v>RSD maximum growth rate of Gas</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_DistrictHeat</v>
@@ -6725,7 +6725,7 @@
         <v>RSD maximum growth rate of DistrictHeat</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_LPG</v>
@@ -6765,7 +6765,7 @@
         <v>RSD maximum growth rate of LPG</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Kerosene</v>
@@ -6805,7 +6805,7 @@
         <v>RSD maximum growth rate of Kerosene</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Solar</v>
@@ -6845,7 +6845,7 @@
         <v>RSD maximum growth rate of Solar</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -6858,7 +6858,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>117</v>
       </c>
@@ -6866,7 +6866,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>196</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>196</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>196</v>
       </c>
@@ -6902,7 +6902,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>196</v>
       </c>
@@ -6916,7 +6916,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>196</v>
       </c>
@@ -6930,7 +6930,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>196</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>196</v>
       </c>
@@ -6958,7 +6958,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>196</v>
       </c>
@@ -6972,7 +6972,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>196</v>
       </c>
@@ -6986,7 +6986,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>196</v>
       </c>
@@ -7000,7 +7000,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>196</v>
       </c>
@@ -7014,7 +7014,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>196</v>
       </c>
@@ -7042,19 +7042,19 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -7072,7 +7072,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7089,7 +7089,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7106,7 +7106,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
         <v>UC_SRV_MaxGrowth_Biomass</v>
@@ -7187,7 +7187,7 @@
         <v>SRV maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
         <v>UC_SRV_MaxGrowth_Biogas</v>
@@ -7227,7 +7227,7 @@
         <v>SRV maximum growth rate of Biogas</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
         <v>UC_SRV_MaxGrowth_AmbientHeat</v>
@@ -7267,7 +7267,7 @@
         <v>SRV maximum growth rate of AmbientHeat</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A17,"MaxGrowth",B17)</f>
         <v>UC_SRV_MaxGrowth_DistrictHeat</v>
@@ -7307,7 +7307,7 @@
         <v>SRV maximum growth rate of DistrictHeat</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_SRV_MaxGrowth_Gas</v>
@@ -7347,7 +7347,7 @@
         <v>SRV maximum growth rate of Gas</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -7361,7 +7361,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>117</v>
       </c>
@@ -7369,7 +7369,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>140</v>
       </c>
@@ -7383,7 +7383,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -7397,7 +7397,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -7411,7 +7411,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>140</v>
       </c>
@@ -7425,7 +7425,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -7449,27 +7449,27 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:P53"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3,Regions!E3:AD3)</f>
         <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
@@ -7488,7 +7488,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7506,7 +7506,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7524,7 +7524,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6:B23" si="0">IF(H27="*","*",_xlfn.TEXTJOIN("",TRUE,"UC-",I27,"_MaxGrowth",J27))</f>
         <v>UC-CAR_MaxGrowthBEV</v>
@@ -7589,7 +7589,7 @@
       </c>
       <c r="J6" s="26">
         <f t="shared" ref="J6:J23" si="1">1+$K27</f>
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
@@ -7606,7 +7606,7 @@
         <v>CARs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthPHEV</v>
@@ -7647,7 +7647,7 @@
         <v>CARs maximum growth rate of PHEVs</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthNG-ICE</v>
@@ -7688,7 +7688,7 @@
         <v>CARs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthFCV</v>
@@ -7729,7 +7729,7 @@
         <v>CARs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthBEV</v>
@@ -7770,7 +7770,7 @@
         <v>LGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthPHEV</v>
@@ -7811,7 +7811,7 @@
         <v>LGTs maximum growth rate of PHEVs</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthNG-ICE</v>
@@ -7852,7 +7852,7 @@
         <v>LGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthFCV</v>
@@ -7893,7 +7893,7 @@
         <v>LGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthBEV</v>
@@ -7934,7 +7934,7 @@
         <v>MGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthNG-ICE</v>
@@ -7975,7 +7975,7 @@
         <v>MGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthLNG-ICE</v>
@@ -8016,7 +8016,7 @@
         <v>MGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthHEV</v>
@@ -8057,7 +8057,7 @@
         <v>MGTs maximum growth rate of HEVs</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthFCV</v>
@@ -8098,7 +8098,7 @@
         <v>MGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthBEV</v>
@@ -8139,7 +8139,7 @@
         <v>HGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthNG-ICE</v>
@@ -8180,7 +8180,7 @@
         <v>HGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthLNG-ICE</v>
@@ -8221,7 +8221,7 @@
         <v>HGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthHEV</v>
@@ -8263,7 +8263,7 @@
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B23" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthFCV</v>
@@ -8304,7 +8304,7 @@
         <v>HGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H26" t="s">
         <v>153</v>
       </c>
@@ -8321,7 +8321,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I27" t="s">
         <v>148</v>
       </c>
@@ -8329,13 +8329,13 @@
         <v>130</v>
       </c>
       <c r="K27" s="11">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="L27" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -8352,7 +8352,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8" t="s">
@@ -8377,7 +8377,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="48" t="s">
         <v>27</v>
       </c>
@@ -8407,7 +8407,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="48"/>
       <c r="B31" t="s">
         <v>25</v>
@@ -8435,7 +8435,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="48"/>
       <c r="B32" t="s">
         <v>24</v>
@@ -8463,7 +8463,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A33" s="48"/>
       <c r="B33" t="s">
         <v>23</v>
@@ -8491,7 +8491,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A34" s="48"/>
       <c r="B34" t="s">
         <v>22</v>
@@ -8519,7 +8519,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A35" s="48"/>
       <c r="B35" t="s">
         <v>21</v>
@@ -8547,7 +8547,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>20</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>19</v>
       </c>
@@ -8601,7 +8601,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>18</v>
       </c>
@@ -8628,7 +8628,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5" t="s">
         <v>17</v>
@@ -8656,7 +8656,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -8673,7 +8673,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I41" t="s">
         <v>136</v>
       </c>
@@ -8687,7 +8687,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I42" t="s">
         <v>136</v>
       </c>
@@ -8701,7 +8701,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I43" t="s">
         <v>136</v>
       </c>
@@ -8715,7 +8715,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I44" t="s">
         <v>136</v>
       </c>
@@ -8729,12 +8729,12 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>33</v>
       </c>
@@ -8742,7 +8742,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
         <v>0.5</v>
       </c>
@@ -8750,7 +8750,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C48">
         <v>2018</v>
       </c>
@@ -8794,7 +8794,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>34</v>
       </c>
@@ -8838,7 +8838,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -8903,7 +8903,7 @@
         <v>22797</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -8968,7 +8968,7 @@
         <v>11207</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -9033,7 +9033,7 @@
         <v>328695</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -9115,6 +9115,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9325,15 +9334,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
@@ -9344,6 +9344,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9360,12 +9368,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
RSDHET* and SRVHET* used for Max Growth
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08406A3D-1C92-41FC-87D7-FFC0A1FE940A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D361F6-AB92-41C2-A35C-54BFF47CC31B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -769,9 +769,6 @@
     <t>DistrictHeat</t>
   </si>
   <si>
-    <t>SRVHET</t>
-  </si>
-  <si>
     <t>Gas</t>
   </si>
   <si>
@@ -859,7 +856,10 @@
     <t>BIOGAS1G,BIOGAS2G</t>
   </si>
   <si>
-    <t>RSDHET_1,RSDHET_2,RSDHET_3,RSDHET_X</t>
+    <t>RSDHET*</t>
+  </si>
+  <si>
+    <t>SRVHET*</t>
   </si>
 </sst>
 </file>
@@ -5743,19 +5743,19 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15" s="45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H15" s="46"/>
     </row>
     <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C16" s="47" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E16" s="47" t="s">
         <v>7</v>
@@ -5769,12 +5769,12 @@
         <v>National</v>
       </c>
       <c r="H16" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E17">
         <v>2018</v>
@@ -5787,7 +5787,7 @@
         <v>2222</v>
       </c>
       <c r="H17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -6346,7 +6346,7 @@
   <dimension ref="A2:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6467,7 +6467,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>142</v>
@@ -6507,7 +6507,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="F7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>142</v>
@@ -6547,7 +6547,7 @@
       </c>
       <c r="D8" s="2"/>
       <c r="F8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>142</v>
@@ -6587,7 +6587,7 @@
       </c>
       <c r="D9" s="2"/>
       <c r="F9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>142</v>
@@ -6627,7 +6627,7 @@
       </c>
       <c r="D10" s="2"/>
       <c r="F10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>142</v>
@@ -6667,7 +6667,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="F11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>142</v>
@@ -6707,7 +6707,7 @@
       </c>
       <c r="D12" s="2"/>
       <c r="F12" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>142</v>
@@ -6747,7 +6747,7 @@
       </c>
       <c r="D13" s="2"/>
       <c r="F13" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>142</v>
@@ -6787,7 +6787,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="F14" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>142</v>
@@ -6807,7 +6807,7 @@
       </c>
       <c r="L14" s="16">
         <f t="shared" si="2"/>
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="M14" s="2">
         <v>5</v>
@@ -6827,7 +6827,7 @@
       </c>
       <c r="D15" s="2"/>
       <c r="F15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>142</v>
@@ -6867,7 +6867,7 @@
       </c>
       <c r="D16" s="2"/>
       <c r="F16" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>142</v>
@@ -6907,7 +6907,7 @@
       </c>
       <c r="D17" s="2"/>
       <c r="F17" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>142</v>
@@ -6960,7 +6960,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B21" t="s">
         <v>190</v>
@@ -6968,10 +6968,10 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B22" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C22" s="11">
         <v>0.1</v>
@@ -6982,7 +6982,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B23" t="s">
         <v>137</v>
@@ -6996,10 +6996,10 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C24" s="11">
         <v>0.1</v>
@@ -7010,10 +7010,10 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B25" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C25" s="11">
         <v>0.1</v>
@@ -7024,10 +7024,10 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C26" s="11">
         <v>0.1</v>
@@ -7038,10 +7038,10 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C27" s="11">
         <v>0.1</v>
@@ -7052,10 +7052,10 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C28" s="11">
         <v>0.1</v>
@@ -7066,7 +7066,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B29" t="s">
         <v>191</v>
@@ -7075,15 +7075,15 @@
         <v>0.1</v>
       </c>
       <c r="D29">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B30" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C30" s="11">
         <v>0.1</v>
@@ -7094,10 +7094,10 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B31" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C31" s="11">
         <v>0.1</v>
@@ -7108,10 +7108,10 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C32" s="11">
         <v>0.1</v>
@@ -7122,19 +7122,19 @@
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H35" s="46"/>
     </row>
     <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C36" s="47" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E36" s="47" t="s">
         <v>7</v>
@@ -7148,12 +7148,12 @@
         <v>National</v>
       </c>
       <c r="H36" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E37">
         <v>2018</v>
@@ -7167,7 +7167,7 @@
       </c>
       <c r="H37" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F17)</f>
-        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET_1,RSDHET_2,RSDHET_3,RSDHET_X,RSDLPG,RSDKER,RSDSOL</v>
+        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDSOL</v>
       </c>
     </row>
   </sheetData>
@@ -7181,7 +7181,7 @@
   <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7383,7 +7383,7 @@
       </c>
       <c r="D8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>142</v>
@@ -7423,7 +7423,7 @@
       </c>
       <c r="D9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>142</v>
@@ -7463,7 +7463,7 @@
       </c>
       <c r="D10" s="2"/>
       <c r="F10" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>142</v>
@@ -7576,7 +7576,7 @@
         <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C18" s="11">
         <v>0.08</v>
@@ -7587,19 +7587,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="45" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H22" s="46"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="47" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C23" s="47" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="47" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E23" s="47" t="s">
         <v>7</v>
@@ -7613,12 +7613,12 @@
         <v>National</v>
       </c>
       <c r="H23" s="49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E24">
         <v>2018</v>
@@ -7632,7 +7632,7 @@
       </c>
       <c r="H24" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F10)</f>
-        <v>SRVBIO,SRVBGS,SRVAHT,SRVAHT2,SRVHET,SRVGAS</v>
+        <v>SRVBIO,SRVBGS,SRVAHT,SRVAHT2,SRVHET*,SRVGAS</v>
       </c>
     </row>
   </sheetData>
@@ -9516,18 +9516,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9550,18 +9550,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Modify the LDVs, and freight vehicles stock
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bcf850925e8c42cd/Desktop/times-ireland-model/SuppXLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B1D48E-FB4E-4833-B6D6-DA1E5E1EE1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{42B1D48E-FB4E-4833-B6D6-DA1E5E1EE1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55442538-6B86-411B-B2AA-40E91E3F0557}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-108" yWindow="12852" windowWidth="23256" windowHeight="13176" activeTab="6" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -1237,6 +1237,13 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1249,13 +1256,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1957,20 +1957,20 @@
       <selection activeCell="B20" sqref="B20:D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="6" width="14.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
-    <col min="8" max="10" width="8.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" customWidth="1"/>
+    <col min="1" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="6" width="14.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="8" max="10" width="8.109375" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="12" max="12" width="8.109375" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.44140625" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -1998,7 +1998,7 @@
       <c r="Y1" s="31"/>
       <c r="Z1" s="31"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -2026,7 +2026,7 @@
       <c r="Y2" s="31"/>
       <c r="Z2" s="31"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" s="30"/>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -2054,7 +2054,7 @@
       <c r="Y3" s="31"/>
       <c r="Z3" s="31"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4" s="30"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -2082,7 +2082,7 @@
       <c r="Y4" s="31"/>
       <c r="Z4" s="31"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
@@ -2110,7 +2110,7 @@
       <c r="Y5" s="31"/>
       <c r="Z5" s="31"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -2138,7 +2138,7 @@
       <c r="Y6" s="31"/>
       <c r="Z6" s="31"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7" s="30"/>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
@@ -2166,7 +2166,7 @@
       <c r="Y7" s="31"/>
       <c r="Z7" s="31"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8" s="30"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
@@ -2194,7 +2194,7 @@
       <c r="Y8" s="31"/>
       <c r="Z8" s="31"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
@@ -2222,7 +2222,7 @@
       <c r="Y9" s="31"/>
       <c r="Z9" s="31"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10" s="30"/>
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
@@ -2250,7 +2250,7 @@
       <c r="Y10" s="31"/>
       <c r="Z10" s="31"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11" s="30"/>
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
@@ -2278,7 +2278,7 @@
       <c r="Y11" s="31"/>
       <c r="Z11" s="31"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12" s="30"/>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
@@ -2306,7 +2306,7 @@
       <c r="Y12" s="31"/>
       <c r="Z12" s="31"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
@@ -2334,7 +2334,7 @@
       <c r="Y13" s="31"/>
       <c r="Z13" s="31"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
@@ -2362,7 +2362,7 @@
       <c r="Y14" s="31"/>
       <c r="Z14" s="31"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15" s="30"/>
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
@@ -2390,13 +2390,13 @@
       <c r="Y15" s="31"/>
       <c r="Z15" s="31"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="51" t="s">
         <v>161</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="32"/>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -2420,7 +2420,7 @@
       <c r="Y16" s="31"/>
       <c r="Z16" s="31"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="34"/>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
@@ -2448,7 +2448,7 @@
       <c r="Y17" s="31"/>
       <c r="Z17" s="31"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="34"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
@@ -2476,15 +2476,15 @@
       <c r="Y18" s="31"/>
       <c r="Z18" s="31"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
       <c r="G19" s="39"/>
@@ -2508,15 +2508,15 @@
       <c r="Y19" s="31"/>
       <c r="Z19" s="31"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="50" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
       <c r="G20" s="39"/>
@@ -2540,7 +2540,7 @@
       <c r="Y20" s="31"/>
       <c r="Z20" s="31"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="37" t="s">
         <v>164</v>
       </c>
@@ -2572,7 +2572,7 @@
       <c r="Y21" s="31"/>
       <c r="Z21" s="31"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="37"/>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -2600,15 +2600,15 @@
       <c r="Y22" s="31"/>
       <c r="Z22" s="31"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="50" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
@@ -2632,13 +2632,13 @@
       <c r="Y23" s="31"/>
       <c r="Z23" s="31"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
@@ -2662,7 +2662,7 @@
       <c r="Y24" s="31"/>
       <c r="Z24" s="31"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="37"/>
       <c r="B25" s="40" t="s">
         <v>175</v>
@@ -2692,15 +2692,15 @@
       <c r="Y25" s="31"/>
       <c r="Z25" s="31"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
@@ -2724,7 +2724,7 @@
       <c r="Y26" s="31"/>
       <c r="Z26" s="31"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37"/>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
@@ -2752,7 +2752,7 @@
       <c r="Y27" s="31"/>
       <c r="Z27" s="31"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="37"/>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -2780,7 +2780,7 @@
       <c r="Y28" s="31"/>
       <c r="Z28" s="31"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="37" t="s">
         <v>167</v>
       </c>
@@ -2812,15 +2812,15 @@
       <c r="Y29" s="31"/>
       <c r="Z29" s="31"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="42"/>
       <c r="F30" s="42"/>
       <c r="G30" s="31"/>
@@ -2844,15 +2844,15 @@
       <c r="Y30" s="31"/>
       <c r="Z30" s="31"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
       <c r="E31" s="42"/>
       <c r="F31" s="42"/>
       <c r="G31" s="31"/>
@@ -2876,7 +2876,7 @@
       <c r="Y31" s="31"/>
       <c r="Z31" s="31"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="43"/>
       <c r="B32" s="44" t="s">
         <v>172</v>
@@ -2906,7 +2906,7 @@
       <c r="Y32" s="31"/>
       <c r="Z32" s="31"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
@@ -2934,7 +2934,7 @@
       <c r="Y33" s="31"/>
       <c r="Z33" s="31"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="30"/>
       <c r="B34" s="30"/>
       <c r="C34" s="30"/>
@@ -2962,7 +2962,7 @@
       <c r="Y34" s="31"/>
       <c r="Z34" s="31"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A35" s="30"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -2990,7 +2990,7 @@
       <c r="Y35" s="31"/>
       <c r="Z35" s="31"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A36" s="30"/>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
@@ -3018,7 +3018,7 @@
       <c r="Y36" s="31"/>
       <c r="Z36" s="31"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A37" s="30"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
@@ -3046,7 +3046,7 @@
       <c r="Y37" s="31"/>
       <c r="Z37" s="31"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A38" s="30"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -3074,7 +3074,7 @@
       <c r="Y38" s="31"/>
       <c r="Z38" s="31"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A39" s="30"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -3102,7 +3102,7 @@
       <c r="Y39" s="31"/>
       <c r="Z39" s="31"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A40" s="30"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
@@ -3130,7 +3130,7 @@
       <c r="Y40" s="31"/>
       <c r="Z40" s="31"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -3158,7 +3158,7 @@
       <c r="Y41" s="31"/>
       <c r="Z41" s="31"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A42" s="30"/>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
@@ -3186,7 +3186,7 @@
       <c r="Y42" s="31"/>
       <c r="Z42" s="31"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A43" s="31"/>
       <c r="B43" s="31"/>
       <c r="C43" s="31"/>
@@ -3214,7 +3214,7 @@
       <c r="Y43" s="31"/>
       <c r="Z43" s="31"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A44" s="31"/>
       <c r="B44" s="31"/>
       <c r="C44" s="31"/>
@@ -3242,7 +3242,7 @@
       <c r="Y44" s="31"/>
       <c r="Z44" s="31"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A45" s="31"/>
       <c r="B45" s="31"/>
       <c r="C45" s="31"/>
@@ -3270,7 +3270,7 @@
       <c r="Y45" s="31"/>
       <c r="Z45" s="31"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A46" s="31"/>
       <c r="B46" s="31"/>
       <c r="C46" s="31"/>
@@ -3298,7 +3298,7 @@
       <c r="Y46" s="31"/>
       <c r="Z46" s="31"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="31"/>
       <c r="B47" s="31"/>
       <c r="C47" s="31"/>
@@ -3326,7 +3326,7 @@
       <c r="Y47" s="31"/>
       <c r="Z47" s="31"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="31"/>
       <c r="B48" s="31"/>
       <c r="C48" s="31"/>
@@ -3354,7 +3354,7 @@
       <c r="Y48" s="31"/>
       <c r="Z48" s="31"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A49" s="31"/>
       <c r="B49" s="31"/>
       <c r="C49" s="31"/>
@@ -3382,7 +3382,7 @@
       <c r="Y49" s="31"/>
       <c r="Z49" s="31"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A50" s="31"/>
       <c r="B50" s="31"/>
       <c r="C50" s="31"/>
@@ -3410,7 +3410,7 @@
       <c r="Y50" s="31"/>
       <c r="Z50" s="31"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A51" s="31"/>
       <c r="B51" s="31"/>
       <c r="C51" s="31"/>
@@ -3438,7 +3438,7 @@
       <c r="Y51" s="31"/>
       <c r="Z51" s="31"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A52" s="31"/>
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
@@ -3466,7 +3466,7 @@
       <c r="Y52" s="31"/>
       <c r="Z52" s="31"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A53" s="31"/>
       <c r="B53" s="31"/>
       <c r="C53" s="31"/>
@@ -3494,7 +3494,7 @@
       <c r="Y53" s="31"/>
       <c r="Z53" s="31"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A54" s="31"/>
       <c r="B54" s="31"/>
       <c r="C54" s="31"/>
@@ -3522,7 +3522,7 @@
       <c r="Y54" s="31"/>
       <c r="Z54" s="31"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A55" s="31"/>
       <c r="B55" s="31"/>
       <c r="C55" s="31"/>
@@ -3550,7 +3550,7 @@
       <c r="Y55" s="31"/>
       <c r="Z55" s="31"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A56" s="31"/>
       <c r="B56" s="31"/>
       <c r="C56" s="31"/>
@@ -3578,7 +3578,7 @@
       <c r="Y56" s="31"/>
       <c r="Z56" s="31"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A57" s="31"/>
       <c r="B57" s="31"/>
       <c r="C57" s="31"/>
@@ -3606,7 +3606,7 @@
       <c r="Y57" s="31"/>
       <c r="Z57" s="31"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A58" s="31"/>
       <c r="B58" s="31"/>
       <c r="C58" s="31"/>
@@ -3634,7 +3634,7 @@
       <c r="Y58" s="31"/>
       <c r="Z58" s="31"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A59" s="31"/>
       <c r="B59" s="31"/>
       <c r="C59" s="31"/>
@@ -3662,7 +3662,7 @@
       <c r="Y59" s="31"/>
       <c r="Z59" s="31"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A60" s="31"/>
       <c r="B60" s="31"/>
       <c r="C60" s="31"/>
@@ -3690,7 +3690,7 @@
       <c r="Y60" s="31"/>
       <c r="Z60" s="31"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A61" s="31"/>
       <c r="B61" s="31"/>
       <c r="C61" s="31"/>
@@ -3718,7 +3718,7 @@
       <c r="Y61" s="31"/>
       <c r="Z61" s="31"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A62" s="31"/>
       <c r="B62" s="31"/>
       <c r="C62" s="31"/>
@@ -3746,7 +3746,7 @@
       <c r="Y62" s="31"/>
       <c r="Z62" s="31"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A63" s="31"/>
       <c r="B63" s="31"/>
       <c r="C63" s="31"/>
@@ -3774,7 +3774,7 @@
       <c r="Y63" s="31"/>
       <c r="Z63" s="31"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A64" s="31"/>
       <c r="B64" s="31"/>
       <c r="C64" s="31"/>
@@ -3802,7 +3802,7 @@
       <c r="Y64" s="31"/>
       <c r="Z64" s="31"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="31"/>
       <c r="B65" s="31"/>
       <c r="C65" s="31"/>
@@ -3830,7 +3830,7 @@
       <c r="Y65" s="31"/>
       <c r="Z65" s="31"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="31"/>
       <c r="B66" s="31"/>
       <c r="C66" s="31"/>
@@ -3858,7 +3858,7 @@
       <c r="Y66" s="31"/>
       <c r="Z66" s="31"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="31"/>
       <c r="B67" s="31"/>
       <c r="C67" s="31"/>
@@ -3886,7 +3886,7 @@
       <c r="Y67" s="31"/>
       <c r="Z67" s="31"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" s="31"/>
       <c r="B68" s="31"/>
       <c r="C68" s="31"/>
@@ -3914,7 +3914,7 @@
       <c r="Y68" s="31"/>
       <c r="Z68" s="31"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" s="31"/>
       <c r="B69" s="31"/>
       <c r="C69" s="31"/>
@@ -3942,7 +3942,7 @@
       <c r="Y69" s="31"/>
       <c r="Z69" s="31"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="31"/>
       <c r="B70" s="31"/>
       <c r="C70" s="31"/>
@@ -3970,7 +3970,7 @@
       <c r="Y70" s="31"/>
       <c r="Z70" s="31"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="31"/>
       <c r="B71" s="31"/>
       <c r="C71" s="31"/>
@@ -3998,7 +3998,7 @@
       <c r="Y71" s="31"/>
       <c r="Z71" s="31"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="31"/>
       <c r="B72" s="31"/>
       <c r="C72" s="31"/>
@@ -4026,7 +4026,7 @@
       <c r="Y72" s="31"/>
       <c r="Z72" s="31"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" s="31"/>
       <c r="B73" s="31"/>
       <c r="C73" s="31"/>
@@ -4054,7 +4054,7 @@
       <c r="Y73" s="31"/>
       <c r="Z73" s="31"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74" s="31"/>
       <c r="B74" s="31"/>
       <c r="C74" s="31"/>
@@ -4082,7 +4082,7 @@
       <c r="Y74" s="31"/>
       <c r="Z74" s="31"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" s="31"/>
       <c r="B75" s="31"/>
       <c r="C75" s="31"/>
@@ -4110,7 +4110,7 @@
       <c r="Y75" s="31"/>
       <c r="Z75" s="31"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="31"/>
       <c r="B76" s="31"/>
       <c r="C76" s="31"/>
@@ -4138,7 +4138,7 @@
       <c r="Y76" s="31"/>
       <c r="Z76" s="31"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" s="31"/>
       <c r="B77" s="31"/>
       <c r="C77" s="31"/>
@@ -4166,7 +4166,7 @@
       <c r="Y77" s="31"/>
       <c r="Z77" s="31"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" s="31"/>
       <c r="B78" s="31"/>
       <c r="C78" s="31"/>
@@ -4194,7 +4194,7 @@
       <c r="Y78" s="31"/>
       <c r="Z78" s="31"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" s="31"/>
       <c r="B79" s="31"/>
       <c r="C79" s="31"/>
@@ -4222,7 +4222,7 @@
       <c r="Y79" s="31"/>
       <c r="Z79" s="31"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" s="31"/>
       <c r="B80" s="31"/>
       <c r="C80" s="31"/>
@@ -4250,7 +4250,7 @@
       <c r="Y80" s="31"/>
       <c r="Z80" s="31"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="31"/>
       <c r="B81" s="31"/>
       <c r="C81" s="31"/>
@@ -4278,7 +4278,7 @@
       <c r="Y81" s="31"/>
       <c r="Z81" s="31"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="31"/>
       <c r="B82" s="31"/>
       <c r="C82" s="31"/>
@@ -4306,7 +4306,7 @@
       <c r="Y82" s="31"/>
       <c r="Z82" s="31"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="31"/>
       <c r="B83" s="31"/>
       <c r="C83" s="31"/>
@@ -4334,7 +4334,7 @@
       <c r="Y83" s="31"/>
       <c r="Z83" s="31"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84" s="31"/>
       <c r="B84" s="31"/>
       <c r="C84" s="31"/>
@@ -4362,7 +4362,7 @@
       <c r="Y84" s="31"/>
       <c r="Z84" s="31"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85" s="31"/>
       <c r="B85" s="31"/>
       <c r="C85" s="31"/>
@@ -4390,7 +4390,7 @@
       <c r="Y85" s="31"/>
       <c r="Z85" s="31"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86" s="31"/>
       <c r="B86" s="31"/>
       <c r="C86" s="31"/>
@@ -4418,7 +4418,7 @@
       <c r="Y86" s="31"/>
       <c r="Z86" s="31"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A87" s="31"/>
       <c r="B87" s="31"/>
       <c r="C87" s="31"/>
@@ -4446,7 +4446,7 @@
       <c r="Y87" s="31"/>
       <c r="Z87" s="31"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A88" s="31"/>
       <c r="B88" s="31"/>
       <c r="C88" s="31"/>
@@ -4474,7 +4474,7 @@
       <c r="Y88" s="31"/>
       <c r="Z88" s="31"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A89" s="31"/>
       <c r="B89" s="31"/>
       <c r="C89" s="31"/>
@@ -4502,7 +4502,7 @@
       <c r="Y89" s="31"/>
       <c r="Z89" s="31"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A90" s="31"/>
       <c r="B90" s="31"/>
       <c r="C90" s="31"/>
@@ -4530,7 +4530,7 @@
       <c r="Y90" s="31"/>
       <c r="Z90" s="31"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A91" s="31"/>
       <c r="B91" s="31"/>
       <c r="C91" s="31"/>
@@ -4558,7 +4558,7 @@
       <c r="Y91" s="31"/>
       <c r="Z91" s="31"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A92" s="31"/>
       <c r="B92" s="31"/>
       <c r="C92" s="31"/>
@@ -4586,7 +4586,7 @@
       <c r="Y92" s="31"/>
       <c r="Z92" s="31"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A93" s="31"/>
       <c r="B93" s="31"/>
       <c r="C93" s="31"/>
@@ -4614,7 +4614,7 @@
       <c r="Y93" s="31"/>
       <c r="Z93" s="31"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A94" s="31"/>
       <c r="B94" s="31"/>
       <c r="C94" s="31"/>
@@ -4642,7 +4642,7 @@
       <c r="Y94" s="31"/>
       <c r="Z94" s="31"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A95" s="31"/>
       <c r="B95" s="31"/>
       <c r="C95" s="31"/>
@@ -4670,7 +4670,7 @@
       <c r="Y95" s="31"/>
       <c r="Z95" s="31"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A96" s="31"/>
       <c r="B96" s="31"/>
       <c r="C96" s="31"/>
@@ -4698,7 +4698,7 @@
       <c r="Y96" s="31"/>
       <c r="Z96" s="31"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A97" s="31"/>
       <c r="B97" s="31"/>
       <c r="C97" s="31"/>
@@ -4726,7 +4726,7 @@
       <c r="Y97" s="31"/>
       <c r="Z97" s="31"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A98" s="31"/>
       <c r="B98" s="31"/>
       <c r="C98" s="31"/>
@@ -4754,7 +4754,7 @@
       <c r="Y98" s="31"/>
       <c r="Z98" s="31"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A99" s="31"/>
       <c r="B99" s="31"/>
       <c r="C99" s="31"/>
@@ -4812,39 +4812,39 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5703125" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5546875" customWidth="1"/>
+    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="C3" s="20" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -4958,12 +4958,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5195,7 +5195,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -5312,7 +5312,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>56</v>
       </c>
@@ -5320,7 +5320,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>58</v>
       </c>
@@ -5328,7 +5328,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" s="24" t="s">
         <v>60</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>62</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>64</v>
       </c>
@@ -5352,7 +5352,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>66</v>
       </c>
@@ -5360,7 +5360,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>68</v>
       </c>
@@ -5368,7 +5368,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>70</v>
       </c>
@@ -5376,7 +5376,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>72</v>
       </c>
@@ -5384,7 +5384,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>74</v>
       </c>
@@ -5392,7 +5392,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>76</v>
       </c>
@@ -5400,7 +5400,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>78</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>80</v>
       </c>
@@ -5416,7 +5416,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>82</v>
       </c>
@@ -5424,7 +5424,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>84</v>
       </c>
@@ -5432,7 +5432,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>86</v>
       </c>
@@ -5440,7 +5440,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>88</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>90</v>
       </c>
@@ -5456,7 +5456,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>92</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>94</v>
       </c>
@@ -5472,7 +5472,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
         <v>96</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>98</v>
       </c>
@@ -5488,7 +5488,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>100</v>
       </c>
@@ -5496,7 +5496,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>102</v>
       </c>
@@ -5504,7 +5504,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>104</v>
       </c>
@@ -5512,7 +5512,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>106</v>
       </c>
@@ -5520,7 +5520,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
         <v>108</v>
       </c>
@@ -5528,7 +5528,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="25" t="s">
         <v>110</v>
       </c>
@@ -5576,17 +5576,17 @@
       <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -5604,7 +5604,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5621,7 +5621,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -5635,7 +5635,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A10,"MaxGrowth",B10)</f>
         <v>UC_SUP_MaxGrowth_BIOGAS</v>
@@ -5703,7 +5703,7 @@
         <v>SUP maximum growth rate of BIOGAS</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -5715,7 +5715,7 @@
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>117</v>
       </c>
@@ -5723,7 +5723,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>186</v>
       </c>
@@ -5737,43 +5737,43 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="D11" s="2"/>
       <c r="F11" s="2"/>
       <c r="H11" s="16"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="49" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="H15" s="50"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51" t="s">
+      <c r="H15" s="46"/>
+    </row>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="51" t="s">
+      <c r="D16" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="E16" s="51" t="s">
+      <c r="E16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="52" t="str">
+      <c r="F16" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G16" s="52" t="str">
+      <c r="G16" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H16" s="53" t="s">
+      <c r="H16" s="49" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D17" t="s">
         <v>219</v>
       </c>
@@ -5805,17 +5805,17 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -5833,7 +5833,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5850,7 +5850,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -5864,7 +5864,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -5896,7 +5896,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6:B9" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
@@ -5932,7 +5932,7 @@
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_Wave</v>
@@ -5968,7 +5968,7 @@
         <v>PWR maximum growth rate of Wave</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_Tidal</v>
@@ -6004,7 +6004,7 @@
         <v>PWR maximum growth rate of Tidal</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_H2GT</v>
@@ -6040,7 +6040,7 @@
         <v>PWR maximum growth rate of H2GT</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="str">
         <f t="shared" ref="B10:B11" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_PWR_MaxGrowth_PV</v>
@@ -6076,7 +6076,7 @@
         <v>PWR maximum growth rate of PV</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="str">
         <f t="shared" si="4"/>
         <v>UC_PWR_MaxGrowth_CSP</v>
@@ -6112,7 +6112,7 @@
         <v>PWR maximum growth rate of CSP</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>117</v>
       </c>
@@ -6120,7 +6120,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -6134,7 +6134,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -6148,7 +6148,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -6162,7 +6162,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -6176,7 +6176,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -6218,7 +6218,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B23" s="4" t="s">
         <v>1</v>
       </c>
@@ -6247,7 +6247,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>179</v>
       </c>
@@ -6275,7 +6275,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
@@ -6297,7 +6297,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>180</v>
       </c>
@@ -6325,7 +6325,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D27" s="2"/>
       <c r="E27">
         <v>2027</v>
@@ -6350,22 +6350,22 @@
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.140625" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -6383,7 +6383,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -6400,7 +6400,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -6417,7 +6417,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A21,"MaxGrowth",B21)</f>
         <v>UC_RSD_MaxGrowth_AmbientHeat</v>
@@ -6498,7 +6498,7 @@
         <v>RSD maximum growth rate of Biodiesel</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
         <f t="shared" ref="B7:B17" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
         <v>UC_RSD_MaxGrowth_Biodiesel</v>
@@ -6538,7 +6538,7 @@
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Biomass</v>
@@ -6578,7 +6578,7 @@
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Coal</v>
@@ -6618,7 +6618,7 @@
         <v>RSD maximum growth rate of Coal</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Peat</v>
@@ -6658,7 +6658,7 @@
         <v>RSD maximum growth rate of Peat</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Electricity</v>
@@ -6698,7 +6698,7 @@
         <v>RSD maximum growth rate of Electricity</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Ethanol</v>
@@ -6738,7 +6738,7 @@
         <v>RSD maximum growth rate of Ethanol</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Gas</v>
@@ -6778,7 +6778,7 @@
         <v>RSD maximum growth rate of Gas</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_DistrictHeat</v>
@@ -6818,7 +6818,7 @@
         <v>RSD maximum growth rate of DistrictHeat</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_LPG</v>
@@ -6858,7 +6858,7 @@
         <v>RSD maximum growth rate of LPG</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Kerosene</v>
@@ -6898,7 +6898,7 @@
         <v>RSD maximum growth rate of Kerosene</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Solar</v>
@@ -6938,7 +6938,7 @@
         <v>RSD maximum growth rate of Solar</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -6951,7 +6951,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>117</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>195</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>195</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>195</v>
       </c>
@@ -6995,7 +6995,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -7009,7 +7009,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>195</v>
       </c>
@@ -7023,7 +7023,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>195</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>195</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>195</v>
       </c>
@@ -7065,7 +7065,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>195</v>
       </c>
@@ -7079,7 +7079,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>195</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>195</v>
       </c>
@@ -7107,7 +7107,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>195</v>
       </c>
@@ -7121,38 +7121,38 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="49" t="s">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="H35" s="50"/>
-    </row>
-    <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="51" t="s">
+      <c r="H35" s="46"/>
+    </row>
+    <row r="36" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="C36" s="51" t="s">
+      <c r="C36" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="51" t="s">
+      <c r="D36" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="E36" s="51" t="s">
+      <c r="E36" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="52" t="str">
+      <c r="F36" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G36" s="52" t="str">
+      <c r="G36" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H36" s="53" t="s">
+      <c r="H36" s="49" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D37" t="s">
         <v>219</v>
       </c>
@@ -7181,27 +7181,27 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -7219,7 +7219,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7236,7 +7236,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7253,7 +7253,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -7294,7 +7294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
         <v>UC_SRV_MaxGrowth_Biomass</v>
@@ -7334,7 +7334,7 @@
         <v>SRV maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
         <v>UC_SRV_MaxGrowth_Biogas</v>
@@ -7374,7 +7374,7 @@
         <v>SRV maximum growth rate of Biogas</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
         <v>UC_SRV_MaxGrowth_AmbientHeat</v>
@@ -7414,7 +7414,7 @@
         <v>SRV maximum growth rate of AmbientHeat</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A17,"MaxGrowth",B17)</f>
         <v>UC_SRV_MaxGrowth_DistrictHeat</v>
@@ -7454,7 +7454,7 @@
         <v>SRV maximum growth rate of DistrictHeat</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_SRV_MaxGrowth_Gas</v>
@@ -7494,7 +7494,7 @@
         <v>SRV maximum growth rate of Gas</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -7508,7 +7508,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>117</v>
       </c>
@@ -7516,7 +7516,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -7530,7 +7530,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>139</v>
       </c>
@@ -7558,7 +7558,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>139</v>
       </c>
@@ -7572,7 +7572,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -7586,38 +7586,38 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="49" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B22" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="H22" s="50"/>
-    </row>
-    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="51" t="s">
+      <c r="H22" s="46"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="E23" s="51" t="s">
+      <c r="E23" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="52" t="str">
+      <c r="F23" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G23" s="52" t="str">
+      <c r="G23" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H23" s="53" t="s">
+      <c r="H23" s="49" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
         <v>219</v>
       </c>
@@ -7646,27 +7646,27 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:P53"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="24.42578125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" customWidth="1"/>
-    <col min="14" max="14" width="13.5703125" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5546875" customWidth="1"/>
+    <col min="14" max="14" width="13.5546875" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3,Regions!E3:AD3)</f>
         <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
@@ -7685,7 +7685,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7703,7 +7703,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7721,7 +7721,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -7762,7 +7762,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6:B23" si="0">IF(H27="*","*",_xlfn.TEXTJOIN("",TRUE,"UC-",I27,"_MaxGrowth",J27))</f>
         <v>UC-CAR_MaxGrowthBEV</v>
@@ -7786,24 +7786,24 @@
       </c>
       <c r="J6" s="26">
         <f t="shared" ref="J6:J23" si="1">1+$K27</f>
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="16">
-        <f t="shared" ref="L6:L8" si="2">-$B$53*L27/1000</f>
+        <f>-$B$53*L27/1000</f>
         <v>-18.168149999999997</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f t="shared" ref="N6:N23" si="3">_xlfn.TEXTJOIN(" ", TRUE,I27&amp;"s","maximum growth rate of",J27&amp;"s")</f>
+        <f t="shared" ref="N6:N23" si="2">_xlfn.TEXTJOIN(" ", TRUE,I27&amp;"s","maximum growth rate of",J27&amp;"s")</f>
         <v>CARs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthPHEV</v>
@@ -7833,18 +7833,18 @@
         <v>1</v>
       </c>
       <c r="L7" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L6:L8" si="3">-$B$53*L28/1000</f>
         <v>-18.168149999999997</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>CARs maximum growth rate of PHEVs</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthNG-ICE</v>
@@ -7874,18 +7874,18 @@
         <v>1</v>
       </c>
       <c r="L8" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-18.168149999999997</v>
       </c>
       <c r="M8" s="2">
         <v>5</v>
       </c>
       <c r="N8" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>CARs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B9" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthFCV</v>
@@ -7922,11 +7922,11 @@
         <v>5</v>
       </c>
       <c r="N9" s="18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>CARs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthBEV</v>
@@ -7950,7 +7950,7 @@
       </c>
       <c r="J10" s="26">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="K10" s="2">
         <v>1</v>
@@ -7963,11 +7963,11 @@
         <v>5</v>
       </c>
       <c r="N10" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>LGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthPHEV</v>
@@ -7991,7 +7991,7 @@
       </c>
       <c r="J11" s="26">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
@@ -8004,11 +8004,11 @@
         <v>5</v>
       </c>
       <c r="N11" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>LGTs maximum growth rate of PHEVs</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthNG-ICE</v>
@@ -8032,7 +8032,7 @@
       </c>
       <c r="J12" s="26">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
@@ -8045,11 +8045,11 @@
         <v>5</v>
       </c>
       <c r="N12" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>LGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B13" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthFCV</v>
@@ -8073,7 +8073,7 @@
       </c>
       <c r="J13" s="27">
         <f t="shared" si="1"/>
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="K13" s="18">
         <v>1</v>
@@ -8086,11 +8086,11 @@
         <v>5</v>
       </c>
       <c r="N13" s="18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>LGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthBEV</v>
@@ -8127,11 +8127,11 @@
         <v>5</v>
       </c>
       <c r="N14" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>MGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthNG-ICE</v>
@@ -8168,11 +8168,11 @@
         <v>5</v>
       </c>
       <c r="N15" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>MGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthLNG-ICE</v>
@@ -8209,11 +8209,11 @@
         <v>5</v>
       </c>
       <c r="N16" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>MGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthHEV</v>
@@ -8250,11 +8250,11 @@
         <v>5</v>
       </c>
       <c r="N17" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>MGTs maximum growth rate of HEVs</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B18" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthFCV</v>
@@ -8291,11 +8291,11 @@
         <v>5</v>
       </c>
       <c r="N18" s="18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>MGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthBEV</v>
@@ -8332,11 +8332,11 @@
         <v>5</v>
       </c>
       <c r="N19" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>HGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthNG-ICE</v>
@@ -8373,11 +8373,11 @@
         <v>5</v>
       </c>
       <c r="N20" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>HGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthLNG-ICE</v>
@@ -8414,11 +8414,11 @@
         <v>5</v>
       </c>
       <c r="N21" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>HGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthHEV</v>
@@ -8455,12 +8455,12 @@
         <v>5</v>
       </c>
       <c r="N22" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>HGTs maximum growth rate of HEVs</v>
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B23" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthFCV</v>
@@ -8497,11 +8497,11 @@
         <v>5</v>
       </c>
       <c r="N23" s="18" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>HGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="H26" t="s">
         <v>152</v>
       </c>
@@ -8518,7 +8518,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="I27" t="s">
         <v>147</v>
       </c>
@@ -8526,13 +8526,13 @@
         <v>129</v>
       </c>
       <c r="K27" s="11">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="L27" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -8549,7 +8549,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8" t="s">
@@ -8574,8 +8574,8 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A30" s="53" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
@@ -8604,8 +8604,8 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A31" s="53"/>
       <c r="B31" t="s">
         <v>25</v>
       </c>
@@ -8626,14 +8626,14 @@
         <v>129</v>
       </c>
       <c r="K31" s="11">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="L31" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A32" s="53"/>
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -8654,14 +8654,14 @@
         <v>130</v>
       </c>
       <c r="K32" s="11">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="L32" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A33" s="53"/>
       <c r="B33" t="s">
         <v>23</v>
       </c>
@@ -8682,14 +8682,14 @@
         <v>148</v>
       </c>
       <c r="K33" s="11">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="L33" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A34" s="53"/>
       <c r="B34" t="s">
         <v>22</v>
       </c>
@@ -8710,14 +8710,14 @@
         <v>131</v>
       </c>
       <c r="K34" s="11">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="L34" s="11">
         <v>0.15</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A35" s="53"/>
       <c r="B35" t="s">
         <v>21</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>20</v>
       </c>
@@ -8771,7 +8771,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>19</v>
       </c>
@@ -8798,7 +8798,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>18</v>
       </c>
@@ -8825,7 +8825,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="5" t="s">
         <v>17</v>
@@ -8853,7 +8853,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -8870,7 +8870,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I41" t="s">
         <v>135</v>
       </c>
@@ -8884,7 +8884,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I42" t="s">
         <v>135</v>
       </c>
@@ -8898,7 +8898,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I43" t="s">
         <v>135</v>
       </c>
@@ -8912,7 +8912,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I44" t="s">
         <v>135</v>
       </c>
@@ -8926,12 +8926,12 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>33</v>
       </c>
@@ -8939,7 +8939,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B47" s="11">
         <v>0.5</v>
       </c>
@@ -8947,7 +8947,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="C48">
         <v>2018</v>
       </c>
@@ -8991,7 +8991,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>34</v>
       </c>
@@ -9035,7 +9035,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -9100,7 +9100,7 @@
         <v>22797</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -9165,7 +9165,7 @@
         <v>11207</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -9230,7 +9230,7 @@
         <v>328695</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -9312,6 +9312,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9522,15 +9531,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
@@ -9541,6 +9541,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9557,12 +9565,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add growth constraints for domestic production of biodiesel and ethanol
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B1D48E-FB4E-4833-B6D6-DA1E5E1EE1B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EF8370-78CC-482E-BC2C-10A6DB03695A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="229">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -861,6 +861,24 @@
   </si>
   <si>
     <t>BIOGAS1G,BIOGAS2G</t>
+  </si>
+  <si>
+    <t>BIODST1G,BIODST2G</t>
+  </si>
+  <si>
+    <t>BIOETH1G,BIOETH2G</t>
+  </si>
+  <si>
+    <t>BIODST</t>
+  </si>
+  <si>
+    <t>BIOETH</t>
+  </si>
+  <si>
+    <t>SBIORDST*</t>
+  </si>
+  <si>
+    <t>SBIORETH*</t>
   </si>
 </sst>
 </file>
@@ -1237,6 +1255,13 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1249,13 +1274,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2391,12 +2409,12 @@
       <c r="Z15" s="31"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="46" t="s">
+      <c r="A16" s="51" t="s">
         <v>161</v>
       </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="32"/>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -2480,11 +2498,11 @@
       <c r="A19" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="50" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
       <c r="G19" s="39"/>
@@ -2512,11 +2530,11 @@
       <c r="A20" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="50" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
       <c r="G20" s="39"/>
@@ -2604,11 +2622,11 @@
       <c r="A23" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="B23" s="45" t="s">
+      <c r="B23" s="50" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
@@ -2634,11 +2652,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="37"/>
-      <c r="B24" s="45" t="s">
+      <c r="B24" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
@@ -2696,11 +2714,11 @@
       <c r="A26" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="50" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
@@ -2816,11 +2834,11 @@
       <c r="A30" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="47" t="s">
+      <c r="B30" s="52" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
       <c r="E30" s="42"/>
       <c r="F30" s="42"/>
       <c r="G30" s="31"/>
@@ -2848,11 +2866,11 @@
       <c r="A31" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
       <c r="E31" s="42"/>
       <c r="F31" s="42"/>
       <c r="G31" s="31"/>
@@ -5570,10 +5588,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89417C8F-9D07-4311-9372-0B0C534E50C4}">
-  <dimension ref="A2:N17"/>
+  <dimension ref="A2:N21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5669,7 +5687,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A10,"MaxGrowth",B10)</f>
+        <f t="shared" ref="B6" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A12,"MaxGrowth",B12)</f>
         <v>UC_SUP_MaxGrowth_BIOGAS</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5685,110 +5703,243 @@
         <v>15</v>
       </c>
       <c r="G6" s="26">
-        <f t="shared" ref="G6" si="1">1+$C10</f>
+        <f t="shared" ref="G6:G8" si="1">1+$C12</f>
         <v>1.4</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
       </c>
       <c r="I6" s="16">
-        <f t="shared" ref="I6" si="2">-D10</f>
+        <f t="shared" ref="I6" si="2">-D12</f>
         <v>-0.2</v>
       </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
       <c r="K6" s="2" t="str">
-        <f t="shared" ref="K6" si="3">_xlfn.TEXTJOIN(" ",TRUE,A10, "maximum growth rate of",B10)</f>
+        <f t="shared" ref="K6" si="3">_xlfn.TEXTJOIN(" ",TRUE,A12, "maximum growth rate of",B12)</f>
         <v>SUP maximum growth rate of BIOGAS</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="B7" s="2" t="str">
+        <f t="shared" ref="B7:B8" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A13,"MaxGrowth",B13)</f>
+        <v>UC_SUP_MaxGrowth_BIODST</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="26">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="16">
+        <f t="shared" ref="I7:I8" si="5">-D13</f>
+        <v>-1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>5</v>
+      </c>
+      <c r="K7" s="2" t="str">
+        <f t="shared" ref="K7:K8" si="6">_xlfn.TEXTJOIN(" ",TRUE,A13, "maximum growth rate of",B13)</f>
+        <v>SUP maximum growth rate of BIODST</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="str">
+        <f t="shared" si="4"/>
+        <v>UC_SUP_MaxGrowth_BIOETH</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2018</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="26">
+        <f t="shared" si="1"/>
+        <v>1.4</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="16">
+        <f t="shared" si="5"/>
+        <v>-1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>5</v>
+      </c>
+      <c r="K8" s="2" t="str">
+        <f t="shared" si="6"/>
+        <v>SUP maximum growth rate of BIOETH</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
         <v>117</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D11" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>186</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>187</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C12" s="11">
         <v>0.4</v>
       </c>
-      <c r="D10">
+      <c r="D12">
         <v>0.2</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="H11" s="16"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="49" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>186</v>
+      </c>
+      <c r="B13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" t="s">
+        <v>226</v>
+      </c>
+      <c r="C14" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="H15" s="50"/>
-    </row>
-    <row r="16" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="51" t="s">
+      <c r="H17" s="46"/>
+    </row>
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="C16" s="51" t="s">
+      <c r="C18" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="51" t="s">
+      <c r="D18" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="E16" s="51" t="s">
+      <c r="E18" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="52" t="str">
+      <c r="F18" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G16" s="52" t="str">
+      <c r="G18" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H16" s="53" t="s">
+      <c r="H18" s="49" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="D17" t="s">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
         <v>219</v>
       </c>
-      <c r="E17">
+      <c r="E19">
         <v>2018</v>
       </c>
-      <c r="F17">
+      <c r="F19">
         <v>2222</v>
       </c>
-      <c r="G17">
-        <f>F17</f>
+      <c r="G19">
+        <f>F19</f>
         <v>2222</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H19" t="s">
         <v>222</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E20">
+        <v>2018</v>
+      </c>
+      <c r="F20">
+        <v>2222</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ref="G20:G21" si="7">F20</f>
+        <v>2222</v>
+      </c>
+      <c r="H20" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>219</v>
+      </c>
+      <c r="E21">
+        <v>2018</v>
+      </c>
+      <c r="F21">
+        <v>2222</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="7"/>
+        <v>2222</v>
+      </c>
+      <c r="H21" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -7122,33 +7273,33 @@
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="H35" s="50"/>
+      <c r="H35" s="46"/>
     </row>
     <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="51" t="s">
+      <c r="B36" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="C36" s="51" t="s">
+      <c r="C36" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="51" t="s">
+      <c r="D36" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="E36" s="51" t="s">
+      <c r="E36" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="52" t="str">
+      <c r="F36" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G36" s="52" t="str">
+      <c r="G36" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H36" s="53" t="s">
+      <c r="H36" s="49" t="s">
         <v>218</v>
       </c>
     </row>
@@ -7181,7 +7332,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
@@ -7587,33 +7738,33 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="H22" s="50"/>
+      <c r="H22" s="46"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="47" t="s">
         <v>216</v>
       </c>
-      <c r="C23" s="51" t="s">
+      <c r="C23" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="51" t="s">
+      <c r="D23" s="47" t="s">
         <v>217</v>
       </c>
-      <c r="E23" s="51" t="s">
+      <c r="E23" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="52" t="str">
+      <c r="F23" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G23" s="52" t="str">
+      <c r="G23" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H23" s="53" t="s">
+      <c r="H23" s="49" t="s">
         <v>218</v>
       </c>
     </row>
@@ -8575,7 +8726,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="48" t="s">
+      <c r="A30" s="53" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
@@ -8605,7 +8756,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
+      <c r="A31" s="53"/>
       <c r="B31" t="s">
         <v>25</v>
       </c>
@@ -8633,7 +8784,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
+      <c r="A32" s="53"/>
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -8661,7 +8812,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="48"/>
+      <c r="A33" s="53"/>
       <c r="B33" t="s">
         <v>23</v>
       </c>
@@ -8689,7 +8840,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="48"/>
+      <c r="A34" s="53"/>
       <c r="B34" t="s">
         <v>22</v>
       </c>
@@ -8717,7 +8868,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="48"/>
+      <c r="A35" s="53"/>
       <c r="B35" t="s">
         <v>21</v>
       </c>
@@ -9312,6 +9463,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9522,15 +9682,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
@@ -9541,6 +9692,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9557,12 +9716,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add a growth rate constraint for retrofits
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26EF8370-78CC-482E-BC2C-10A6DB03695A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCC8742-F8A7-4793-8502-A6CEC3456416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -18,14 +18,16 @@
     <sheet name="SUP" sheetId="7" r:id="rId3"/>
     <sheet name="PWR" sheetId="4" r:id="rId4"/>
     <sheet name="RSD" sheetId="8" r:id="rId5"/>
-    <sheet name="SRV" sheetId="5" r:id="rId6"/>
-    <sheet name="TRA" sheetId="1" r:id="rId7"/>
+    <sheet name="RSD-Retrofits" sheetId="9" r:id="rId6"/>
+    <sheet name="SRV" sheetId="5" r:id="rId7"/>
+    <sheet name="TRA" sheetId="1" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="3" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="4" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="5" hidden="1">#REF!</definedName>
+    <definedName name="__123Graph_AEUMILKPN" localSheetId="6" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
     <definedName name="_AtRisk_SimSetting_AutomaticallyGenerateReports" hidden="1">FALSE</definedName>
@@ -50,36 +52,42 @@
     <definedName name="_Regression_Y" localSheetId="3" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" localSheetId="4" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" localSheetId="5" hidden="1">#REF!</definedName>
+    <definedName name="_Regression_Y" localSheetId="6" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" localSheetId="2" hidden="1">#REF!</definedName>
     <definedName name="_Regression_Y" hidden="1">#REF!</definedName>
     <definedName name="aa" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="aa" localSheetId="6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="aa" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec" localSheetId="6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec2" localSheetId="6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elec3" localSheetId="6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elec3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="elecc" localSheetId="6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="elecc" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="IQ_FWD_CY" hidden="1">10001</definedName>
@@ -122,12 +130,14 @@
     <definedName name="table6" localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="table6" localSheetId="6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="table6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="0" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="3" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="4" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="5" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
+    <definedName name="wrn.Electricity._.Questionnaire." localSheetId="6" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." localSheetId="2" hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
     <definedName name="wrn.Electricity._.Questionnaire." hidden="1">{#N/A,#N/A,FALSE,"Notes";#N/A,#N/A,FALSE,"Table1";#N/A,#N/A,FALSE,"Table2";#N/A,#N/A,FALSE,"Table3";#N/A,#N/A,FALSE,"Table4";#N/A,#N/A,FALSE,"Table5";#N/A,#N/A,FALSE,"Table6a";#N/A,#N/A,FALSE,"Table6b";#N/A,#N/A,FALSE,"Table6c";#N/A,#N/A,FALSE,"Table7a";#N/A,#N/A,FALSE,"Table7b";#N/A,#N/A,FALSE,"Table8a";#N/A,#N/A,FALSE,"Table8b";#N/A,#N/A,FALSE,"Table8c";#N/A,#N/A,FALSE,"Tables 9a-c";#N/A,#N/A,FALSE,"Tables 9d-f";#N/A,#N/A,FALSE,"Table 9g";#N/A,#N/A,FALSE,"Table 9h-j";#N/A,#N/A,FALSE,"Remarks"}</definedName>
   </definedNames>
@@ -172,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="236">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -879,6 +889,27 @@
   </si>
   <si>
     <t>SBIORETH*</t>
+  </si>
+  <si>
+    <t>NCAP, GROWTH</t>
+  </si>
+  <si>
+    <t>Starting value (kUnits)</t>
+  </si>
+  <si>
+    <t>R-RTFT*</t>
+  </si>
+  <si>
+    <t>Retrofits</t>
+  </si>
+  <si>
+    <t>UC_RSD_MaxNCap_Retrofits</t>
+  </si>
+  <si>
+    <t>RSD maximum new retrofits</t>
+  </si>
+  <si>
+    <t>UC_NCAP~RHS</t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1203,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1274,6 +1305,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -4826,8 +4858,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A3:AD37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5590,7 +5622,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89417C8F-9D07-4311-9372-0B0C534E50C4}">
   <dimension ref="A2:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
@@ -5953,7 +5985,7 @@
   <dimension ref="A2:N27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6497,8 +6529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6631,22 +6663,22 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f>1+C22</f>
+        <f>1+C21</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="16">
-        <f>-D22</f>
+        <f>-D21</f>
         <v>-0.5</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
-        <v>RSD maximum growth rate of Biodiesel</v>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A21, "maximum growth rate of",B21)</f>
+        <v>RSD maximum growth rate of AmbientHeat</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
@@ -6671,22 +6703,22 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f>1+C23</f>
+        <f t="shared" ref="J7:J8" si="1">1+C22</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="16">
-        <f>-D23</f>
+        <f t="shared" ref="L7:L8" si="2">-D22</f>
         <v>-0.5</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
-        <v>RSD maximum growth rate of Biomass</v>
+        <f t="shared" ref="N7:N8" si="3">_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
+        <v>RSD maximum growth rate of Biodiesel</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
@@ -6711,21 +6743,21 @@
         <v>15</v>
       </c>
       <c r="J8" s="29">
-        <f>1+C23</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
       </c>
       <c r="L8" s="16">
-        <f>-D23</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M8" s="2">
         <v>5</v>
       </c>
       <c r="N8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
+        <f t="shared" si="3"/>
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
@@ -6871,21 +6903,21 @@
         <v>15</v>
       </c>
       <c r="J12" s="29">
-        <f t="shared" ref="J12:J17" si="1">1+C27</f>
+        <f t="shared" ref="J12:J17" si="4">1+C27</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
       </c>
       <c r="L12" s="16">
-        <f t="shared" ref="L12:L17" si="2">-D27</f>
+        <f t="shared" ref="L12:L17" si="5">-D27</f>
         <v>-0.5</v>
       </c>
       <c r="M12" s="2">
         <v>5</v>
       </c>
       <c r="N12" s="2" t="str">
-        <f t="shared" ref="N12:N17" si="3">_xlfn.TEXTJOIN(" ",TRUE,A27, "maximum growth rate of",B27)</f>
+        <f t="shared" ref="N12:N17" si="6">_xlfn.TEXTJOIN(" ",TRUE,A27, "maximum growth rate of",B27)</f>
         <v>RSD maximum growth rate of Ethanol</v>
       </c>
     </row>
@@ -6911,21 +6943,21 @@
         <v>15</v>
       </c>
       <c r="J13" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
       </c>
       <c r="L13" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.5</v>
       </c>
       <c r="M13" s="2">
         <v>5</v>
       </c>
       <c r="N13" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>RSD maximum growth rate of Gas</v>
       </c>
     </row>
@@ -6951,21 +6983,21 @@
         <v>15</v>
       </c>
       <c r="J14" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K14" s="2">
         <v>1</v>
       </c>
       <c r="L14" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.5</v>
       </c>
       <c r="M14" s="2">
         <v>5</v>
       </c>
       <c r="N14" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>RSD maximum growth rate of DistrictHeat</v>
       </c>
     </row>
@@ -6991,21 +7023,21 @@
         <v>15</v>
       </c>
       <c r="J15" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K15" s="2">
         <v>1</v>
       </c>
       <c r="L15" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.5</v>
       </c>
       <c r="M15" s="2">
         <v>5</v>
       </c>
       <c r="N15" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>RSD maximum growth rate of LPG</v>
       </c>
     </row>
@@ -7031,21 +7063,21 @@
         <v>15</v>
       </c>
       <c r="J16" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K16" s="2">
         <v>1</v>
       </c>
       <c r="L16" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.5</v>
       </c>
       <c r="M16" s="2">
         <v>5</v>
       </c>
       <c r="N16" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>RSD maximum growth rate of Kerosene</v>
       </c>
     </row>
@@ -7071,21 +7103,21 @@
         <v>15</v>
       </c>
       <c r="J17" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K17" s="2">
         <v>1</v>
       </c>
       <c r="L17" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-0.5</v>
       </c>
       <c r="M17" s="2">
         <v>5</v>
       </c>
       <c r="N17" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>RSD maximum growth rate of Solar</v>
       </c>
     </row>
@@ -7117,6 +7149,12 @@
       <c r="B21" t="s">
         <v>190</v>
       </c>
+      <c r="C21" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -7328,12 +7366,223 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E6F9F7-2BA7-423B-9539-782F2BC14985}">
+  <dimension ref="A2:N10"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="str">
+        <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
+        <v>~UC_Sets: R_E: IE,National</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A10,"MaxGrowth",B10)</f>
+        <v>UC_RSD_MaxGrowth_Retrofits</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2019</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="29">
+        <f>1+C10</f>
+        <v>1.5</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1</v>
+      </c>
+      <c r="L6" s="16">
+        <f>-D10</f>
+        <v>-20</v>
+      </c>
+      <c r="M6" s="2">
+        <v>5</v>
+      </c>
+      <c r="N6" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A10, "maximum growth rate of",LOWER(B10))</f>
+        <v>RSD maximum growth rate of retrofits</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H7">
+        <v>2019</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J7" s="54">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="16">
+        <v>60</v>
+      </c>
+      <c r="M7" s="2">
+        <v>5</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7792,7 +8041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A41B7AF2-8905-43A5-8387-D99F068F4BCD}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:P53"/>
@@ -9463,15 +9712,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9682,6 +9922,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
@@ -9692,14 +9941,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9716,4 +9957,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Results dummies in cooling and max growth rate not working.
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{196E8F95-931F-49E5-8D00-32026047D841}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE7B3AF-6633-47E9-8257-F656B17CF794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -9305,21 +9305,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9530,24 +9515,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9564,4 +9547,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update latest changes  - Incomplete SubRES_PWR_DH.xlsx and Scen_B_SYS_MaxGrowthRates.xlsx
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE7B3AF-6633-47E9-8257-F656B17CF794}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6235F00-3AC1-47D2-8859-AFA2B0251D87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -6345,7 +6345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -7180,8 +7180,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7435,8 +7435,7 @@
         <v>15</v>
       </c>
       <c r="J9" s="29">
-        <f>1+C17</f>
-        <v>1.05</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
@@ -9305,6 +9304,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9515,22 +9529,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9547,21 +9563,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Set max ker degrowth
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6235F00-3AC1-47D2-8859-AFA2B0251D87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEFC553-3F2E-4564-BF96-EBE2B59CCC2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="223">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -6343,10 +6343,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
-  <dimension ref="A2:N37"/>
+  <dimension ref="A2:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6459,7 +6459,7 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A21,"MaxGrowth",B21)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
         <v>UC_RSD_MaxGrowth_AmbientHeat</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -6479,27 +6479,27 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f>1+C22</f>
+        <f>1+C23</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="16">
-        <f>-D22</f>
+        <f>-D23</f>
         <v>-0.5</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
         <v>RSD maximum growth rate of Biodiesel</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f t="shared" ref="B7:B17" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
         <v>UC_RSD_MaxGrowth_Biodiesel</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -6519,27 +6519,27 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f>1+C23</f>
+        <f>1+C24</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="16">
-        <f>-D23</f>
+        <f>-D24</f>
         <v>-0.5</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A24,"MaxGrowth",B24)</f>
         <v>UC_RSD_MaxGrowth_Biomass</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -6559,27 +6559,27 @@
         <v>15</v>
       </c>
       <c r="J8" s="29">
-        <f>1+C23</f>
+        <f>1+C24</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
       </c>
       <c r="L8" s="16">
-        <f>-D23</f>
+        <f>-D24</f>
         <v>-0.5</v>
       </c>
       <c r="M8" s="2">
         <v>5</v>
       </c>
       <c r="N8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A25,"MaxGrowth",B25)</f>
         <v>UC_RSD_MaxGrowth_Coal</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -6599,27 +6599,27 @@
         <v>15</v>
       </c>
       <c r="J9" s="29">
-        <f>1+C24</f>
+        <f>1+C25</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
       </c>
       <c r="L9" s="16">
-        <f>-D24</f>
+        <f>-D25</f>
         <v>-0.5</v>
       </c>
       <c r="M9" s="2">
         <v>5</v>
       </c>
       <c r="N9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A25, "maximum growth rate of",B25)</f>
         <v>RSD maximum growth rate of Coal</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A26,"MaxGrowth",B26)</f>
         <v>UC_RSD_MaxGrowth_Peat</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6639,27 +6639,27 @@
         <v>15</v>
       </c>
       <c r="J10" s="29">
-        <f>1+C25</f>
+        <f>1+C26</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K10" s="2">
         <v>1</v>
       </c>
       <c r="L10" s="16">
-        <f>-D25</f>
+        <f>-D26</f>
         <v>-0.5</v>
       </c>
       <c r="M10" s="2">
         <v>5</v>
       </c>
       <c r="N10" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A25, "maximum growth rate of",B25)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
         <v>RSD maximum growth rate of Peat</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A27,"MaxGrowth",B27)</f>
         <v>UC_RSD_MaxGrowth_Electricity</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6679,27 +6679,27 @@
         <v>15</v>
       </c>
       <c r="J11" s="29">
-        <f>1+C26</f>
+        <f>1+C27</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
       </c>
       <c r="L11" s="16">
-        <f>-D26</f>
+        <f>-D27</f>
         <v>-0.5</v>
       </c>
       <c r="M11" s="2">
         <v>5</v>
       </c>
       <c r="N11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A27, "maximum growth rate of",B27)</f>
         <v>RSD maximum growth rate of Electricity</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A28,"MaxGrowth",B28)</f>
         <v>UC_RSD_MaxGrowth_Ethanol</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6719,27 +6719,27 @@
         <v>15</v>
       </c>
       <c r="J12" s="29">
-        <f t="shared" ref="J12:J17" si="1">1+C27</f>
+        <f>1+C28</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
       </c>
       <c r="L12" s="16">
-        <f t="shared" ref="L12:L17" si="2">-D27</f>
+        <f>-D28</f>
         <v>-0.5</v>
       </c>
       <c r="M12" s="2">
         <v>5</v>
       </c>
       <c r="N12" s="2" t="str">
-        <f t="shared" ref="N12:N17" si="3">_xlfn.TEXTJOIN(" ",TRUE,A27, "maximum growth rate of",B27)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A28, "maximum growth rate of",B28)</f>
         <v>RSD maximum growth rate of Ethanol</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A29,"MaxGrowth",B29)</f>
         <v>UC_RSD_MaxGrowth_Gas</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -6759,27 +6759,27 @@
         <v>15</v>
       </c>
       <c r="J13" s="29">
-        <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <f>1+C29</f>
+        <v>1.05</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
       </c>
       <c r="L13" s="16">
-        <f t="shared" si="2"/>
+        <f>-D29</f>
         <v>-0.5</v>
       </c>
       <c r="M13" s="2">
         <v>5</v>
       </c>
       <c r="N13" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A29, "maximum growth rate of",B29)</f>
         <v>RSD maximum growth rate of Gas</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A30,"MaxGrowth",B30)</f>
         <v>UC_RSD_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -6799,27 +6799,27 @@
         <v>15</v>
       </c>
       <c r="J14" s="29">
-        <f t="shared" si="1"/>
+        <f>1+C30</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K14" s="2">
         <v>1</v>
       </c>
       <c r="L14" s="16">
-        <f t="shared" si="2"/>
+        <f>-D30</f>
         <v>-0.3</v>
       </c>
       <c r="M14" s="2">
         <v>5</v>
       </c>
       <c r="N14" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A30, "maximum growth rate of",B30)</f>
         <v>RSD maximum growth rate of DistrictHeat</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A31,"MaxGrowth",B31)</f>
         <v>UC_RSD_MaxGrowth_LPG</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -6839,27 +6839,27 @@
         <v>15</v>
       </c>
       <c r="J15" s="29">
-        <f t="shared" si="1"/>
+        <f>1+C31</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K15" s="2">
         <v>1</v>
       </c>
       <c r="L15" s="16">
-        <f t="shared" si="2"/>
+        <f>-D31</f>
         <v>-0.5</v>
       </c>
       <c r="M15" s="2">
         <v>5</v>
       </c>
       <c r="N15" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A31, "maximum growth rate of",B31)</f>
         <v>RSD maximum growth rate of LPG</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A32,"MaxGrowth",B32)</f>
         <v>UC_RSD_MaxGrowth_Kerosene</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -6879,35 +6879,35 @@
         <v>15</v>
       </c>
       <c r="J16" s="29">
-        <f t="shared" si="1"/>
+        <f>1+C32</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K16" s="2">
         <v>1</v>
       </c>
       <c r="L16" s="16">
-        <f t="shared" si="2"/>
+        <f>-D32</f>
         <v>-0.5</v>
       </c>
       <c r="M16" s="2">
         <v>5</v>
       </c>
       <c r="N16" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A32, "maximum growth rate of",B32)</f>
         <v>RSD maximum growth rate of Kerosene</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_RSD_MaxGrowth_Solar</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A32,"MaxDegrowth",B32)</f>
+        <v>UC_RSD_MaxDegrowth_Kerosene</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D17" s="2"/>
       <c r="F17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>142</v>
@@ -6919,51 +6919,83 @@
         <v>15</v>
       </c>
       <c r="J17" s="29">
-        <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <f>1-C33</f>
+        <v>0.9</v>
       </c>
       <c r="K17" s="2">
         <v>1</v>
       </c>
       <c r="L17" s="16">
-        <f t="shared" si="2"/>
+        <f>-D33</f>
         <v>-0.5</v>
       </c>
       <c r="M17" s="2">
         <v>5</v>
       </c>
       <c r="N17" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A32, "maximum degrowth rate of",B32)</f>
+        <v>RSD maximum degrowth rate of Kerosene</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="str">
+        <f t="shared" ref="B18" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A33,"MaxGrowth",B33)</f>
+        <v>UC_RSD_MaxGrowth_Solar</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="F18" t="s">
+        <v>212</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H18" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="29">
+        <f t="shared" ref="J18" si="1">1+C33</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+      <c r="L18" s="16">
+        <f t="shared" ref="L18" si="2">-D33</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M18" s="2">
+        <v>5</v>
+      </c>
+      <c r="N18" s="2" t="str">
+        <f t="shared" ref="N18" si="3">_xlfn.TEXTJOIN(" ",TRUE,A33, "maximum growth rate of",B33)</f>
         <v>RSD maximum growth rate of Solar</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="29"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="16"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="16"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
         <v>117</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>194</v>
-      </c>
-      <c r="B21" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -6971,13 +7003,7 @@
         <v>194</v>
       </c>
       <c r="B22" t="s">
-        <v>196</v>
-      </c>
-      <c r="C22" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="D22">
-        <v>0.5</v>
+        <v>190</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -6985,7 +7011,7 @@
         <v>194</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="C23" s="11">
         <v>0.1</v>
@@ -6999,7 +7025,7 @@
         <v>194</v>
       </c>
       <c r="B24" t="s">
-        <v>197</v>
+        <v>137</v>
       </c>
       <c r="C24" s="11">
         <v>0.1</v>
@@ -7013,7 +7039,7 @@
         <v>194</v>
       </c>
       <c r="B25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C25" s="11">
         <v>0.1</v>
@@ -7027,7 +7053,7 @@
         <v>194</v>
       </c>
       <c r="B26" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C26" s="11">
         <v>0.1</v>
@@ -7041,7 +7067,7 @@
         <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C27" s="11">
         <v>0.1</v>
@@ -7055,7 +7081,7 @@
         <v>194</v>
       </c>
       <c r="B28" t="s">
-        <v>192</v>
+        <v>200</v>
       </c>
       <c r="C28" s="11">
         <v>0.1</v>
@@ -7069,13 +7095,13 @@
         <v>194</v>
       </c>
       <c r="B29" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C29" s="11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D29">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -7083,13 +7109,13 @@
         <v>194</v>
       </c>
       <c r="B30" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C30" s="11">
         <v>0.1</v>
       </c>
       <c r="D30">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -7097,7 +7123,7 @@
         <v>194</v>
       </c>
       <c r="B31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C31" s="11">
         <v>0.1</v>
@@ -7111,7 +7137,7 @@
         <v>194</v>
       </c>
       <c r="B32" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C32" s="11">
         <v>0.1</v>
@@ -7120,54 +7146,68 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="45" t="s">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>194</v>
+      </c>
+      <c r="B33" t="s">
+        <v>203</v>
+      </c>
+      <c r="C33" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D33">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="H35" s="46"/>
-    </row>
-    <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="47" t="s">
+      <c r="H36" s="46"/>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B37" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C37" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="47" t="s">
+      <c r="D37" s="47" t="s">
         <v>215</v>
       </c>
-      <c r="E36" s="47" t="s">
+      <c r="E37" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F36" s="48" t="str">
+      <c r="F37" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G36" s="48" t="str">
+      <c r="G37" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H36" s="49" t="s">
+      <c r="H37" s="49" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D37" t="s">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
         <v>217</v>
       </c>
-      <c r="E37">
+      <c r="E38">
         <v>2018</v>
       </c>
-      <c r="F37">
+      <c r="F38">
         <v>2222</v>
       </c>
-      <c r="G37">
-        <f>F37</f>
+      <c r="G38">
+        <f>F38</f>
         <v>2222</v>
       </c>
-      <c r="H37" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F17)</f>
-        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDSOL</v>
+      <c r="H38" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F18)</f>
+        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDKER,RSDSOL</v>
       </c>
     </row>
   </sheetData>
@@ -7180,7 +7220,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -9310,15 +9350,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9529,6 +9560,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
@@ -9539,14 +9579,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9563,4 +9595,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Same share of building arch
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEFC553-3F2E-4564-BF96-EBE2B59CCC2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC37DEE-2C6E-4BD6-8C92-A06988B2CAFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -6346,7 +6346,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6459,7 +6459,7 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
+        <f t="shared" ref="B6:B16" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
         <v>UC_RSD_MaxGrowth_AmbientHeat</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -6499,7 +6499,7 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
+        <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Biodiesel</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -6539,7 +6539,7 @@
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A24,"MaxGrowth",B24)</f>
+        <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Biomass</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -6559,27 +6559,27 @@
         <v>15</v>
       </c>
       <c r="J8" s="29">
-        <f>1+C24</f>
+        <f t="shared" ref="J8:J16" si="1">1+C24</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
       </c>
       <c r="L8" s="16">
-        <f>-D24</f>
+        <f t="shared" ref="L8:L17" si="2">-D24</f>
         <v>-0.5</v>
       </c>
       <c r="M8" s="2">
         <v>5</v>
       </c>
       <c r="N8" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
+        <f t="shared" ref="N8:N16" si="3">_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A25,"MaxGrowth",B25)</f>
+        <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Coal</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -6599,27 +6599,27 @@
         <v>15</v>
       </c>
       <c r="J9" s="29">
-        <f>1+C25</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
       </c>
       <c r="L9" s="16">
-        <f>-D25</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M9" s="2">
         <v>5</v>
       </c>
       <c r="N9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A25, "maximum growth rate of",B25)</f>
+        <f t="shared" si="3"/>
         <v>RSD maximum growth rate of Coal</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A26,"MaxGrowth",B26)</f>
+        <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Peat</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6639,27 +6639,27 @@
         <v>15</v>
       </c>
       <c r="J10" s="29">
-        <f>1+C26</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K10" s="2">
         <v>1</v>
       </c>
       <c r="L10" s="16">
-        <f>-D26</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M10" s="2">
         <v>5</v>
       </c>
       <c r="N10" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
+        <f t="shared" si="3"/>
         <v>RSD maximum growth rate of Peat</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A27,"MaxGrowth",B27)</f>
+        <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Electricity</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6679,27 +6679,27 @@
         <v>15</v>
       </c>
       <c r="J11" s="29">
-        <f>1+C27</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
       </c>
       <c r="L11" s="16">
-        <f>-D27</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M11" s="2">
         <v>5</v>
       </c>
       <c r="N11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A27, "maximum growth rate of",B27)</f>
+        <f t="shared" si="3"/>
         <v>RSD maximum growth rate of Electricity</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A28,"MaxGrowth",B28)</f>
+        <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Ethanol</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6719,27 +6719,27 @@
         <v>15</v>
       </c>
       <c r="J12" s="29">
-        <f>1+C28</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
       </c>
       <c r="L12" s="16">
-        <f>-D28</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M12" s="2">
         <v>5</v>
       </c>
       <c r="N12" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A28, "maximum growth rate of",B28)</f>
+        <f t="shared" si="3"/>
         <v>RSD maximum growth rate of Ethanol</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A29,"MaxGrowth",B29)</f>
+        <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Gas</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -6759,27 +6759,27 @@
         <v>15</v>
       </c>
       <c r="J13" s="29">
-        <f>1+C29</f>
+        <f t="shared" si="1"/>
         <v>1.05</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
       </c>
       <c r="L13" s="16">
-        <f>-D29</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M13" s="2">
         <v>5</v>
       </c>
       <c r="N13" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A29, "maximum growth rate of",B29)</f>
+        <f t="shared" si="3"/>
         <v>RSD maximum growth rate of Gas</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A30,"MaxGrowth",B30)</f>
+        <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -6799,27 +6799,27 @@
         <v>15</v>
       </c>
       <c r="J14" s="29">
-        <f>1+C30</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K14" s="2">
         <v>1</v>
       </c>
       <c r="L14" s="16">
-        <f>-D30</f>
+        <f t="shared" si="2"/>
         <v>-0.3</v>
       </c>
       <c r="M14" s="2">
         <v>5</v>
       </c>
       <c r="N14" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A30, "maximum growth rate of",B30)</f>
+        <f t="shared" si="3"/>
         <v>RSD maximum growth rate of DistrictHeat</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A31,"MaxGrowth",B31)</f>
+        <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_LPG</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -6839,27 +6839,27 @@
         <v>15</v>
       </c>
       <c r="J15" s="29">
-        <f>1+C31</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K15" s="2">
         <v>1</v>
       </c>
       <c r="L15" s="16">
-        <f>-D31</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M15" s="2">
         <v>5</v>
       </c>
       <c r="N15" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A31, "maximum growth rate of",B31)</f>
+        <f t="shared" si="3"/>
         <v>RSD maximum growth rate of LPG</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A32,"MaxGrowth",B32)</f>
+        <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Kerosene</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -6879,21 +6879,21 @@
         <v>15</v>
       </c>
       <c r="J16" s="29">
-        <f>1+C32</f>
+        <f t="shared" si="1"/>
         <v>1.1000000000000001</v>
       </c>
       <c r="K16" s="2">
         <v>1</v>
       </c>
       <c r="L16" s="16">
-        <f>-D32</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M16" s="2">
         <v>5</v>
       </c>
       <c r="N16" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A32, "maximum growth rate of",B32)</f>
+        <f t="shared" si="3"/>
         <v>RSD maximum growth rate of Kerosene</v>
       </c>
     </row>
@@ -6916,7 +6916,7 @@
         <v>2021</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="J17" s="29">
         <f>1-C33</f>
@@ -6926,7 +6926,7 @@
         <v>1</v>
       </c>
       <c r="L17" s="16">
-        <f>-D33</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M17" s="2">
@@ -6939,7 +6939,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="str">
-        <f t="shared" ref="B18" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A33,"MaxGrowth",B33)</f>
+        <f t="shared" ref="B18" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A33,"MaxGrowth",B33)</f>
         <v>UC_RSD_MaxGrowth_Solar</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -6959,21 +6959,21 @@
         <v>15</v>
       </c>
       <c r="J18" s="29">
-        <f t="shared" ref="J18" si="1">1+C33</f>
+        <f t="shared" ref="J18" si="5">1+C33</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K18" s="2">
         <v>1</v>
       </c>
       <c r="L18" s="16">
-        <f t="shared" ref="L18" si="2">-D33</f>
+        <f t="shared" ref="L18" si="6">-D33</f>
         <v>-0.5</v>
       </c>
       <c r="M18" s="2">
         <v>5</v>
       </c>
       <c r="N18" s="2" t="str">
-        <f t="shared" ref="N18" si="3">_xlfn.TEXTJOIN(" ",TRUE,A33, "maximum growth rate of",B33)</f>
+        <f t="shared" ref="N18" si="7">_xlfn.TEXTJOIN(" ",TRUE,A33, "maximum growth rate of",B33)</f>
         <v>RSD maximum growth rate of Solar</v>
       </c>
     </row>
@@ -9350,6 +9350,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9560,15 +9569,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
@@ -9579,6 +9579,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9595,12 +9603,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Solar to HETD to allow storage.
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC37DEE-2C6E-4BD6-8C92-A06988B2CAFA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE100A8-B418-4C78-AEAC-C621D8F6C909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -6346,7 +6346,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="J13" s="29">
         <f t="shared" si="1"/>
-        <v>1.05</v>
+        <v>1.03</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
@@ -7098,7 +7098,7 @@
         <v>192</v>
       </c>
       <c r="C29" s="11">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="D29">
         <v>0.5</v>
@@ -9350,15 +9350,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9569,6 +9560,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
@@ -9579,14 +9579,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9603,4 +9595,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Tweak Solar and Gas
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE100A8-B418-4C78-AEAC-C621D8F6C909}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4684092-B969-4915-83B5-23FCD9BF7E5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="223">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -6346,7 +6346,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="J13" s="29">
         <f t="shared" si="1"/>
-        <v>1.03</v>
+        <v>1.02</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
@@ -6920,7 +6920,7 @@
       </c>
       <c r="J17" s="29">
         <f>1-C33</f>
-        <v>0.9</v>
+        <v>0.85</v>
       </c>
       <c r="K17" s="2">
         <v>1</v>
@@ -6939,7 +6939,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="str">
-        <f t="shared" ref="B18" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A33,"MaxGrowth",B33)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A33,"MaxGrowth",B33)</f>
         <v>UC_RSD_MaxGrowth_Solar</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -6959,36 +6959,63 @@
         <v>15</v>
       </c>
       <c r="J18" s="29">
-        <f t="shared" ref="J18" si="5">1+C33</f>
-        <v>1.1000000000000001</v>
+        <f>1+C33</f>
+        <v>1.1499999999999999</v>
       </c>
       <c r="K18" s="2">
         <v>1</v>
       </c>
       <c r="L18" s="16">
-        <f t="shared" ref="L18" si="6">-D33</f>
+        <f>-D33</f>
         <v>-0.5</v>
       </c>
       <c r="M18" s="2">
         <v>5</v>
       </c>
       <c r="N18" s="2" t="str">
-        <f t="shared" ref="N18" si="7">_xlfn.TEXTJOIN(" ",TRUE,A33, "maximum growth rate of",B33)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A33, "maximum growth rate of",B33)</f>
         <v>RSD maximum growth rate of Solar</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A33,"MinGrowth",B33)</f>
+        <v>UC_RSD_MinGrowth_Solar</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="D19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="16"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+      <c r="F19" t="s">
+        <v>212</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H19" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J19" s="29">
+        <f>1+C33/15</f>
+        <v>1.01</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1</v>
+      </c>
+      <c r="L19" s="16">
+        <f>-D33</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M19" s="2">
+        <v>5</v>
+      </c>
+      <c r="N19" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A33, "minimum growth rate of",B33)</f>
+        <v>RSD minimum growth rate of Solar</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
@@ -7098,7 +7125,7 @@
         <v>192</v>
       </c>
       <c r="C29" s="11">
-        <v>0.03</v>
+        <v>0.02</v>
       </c>
       <c r="D29">
         <v>0.5</v>
@@ -7154,7 +7181,7 @@
         <v>203</v>
       </c>
       <c r="C33" s="11">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
       <c r="D33">
         <v>0.5</v>

</xml_diff>

<commit_message>
Update CCS, biofuel growth and detached gas
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4684092-B969-4915-83B5-23FCD9BF7E5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71968B13-90DB-47FE-B123-DF8D3E30A7C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="223">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -6343,10 +6343,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
-  <dimension ref="A2:N38"/>
+  <dimension ref="A2:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6459,7 +6459,7 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6:B16" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A24,"MaxGrowth",B24)</f>
         <v>UC_RSD_MaxGrowth_AmbientHeat</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -6479,27 +6479,27 @@
         <v>15</v>
       </c>
       <c r="J6" s="29">
-        <f>1+C23</f>
-        <v>1.1000000000000001</v>
+        <f>1+C25</f>
+        <v>1.05</v>
       </c>
       <c r="K6" s="2">
         <v>1</v>
       </c>
       <c r="L6" s="16">
-        <f>-D23</f>
+        <f>-D25</f>
         <v>-0.5</v>
       </c>
       <c r="M6" s="2">
         <v>5</v>
       </c>
       <c r="N6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A25, "maximum growth rate of",B25)</f>
         <v>RSD maximum growth rate of Biodiesel</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A25,"MaxGrowth",B25)</f>
         <v>UC_RSD_MaxGrowth_Biodiesel</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -6519,27 +6519,27 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f>1+C24</f>
+        <f>1+C26</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="16">
-        <f>-D24</f>
+        <f>-D26</f>
         <v>-0.5</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
       </c>
       <c r="N7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A26,"MaxGrowth",B26)</f>
         <v>UC_RSD_MaxGrowth_Biomass</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -6559,27 +6559,27 @@
         <v>15</v>
       </c>
       <c r="J8" s="29">
-        <f t="shared" ref="J8:J16" si="1">1+C24</f>
+        <f>1+C26</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
       </c>
       <c r="L8" s="16">
-        <f t="shared" ref="L8:L17" si="2">-D24</f>
+        <f>-D26</f>
         <v>-0.5</v>
       </c>
       <c r="M8" s="2">
         <v>5</v>
       </c>
       <c r="N8" s="2" t="str">
-        <f t="shared" ref="N8:N16" si="3">_xlfn.TEXTJOIN(" ",TRUE,A24, "maximum growth rate of",B24)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A27,"MaxGrowth",B27)</f>
         <v>UC_RSD_MaxGrowth_Coal</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -6599,35 +6599,35 @@
         <v>15</v>
       </c>
       <c r="J9" s="29">
-        <f t="shared" si="1"/>
+        <f>1+C27</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
       </c>
       <c r="L9" s="16">
-        <f t="shared" si="2"/>
+        <f>-D27</f>
         <v>-0.5</v>
       </c>
       <c r="M9" s="2">
         <v>5</v>
       </c>
       <c r="N9" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A27, "maximum growth rate of",B27)</f>
         <v>RSD maximum growth rate of Coal</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_RSD_MaxGrowth_Peat</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A27,"MaxGrowth",B27)</f>
+        <v>UC_RSD_MaxGrowth_Coal</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D10" s="2"/>
       <c r="F10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>142</v>
@@ -6636,38 +6636,38 @@
         <v>2021</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="J10" s="29">
-        <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <f>1-C28</f>
+        <v>0.9</v>
       </c>
       <c r="K10" s="2">
         <v>1</v>
       </c>
       <c r="L10" s="16">
-        <f t="shared" si="2"/>
+        <f>-D28</f>
         <v>-0.5</v>
       </c>
       <c r="M10" s="2">
         <v>5</v>
       </c>
       <c r="N10" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>RSD maximum growth rate of Peat</v>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A28, "maximum degrowth rate of",B27)</f>
+        <v>RSD maximum degrowth rate of Coal</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_RSD_MaxGrowth_Electricity</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A28,"MaxGrowth",B28)</f>
+        <v>UC_RSD_MaxGrowth_Peat</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D11" s="2"/>
       <c r="F11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>142</v>
@@ -6679,35 +6679,35 @@
         <v>15</v>
       </c>
       <c r="J11" s="29">
-        <f t="shared" si="1"/>
+        <f>1+C28</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
       </c>
       <c r="L11" s="16">
-        <f t="shared" si="2"/>
+        <f>-D28</f>
         <v>-0.5</v>
       </c>
       <c r="M11" s="2">
         <v>5</v>
       </c>
       <c r="N11" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>RSD maximum growth rate of Electricity</v>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A28, "maximum growth rate of",B28)</f>
+        <v>RSD maximum growth rate of Peat</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_RSD_MaxGrowth_Ethanol</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A29,"MaxGrowth",B28)</f>
+        <v>UC_RSD_MaxGrowth_Peat</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D12" s="2"/>
       <c r="F12" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>142</v>
@@ -6716,38 +6716,38 @@
         <v>2021</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="J12" s="29">
-        <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <f>1-C28</f>
+        <v>0.9</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
       </c>
       <c r="L12" s="16">
-        <f t="shared" si="2"/>
+        <f>-D29</f>
         <v>-0.5</v>
       </c>
       <c r="M12" s="2">
         <v>5</v>
       </c>
       <c r="N12" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>RSD maximum growth rate of Ethanol</v>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A29, "maximum degrowth rate of",B28)</f>
+        <v>RSD maximum degrowth rate of Peat</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_RSD_MaxGrowth_Gas</v>
+        <f t="shared" ref="B13:B18" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A29,"MaxGrowth",B29)</f>
+        <v>UC_RSD_MaxGrowth_Electricity</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D13" s="2"/>
       <c r="F13" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>142</v>
@@ -6759,35 +6759,35 @@
         <v>15</v>
       </c>
       <c r="J13" s="29">
-        <f t="shared" si="1"/>
-        <v>1.02</v>
+        <f t="shared" ref="J13:J18" si="1">1+C29</f>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
       </c>
       <c r="L13" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L13:L19" si="2">-D29</f>
         <v>-0.5</v>
       </c>
       <c r="M13" s="2">
         <v>5</v>
       </c>
       <c r="N13" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>RSD maximum growth rate of Gas</v>
+        <f t="shared" ref="N13:N18" si="3">_xlfn.TEXTJOIN(" ",TRUE,A29, "maximum growth rate of",B29)</f>
+        <v>RSD maximum growth rate of Electricity</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>UC_RSD_MaxGrowth_DistrictHeat</v>
+        <v>UC_RSD_MaxGrowth_Ethanol</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D14" s="2"/>
       <c r="F14" t="s">
-        <v>221</v>
+        <v>208</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>142</v>
@@ -6807,27 +6807,27 @@
       </c>
       <c r="L14" s="16">
         <f t="shared" si="2"/>
-        <v>-0.3</v>
+        <v>-0.5</v>
       </c>
       <c r="M14" s="2">
         <v>5</v>
       </c>
       <c r="N14" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>RSD maximum growth rate of DistrictHeat</v>
+        <v>RSD maximum growth rate of Ethanol</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>UC_RSD_MaxGrowth_LPG</v>
+        <v>UC_RSD_MaxGrowth_Gas</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D15" s="2"/>
       <c r="F15" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>142</v>
@@ -6840,7 +6840,7 @@
       </c>
       <c r="J15" s="29">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>1.01</v>
       </c>
       <c r="K15" s="2">
         <v>1</v>
@@ -6854,20 +6854,20 @@
       </c>
       <c r="N15" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>RSD maximum growth rate of LPG</v>
+        <v>RSD maximum growth rate of Gas</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>UC_RSD_MaxGrowth_Kerosene</v>
+        <v>UC_RSD_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D16" s="2"/>
       <c r="F16" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>142</v>
@@ -6887,27 +6887,27 @@
       </c>
       <c r="L16" s="16">
         <f t="shared" si="2"/>
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="M16" s="2">
         <v>5</v>
       </c>
       <c r="N16" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>RSD maximum growth rate of Kerosene</v>
+        <v>RSD maximum growth rate of DistrictHeat</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A32,"MaxDegrowth",B32)</f>
-        <v>UC_RSD_MaxDegrowth_Kerosene</v>
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_LPG</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D17" s="2"/>
       <c r="F17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>142</v>
@@ -6916,11 +6916,11 @@
         <v>2021</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="J17" s="29">
-        <f>1-C33</f>
-        <v>0.85</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K17" s="2">
         <v>1</v>
@@ -6933,21 +6933,21 @@
         <v>5</v>
       </c>
       <c r="N17" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A32, "maximum degrowth rate of",B32)</f>
-        <v>RSD maximum degrowth rate of Kerosene</v>
+        <f t="shared" si="3"/>
+        <v>RSD maximum growth rate of LPG</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A33,"MaxGrowth",B33)</f>
-        <v>UC_RSD_MaxGrowth_Solar</v>
+        <f t="shared" si="0"/>
+        <v>UC_RSD_MaxGrowth_Kerosene</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D18" s="2"/>
       <c r="F18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>142</v>
@@ -6959,35 +6959,35 @@
         <v>15</v>
       </c>
       <c r="J18" s="29">
-        <f>1+C33</f>
-        <v>1.1499999999999999</v>
+        <f t="shared" si="1"/>
+        <v>1.1000000000000001</v>
       </c>
       <c r="K18" s="2">
         <v>1</v>
       </c>
       <c r="L18" s="16">
-        <f>-D33</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M18" s="2">
         <v>5</v>
       </c>
       <c r="N18" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A33, "maximum growth rate of",B33)</f>
-        <v>RSD maximum growth rate of Solar</v>
+        <f t="shared" si="3"/>
+        <v>RSD maximum growth rate of Kerosene</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A33,"MinGrowth",B33)</f>
-        <v>UC_RSD_MinGrowth_Solar</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A34,"MaxDegrowth",B34)</f>
+        <v>UC_RSD_MaxDegrowth_Kerosene</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>144</v>
       </c>
       <c r="D19" s="2"/>
       <c r="F19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>142</v>
@@ -6999,52 +6999,110 @@
         <v>185</v>
       </c>
       <c r="J19" s="29">
-        <f>1+C33/15</f>
-        <v>1.01</v>
+        <f>1-C35</f>
+        <v>0.9</v>
       </c>
       <c r="K19" s="2">
         <v>1</v>
       </c>
       <c r="L19" s="16">
-        <f>-D33</f>
+        <f t="shared" si="2"/>
         <v>-0.5</v>
       </c>
       <c r="M19" s="2">
         <v>5</v>
       </c>
       <c r="N19" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A33, "minimum growth rate of",B33)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A34, "maximum degrowth rate of",B34)</f>
+        <v>RSD maximum degrowth rate of Kerosene</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A35,"MaxGrowth",B35)</f>
+        <v>UC_RSD_MaxGrowth_Solar</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D20" s="2"/>
+      <c r="F20" t="s">
+        <v>212</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H20" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" s="29">
+        <f>1+C35</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1</v>
+      </c>
+      <c r="L20" s="16">
+        <f>-D35</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M20" s="2">
+        <v>5</v>
+      </c>
+      <c r="N20" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A35, "maximum growth rate of",B35)</f>
+        <v>RSD maximum growth rate of Solar</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A35,"MinGrowth",B35)</f>
+        <v>UC_RSD_MinGrowth_Solar</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="F21" t="s">
+        <v>212</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="H21" s="2">
+        <v>2021</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J21" s="29">
+        <f>1+C35/15</f>
+        <v>1.0066666666666666</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1</v>
+      </c>
+      <c r="L21" s="16">
+        <f>-D35</f>
+        <v>-0.5</v>
+      </c>
+      <c r="M21" s="2">
+        <v>5</v>
+      </c>
+      <c r="N21" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A35, "minimum growth rate of",B35)</f>
         <v>RSD minimum growth rate of Solar</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>117</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>194</v>
-      </c>
-      <c r="B22" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>194</v>
-      </c>
-      <c r="B23" t="s">
-        <v>196</v>
-      </c>
-      <c r="C23" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="D23">
-        <v>0.5</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -7052,13 +7110,7 @@
         <v>194</v>
       </c>
       <c r="B24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="D24">
-        <v>0.5</v>
+        <v>190</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -7066,10 +7118,10 @@
         <v>194</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C25" s="11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D25">
         <v>0.5</v>
@@ -7080,7 +7132,7 @@
         <v>194</v>
       </c>
       <c r="B26" t="s">
-        <v>198</v>
+        <v>137</v>
       </c>
       <c r="C26" s="11">
         <v>0.1</v>
@@ -7094,7 +7146,7 @@
         <v>194</v>
       </c>
       <c r="B27" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C27" s="11">
         <v>0.1</v>
@@ -7108,7 +7160,7 @@
         <v>194</v>
       </c>
       <c r="B28" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C28" s="11">
         <v>0.1</v>
@@ -7122,10 +7174,10 @@
         <v>194</v>
       </c>
       <c r="B29" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="C29" s="11">
-        <v>0.02</v>
+        <v>0.1</v>
       </c>
       <c r="D29">
         <v>0.5</v>
@@ -7136,13 +7188,13 @@
         <v>194</v>
       </c>
       <c r="B30" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="C30" s="11">
         <v>0.1</v>
       </c>
       <c r="D30">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -7150,10 +7202,10 @@
         <v>194</v>
       </c>
       <c r="B31" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C31" s="11">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="D31">
         <v>0.5</v>
@@ -7164,13 +7216,13 @@
         <v>194</v>
       </c>
       <c r="B32" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C32" s="11">
         <v>0.1</v>
       </c>
       <c r="D32">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -7178,63 +7230,91 @@
         <v>194</v>
       </c>
       <c r="B33" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C33" s="11">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D33">
         <v>0.5</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="45" t="s">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" t="s">
+        <v>202</v>
+      </c>
+      <c r="C34" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D34">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>194</v>
+      </c>
+      <c r="B35" t="s">
+        <v>203</v>
+      </c>
+      <c r="C35" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="D35">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="H36" s="46"/>
-    </row>
-    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="47" t="s">
+      <c r="H38" s="46"/>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="C37" s="47" t="s">
+      <c r="C39" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="47" t="s">
+      <c r="D39" s="47" t="s">
         <v>215</v>
       </c>
-      <c r="E37" s="47" t="s">
+      <c r="E39" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="48" t="str">
+      <c r="F39" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!C$3,"*")</f>
         <v>IE</v>
       </c>
-      <c r="G37" s="48" t="str">
+      <c r="G39" s="48" t="str">
         <f>IF(Regions!C$3&lt;&gt;"",Regions!D$3,"*")</f>
         <v>National</v>
       </c>
-      <c r="H37" s="49" t="s">
+      <c r="H39" s="49" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
         <v>217</v>
       </c>
-      <c r="E38">
+      <c r="E40">
         <v>2018</v>
       </c>
-      <c r="F38">
+      <c r="F40">
         <v>2222</v>
       </c>
-      <c r="G38">
-        <f>F38</f>
+      <c r="G40">
+        <f>F40</f>
         <v>2222</v>
       </c>
-      <c r="H38" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F18)</f>
-        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDKER,RSDSOL</v>
+      <c r="H40" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F20)</f>
+        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDCOA,RSDPEA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDKER,RSDSOL</v>
       </c>
     </row>
   </sheetData>
@@ -9377,6 +9457,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9587,15 +9676,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
@@ -9606,6 +9686,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9622,12 +9710,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update CB and Max Growth
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71968B13-90DB-47FE-B123-DF8D3E30A7C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CAA722-C92E-4202-88DB-0975DD770E9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -6346,7 +6346,7 @@
   <dimension ref="A2:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6519,8 +6519,8 @@
         <v>15</v>
       </c>
       <c r="J7" s="29">
-        <f>1+C26</f>
-        <v>1.1000000000000001</v>
+        <f>1+C25</f>
+        <v>1.05</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
@@ -6560,7 +6560,7 @@
       </c>
       <c r="J8" s="29">
         <f>1+C26</f>
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="K8" s="2">
         <v>1</v>
@@ -6600,7 +6600,7 @@
       </c>
       <c r="J9" s="29">
         <f>1+C27</f>
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
@@ -6639,7 +6639,7 @@
         <v>185</v>
       </c>
       <c r="J10" s="29">
-        <f>1-C28</f>
+        <f>1-C27*2</f>
         <v>0.9</v>
       </c>
       <c r="K10" s="2">
@@ -6680,7 +6680,7 @@
       </c>
       <c r="J11" s="29">
         <f>1+C28</f>
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
@@ -6719,7 +6719,7 @@
         <v>185</v>
       </c>
       <c r="J12" s="29">
-        <f>1-C28</f>
+        <f>1-C28*2</f>
         <v>0.9</v>
       </c>
       <c r="K12" s="2">
@@ -6840,7 +6840,7 @@
       </c>
       <c r="J15" s="29">
         <f t="shared" si="1"/>
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="K15" s="2">
         <v>1</v>
@@ -6920,7 +6920,7 @@
       </c>
       <c r="J17" s="29">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="K17" s="2">
         <v>1</v>
@@ -6960,7 +6960,7 @@
       </c>
       <c r="J18" s="29">
         <f t="shared" si="1"/>
-        <v>1.1000000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="K18" s="2">
         <v>1</v>
@@ -6999,7 +6999,7 @@
         <v>185</v>
       </c>
       <c r="J19" s="29">
-        <f>1-C35</f>
+        <f>1-C34*2</f>
         <v>0.9</v>
       </c>
       <c r="K19" s="2">
@@ -7135,7 +7135,7 @@
         <v>137</v>
       </c>
       <c r="C26" s="11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D26">
         <v>0.5</v>
@@ -7149,7 +7149,7 @@
         <v>197</v>
       </c>
       <c r="C27" s="11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D27">
         <v>0.5</v>
@@ -7163,7 +7163,7 @@
         <v>198</v>
       </c>
       <c r="C28" s="11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D28">
         <v>0.5</v>
@@ -7205,7 +7205,7 @@
         <v>192</v>
       </c>
       <c r="C31" s="11">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D31">
         <v>0.5</v>
@@ -7233,7 +7233,7 @@
         <v>201</v>
       </c>
       <c r="C33" s="11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D33">
         <v>0.5</v>
@@ -7247,7 +7247,7 @@
         <v>202</v>
       </c>
       <c r="C34" s="11">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="D34">
         <v>0.5</v>
@@ -9451,21 +9451,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9676,24 +9661,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9710,4 +9693,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Test Ambient Heat Share and add SRV Biogas Constraint
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B3B95D-AD0F-4EFE-9A67-84136C5D601E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA71C92-7FDC-41F0-875D-DF6CB83FAD97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -7331,7 +7331,7 @@
   <dimension ref="A2:N25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7506,14 +7506,14 @@
       </c>
       <c r="J7" s="29">
         <f>1+C16</f>
-        <v>1.05</v>
+        <v>1.01</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
       </c>
       <c r="L7" s="16">
         <f t="shared" si="1"/>
-        <v>-0.3</v>
+        <v>-0.1</v>
       </c>
       <c r="M7" s="2">
         <v>5</v>
@@ -7726,10 +7726,10 @@
         <v>138</v>
       </c>
       <c r="C16" s="11">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="D16">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -9517,12 +9517,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9733,6 +9727,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
@@ -9742,15 +9742,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9767,4 +9758,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Minimum Biogas RSD - match SRV.
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA71C92-7FDC-41F0-875D-DF6CB83FAD97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC46CF9F-85FF-479B-AC6A-7AB1601142EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -6348,8 +6348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6843,7 +6843,7 @@
       </c>
       <c r="J15" s="29">
         <f t="shared" si="1"/>
-        <v>1.02</v>
+        <v>1.01</v>
       </c>
       <c r="K15" s="2">
         <v>1</v>
@@ -7208,7 +7208,7 @@
         <v>192</v>
       </c>
       <c r="C31" s="11">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="D31">
         <v>0.1</v>
@@ -7331,7 +7331,7 @@
   <dimension ref="A2:N25"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7506,7 +7506,7 @@
       </c>
       <c r="J7" s="29">
         <f>1+C16</f>
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
@@ -7726,7 +7726,7 @@
         <v>138</v>
       </c>
       <c r="C16" s="11">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D16">
         <v>0.1</v>
@@ -9517,6 +9517,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9727,12 +9733,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
@@ -9742,6 +9742,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9758,13 +9767,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DC efficieny and SOL Act Bnd
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{387508AF-E8BE-46C7-B556-2830453C1179}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599D672E-1362-4CDE-92B8-64F5C0C34ECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="230">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -875,6 +875,12 @@
   </si>
   <si>
     <t>DH_IND</t>
+  </si>
+  <si>
+    <t>DH_SOL</t>
+  </si>
+  <si>
+    <t>DH_SOL*</t>
   </si>
 </sst>
 </file>
@@ -5815,10 +5821,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:N28"/>
+  <dimension ref="A2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5914,7 +5920,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6:B9" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
+        <f t="shared" ref="B6:B9" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5930,21 +5936,21 @@
         <v>15</v>
       </c>
       <c r="G6" s="26">
-        <f t="shared" ref="G6:G9" si="1">1+$C15</f>
+        <f t="shared" ref="G6:G9" si="1">1+$C16</f>
         <v>1.05</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
       </c>
       <c r="I6" s="16">
-        <f t="shared" ref="I6:I11" si="2">-D15</f>
+        <f t="shared" ref="I6:I11" si="2">-D16</f>
         <v>-0.1</v>
       </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
       <c r="K6" s="2" t="str">
-        <f t="shared" ref="K6:K11" si="3">_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
+        <f t="shared" ref="K6:K11" si="3">_xlfn.TEXTJOIN(" ",TRUE,A16, "maximum growth rate of",B16)</f>
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
@@ -6058,7 +6064,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
-        <f t="shared" ref="B10:B12" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A19,"MaxGrowth",B19)</f>
+        <f t="shared" ref="B10:B12" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A20,"MaxGrowth",B20)</f>
         <v>UC_PWR_MaxGrowth_PV</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6074,7 +6080,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="26">
-        <f t="shared" ref="G10:G12" si="5">1+$C19</f>
+        <f t="shared" ref="G10:G13" si="5">1+$C20</f>
         <v>1.2</v>
       </c>
       <c r="H10" s="2">
@@ -6153,37 +6159,59 @@
         <v>1</v>
       </c>
       <c r="I12" s="16">
-        <f t="shared" ref="I12" si="6">-D21</f>
+        <f t="shared" ref="I12" si="6">-D22</f>
         <v>-0.1</v>
       </c>
       <c r="J12" s="2">
         <v>5</v>
       </c>
       <c r="K12" s="2" t="str">
-        <f t="shared" ref="K12" si="7">_xlfn.TEXTJOIN(" ",TRUE,A21, "maximum growth rate of",B21)</f>
+        <f t="shared" ref="K12" si="7">_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
         <v>PWR maximum growth rate of DH_IND</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="str">
+        <f t="shared" ref="B13" si="8">_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
+        <v>UC_PWR_MaxGrowth_DH_SOL</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E13">
+        <v>2018</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="26">
+        <f t="shared" si="5"/>
+        <v>1.02</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="16">
+        <f t="shared" ref="I13" si="9">-D23</f>
+        <v>-0.1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>5</v>
+      </c>
+      <c r="K13" s="2" t="str">
+        <f t="shared" ref="K13" si="10">_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
+        <v>PWR maximum growth rate of DH_SOL</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>117</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>128</v>
-      </c>
-      <c r="B15" t="s">
-        <v>124</v>
-      </c>
-      <c r="C15" s="11">
-        <v>0.05</v>
-      </c>
-      <c r="D15">
-        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -6191,13 +6219,13 @@
         <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C16" s="11">
-        <v>0.2</v>
+        <v>0.05</v>
       </c>
       <c r="D16">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -6205,13 +6233,13 @@
         <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C17" s="11">
         <v>0.2</v>
       </c>
       <c r="D17">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -6219,13 +6247,13 @@
         <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="C18" s="11">
         <v>0.2</v>
       </c>
       <c r="D18">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -6233,7 +6261,7 @@
         <v>128</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C19" s="11">
         <v>0.2</v>
@@ -6247,7 +6275,7 @@
         <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" s="11">
         <v>0.2</v>
@@ -6261,94 +6289,96 @@
         <v>128</v>
       </c>
       <c r="B21" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
         <v>227</v>
       </c>
-      <c r="C21" s="11">
+      <c r="C22" s="11">
         <v>0.02</v>
       </c>
-      <c r="D21">
+      <c r="D22">
         <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
+      <c r="A23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" t="s">
+        <v>228</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.02</v>
+      </c>
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E25" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J25" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2019</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G25" s="26">
-        <f>1+$C30</f>
-        <v>1</v>
-      </c>
-      <c r="H25" s="16">
-        <v>0.6</v>
-      </c>
-      <c r="I25" s="2">
-        <v>3</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
         <v>154</v>
       </c>
       <c r="E26" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>185</v>
@@ -6358,48 +6388,74 @@
         <v>1</v>
       </c>
       <c r="H26" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="I26" s="2">
+        <v>3</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>180</v>
-      </c>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E27">
-        <v>2026</v>
+        <v>154</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2020</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>185</v>
       </c>
       <c r="G27" s="26">
-        <f>1+$C31</f>
+        <f>1+$C32</f>
         <v>1</v>
       </c>
       <c r="H27" s="16">
-        <v>1</v>
-      </c>
-      <c r="I27" s="2">
-        <v>3</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>184</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="E28">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="G28" s="26">
+        <f>1+$C32</f>
+        <v>1</v>
+      </c>
       <c r="H28" s="16">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <v>3</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+      <c r="E29">
+        <v>2027</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H29" s="16">
         <v>2</v>
       </c>
     </row>
@@ -9725,6 +9781,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9935,15 +10000,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
@@ -9954,6 +10010,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9970,12 +10034,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Max Growth edit, no ker in Apt, Sol DH start 2022
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88731729-5641-47B6-8619-2F9B8DCCA5A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A48C89E-0895-499C-8E2E-CBB4CC41890D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -6469,7 +6469,7 @@
   <dimension ref="A2:N40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6883,7 +6883,7 @@
       </c>
       <c r="J13" s="29">
         <f t="shared" ref="J13:J18" si="1">1+C29</f>
-        <v>1.1499999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
@@ -6963,7 +6963,7 @@
       </c>
       <c r="J15" s="29">
         <f t="shared" si="1"/>
-        <v>1.03</v>
+        <v>1.0249999999999999</v>
       </c>
       <c r="K15" s="2">
         <v>1</v>
@@ -7043,7 +7043,7 @@
       </c>
       <c r="J17" s="29">
         <f t="shared" si="1"/>
-        <v>1.04</v>
+        <v>1.0249999999999999</v>
       </c>
       <c r="K17" s="2">
         <v>1</v>
@@ -7083,7 +7083,7 @@
       </c>
       <c r="J18" s="29">
         <f t="shared" si="1"/>
-        <v>1.1499999999999999</v>
+        <v>1.01</v>
       </c>
       <c r="K18" s="2">
         <v>1</v>
@@ -7122,7 +7122,7 @@
         <v>185</v>
       </c>
       <c r="J19" s="29">
-        <f>1-C34*2</f>
+        <f>1-C34*30</f>
         <v>0.7</v>
       </c>
       <c r="K19" s="2">
@@ -7235,7 +7235,7 @@
       <c r="B24" t="s">
         <v>190</v>
       </c>
-      <c r="C24" s="11">
+      <c r="C24" s="50">
         <v>0.2</v>
       </c>
       <c r="D24">
@@ -7249,7 +7249,7 @@
       <c r="B25" t="s">
         <v>196</v>
       </c>
-      <c r="C25" s="11">
+      <c r="C25" s="50">
         <v>0.02</v>
       </c>
       <c r="D25">
@@ -7263,7 +7263,7 @@
       <c r="B26" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="11">
+      <c r="C26" s="50">
         <v>0.02</v>
       </c>
       <c r="D26">
@@ -7277,7 +7277,7 @@
       <c r="B27" t="s">
         <v>197</v>
       </c>
-      <c r="C27" s="11">
+      <c r="C27" s="50">
         <v>0.01</v>
       </c>
       <c r="D27">
@@ -7291,7 +7291,7 @@
       <c r="B28" t="s">
         <v>198</v>
       </c>
-      <c r="C28" s="11">
+      <c r="C28" s="50">
         <v>0.01</v>
       </c>
       <c r="D28">
@@ -7305,8 +7305,8 @@
       <c r="B29" t="s">
         <v>199</v>
       </c>
-      <c r="C29" s="11">
-        <v>0.15</v>
+      <c r="C29" s="50">
+        <v>0.2</v>
       </c>
       <c r="D29">
         <v>0.1</v>
@@ -7319,7 +7319,7 @@
       <c r="B30" t="s">
         <v>200</v>
       </c>
-      <c r="C30" s="11">
+      <c r="C30" s="50">
         <v>0.1</v>
       </c>
       <c r="D30">
@@ -7333,8 +7333,8 @@
       <c r="B31" t="s">
         <v>192</v>
       </c>
-      <c r="C31" s="11">
-        <v>0.03</v>
+      <c r="C31" s="50">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D31">
         <v>0.1</v>
@@ -7347,7 +7347,7 @@
       <c r="B32" t="s">
         <v>191</v>
       </c>
-      <c r="C32" s="11">
+      <c r="C32" s="50">
         <v>0.15</v>
       </c>
       <c r="D32">
@@ -7361,8 +7361,8 @@
       <c r="B33" t="s">
         <v>201</v>
       </c>
-      <c r="C33" s="11">
-        <v>0.04</v>
+      <c r="C33" s="50">
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D33">
         <v>0.1</v>
@@ -7375,8 +7375,8 @@
       <c r="B34" t="s">
         <v>202</v>
       </c>
-      <c r="C34" s="11">
-        <v>0.15</v>
+      <c r="C34" s="50">
+        <v>0.01</v>
       </c>
       <c r="D34">
         <v>0.1</v>
@@ -7389,7 +7389,7 @@
       <c r="B35" t="s">
         <v>203</v>
       </c>
-      <c r="C35" s="11">
+      <c r="C35" s="50">
         <v>0.15</v>
       </c>
       <c r="D35">
@@ -9992,18 +9992,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -10026,18 +10026,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
ccs to 1.5% and 0.1GW
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84D1BC2F-40B0-4AE2-9E70-13CFF63AE0BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA20975-772A-4802-828A-345A7F0F5D38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -5821,10 +5821,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:N29"/>
+  <dimension ref="A2:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5937,14 +5937,14 @@
       </c>
       <c r="G6" s="26">
         <f t="shared" ref="G6:G9" si="1">1+$C16</f>
-        <v>1.01</v>
+        <v>1.0149999999999999</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
       </c>
       <c r="I6" s="16">
         <f t="shared" ref="I6:I11" si="2">-D16</f>
-        <v>-0.05</v>
+        <v>-0.1</v>
       </c>
       <c r="J6" s="2">
         <v>5</v>
@@ -6221,11 +6221,11 @@
       <c r="B16" t="s">
         <v>124</v>
       </c>
-      <c r="C16" s="11">
-        <v>0.01</v>
+      <c r="C16" s="50">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="D16">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -6327,84 +6327,61 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2" t="s">
+      <c r="C24" s="11"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C26" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D26" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E26" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F26" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G26" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H26" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="J26" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E26" s="2">
-        <v>2019</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G26" s="26">
-        <f>1+$C31</f>
-        <v>1</v>
-      </c>
-      <c r="H26" s="16">
-        <v>0.6</v>
-      </c>
-      <c r="I26" s="2">
-        <v>3</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
         <v>154</v>
       </c>
       <c r="E27" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>185</v>
@@ -6414,48 +6391,74 @@
         <v>1</v>
       </c>
       <c r="H27" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="I27" s="2">
+        <v>3</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>180</v>
-      </c>
+      <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E28">
-        <v>2026</v>
+        <v>154</v>
+      </c>
+      <c r="E28" s="2">
+        <v>2020</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>185</v>
       </c>
       <c r="G28" s="26">
-        <f>1+$C32</f>
+        <f>1+$C33</f>
         <v>1</v>
       </c>
       <c r="H28" s="16">
-        <v>1</v>
-      </c>
-      <c r="I28" s="2">
-        <v>3</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>184</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D29" s="2"/>
+      <c r="B29" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="E29">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="G29" s="26">
+        <f>1+$C33</f>
+        <v>1</v>
+      </c>
       <c r="H29" s="16">
+        <v>1</v>
+      </c>
+      <c r="I29" s="2">
+        <v>3</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D30" s="2"/>
+      <c r="E30">
+        <v>2027</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H30" s="16">
         <v>2</v>
       </c>
     </row>
@@ -9781,21 +9784,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10006,24 +9994,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10040,4 +10026,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update all growth rates
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1745DBC-ABA1-4E55-9CC1-2C557A60F550}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627FF095-8BBA-45D8-97A4-793CC181E807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -5823,8 +5823,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:N30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6153,7 +6153,7 @@
       </c>
       <c r="G12" s="26">
         <f t="shared" si="5"/>
-        <v>1.05</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H12" s="2">
         <v>1</v>
@@ -6189,7 +6189,7 @@
       </c>
       <c r="G13" s="26">
         <f t="shared" si="5"/>
-        <v>1.05</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H13" s="2">
         <v>1</v>
@@ -6306,7 +6306,7 @@
         <v>227</v>
       </c>
       <c r="C22" s="11">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D22">
         <v>0.1</v>
@@ -6320,7 +6320,7 @@
         <v>228</v>
       </c>
       <c r="C23" s="11">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D23">
         <v>0.1</v>
@@ -6472,7 +6472,7 @@
   <dimension ref="A2:N37"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C21" sqref="C21:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7339,8 +7339,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9664,6 +9664,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9874,22 +9889,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9906,21 +9923,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Biodiesel start 2030 with 2% growth and no CB6 Residential
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627FF095-8BBA-45D8-97A4-793CC181E807}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6BEED6-86B0-4909-B850-5A83ADE43101}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -5823,7 +5823,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
@@ -6471,8 +6471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:D32"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7136,7 +7136,7 @@
         <v>0.02</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -7340,7 +7340,7 @@
   <dimension ref="A2:N28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:D24"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9664,21 +9664,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9889,24 +9874,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9923,4 +9906,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
No Max Growth DH and update AF DH
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3832DBE5-C176-416E-B3D0-F08728C2B4D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E4E75F-EC08-4826-A30C-3BE84FFED2E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="228">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -871,16 +871,10 @@
     <t>SRVLPG</t>
   </si>
   <si>
-    <t>DH_IND*</t>
-  </si>
-  <si>
     <t>DH_IND</t>
   </si>
   <si>
     <t>DH_SOL</t>
-  </si>
-  <si>
-    <t>DH_SOL*</t>
   </si>
 </sst>
 </file>
@@ -5821,10 +5815,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:N30"/>
+  <dimension ref="A2:N28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5920,7 +5914,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6:B9" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
+        <f t="shared" ref="B6:B9" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5936,21 +5930,21 @@
         <v>15</v>
       </c>
       <c r="G6" s="26">
-        <f t="shared" ref="G6:G9" si="1">1+$C16</f>
+        <f t="shared" ref="G6:G9" si="1">1+$C14</f>
         <v>1.02</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
       </c>
       <c r="I6" s="16">
-        <f t="shared" ref="I6:I11" si="2">-D16</f>
+        <f t="shared" ref="I6:I11" si="2">-D14</f>
         <v>-0.1</v>
       </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
       <c r="K6" s="2" t="str">
-        <f t="shared" ref="K6:K11" si="3">_xlfn.TEXTJOIN(" ",TRUE,A16, "maximum growth rate of",B16)</f>
+        <f t="shared" ref="K6:K11" si="3">_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
@@ -6064,7 +6058,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
-        <f t="shared" ref="B10:B12" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A20,"MaxGrowth",B20)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_PWR_MaxGrowth_PV</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6080,7 +6074,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="26">
-        <f t="shared" ref="G10:G13" si="5">1+$C20</f>
+        <f>1+$C18</f>
         <v>1.2</v>
       </c>
       <c r="H10" s="2">
@@ -6100,7 +6094,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A19,"MaxGrowth",B19)</f>
         <v>UC_PWR_MaxGrowth_CSP</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6116,7 +6110,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="26">
-        <f t="shared" si="5"/>
+        <f>1+$C19</f>
         <v>1.2</v>
       </c>
       <c r="H11" s="2">
@@ -6134,84 +6128,40 @@
         <v>PWR maximum growth rate of CSP</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>UC_PWR_MaxGrowth_DH_IND</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="E12">
-        <v>2018</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="26">
-        <f t="shared" si="5"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H12" s="2">
-        <v>1</v>
-      </c>
-      <c r="I12" s="16">
-        <f t="shared" ref="I12" si="6">-D22</f>
-        <v>-0.1</v>
-      </c>
-      <c r="J12" s="2">
-        <v>5</v>
-      </c>
-      <c r="K12" s="2" t="str">
-        <f t="shared" ref="K12" si="7">_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
-        <v>PWR maximum growth rate of DH_IND</v>
-      </c>
-    </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="str">
-        <f t="shared" ref="B13" si="8">_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
-        <v>UC_PWR_MaxGrowth_DH_SOL</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="E13">
-        <v>2018</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="26">
-        <f t="shared" si="5"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H13" s="2">
-        <v>1</v>
-      </c>
-      <c r="I13" s="16">
-        <f t="shared" ref="I13" si="9">-D23</f>
-        <v>-0.1</v>
-      </c>
-      <c r="J13" s="2">
-        <v>5</v>
-      </c>
-      <c r="K13" s="2" t="str">
-        <f t="shared" ref="K13" si="10">_xlfn.TEXTJOIN(" ",TRUE,A23, "maximum growth rate of",B23)</f>
-        <v>PWR maximum growth rate of DH_SOL</v>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="50">
+        <v>0.02</v>
+      </c>
+      <c r="D14">
+        <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>117</v>
-      </c>
-      <c r="D15" t="s">
-        <v>119</v>
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="D15">
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -6219,10 +6169,10 @@
         <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>124</v>
-      </c>
-      <c r="C16" s="50">
-        <v>0.02</v>
+        <v>126</v>
+      </c>
+      <c r="C16" s="11">
+        <v>0.2</v>
       </c>
       <c r="D16">
         <v>0.1</v>
@@ -6233,13 +6183,13 @@
         <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="C17" s="11">
         <v>0.2</v>
       </c>
       <c r="D17">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -6247,13 +6197,13 @@
         <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>156</v>
       </c>
       <c r="C18" s="11">
         <v>0.2</v>
       </c>
       <c r="D18">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -6261,7 +6211,7 @@
         <v>128</v>
       </c>
       <c r="B19" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C19" s="11">
         <v>0.2</v>
@@ -6275,13 +6225,13 @@
         <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>156</v>
+        <v>226</v>
       </c>
       <c r="C20" s="11">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D20">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -6289,176 +6239,148 @@
         <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>157</v>
+        <v>227</v>
       </c>
       <c r="C21" s="11">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D21">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="11"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E25" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G25" s="26">
+        <f>1+$C30</f>
+        <v>1</v>
+      </c>
+      <c r="H25" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="I25" s="2">
+        <v>3</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2020</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G26" s="26">
+        <f>1+$C31</f>
+        <v>1</v>
+      </c>
+      <c r="H26" s="16">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>128</v>
-      </c>
-      <c r="B22" t="s">
-        <v>227</v>
-      </c>
-      <c r="C22" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="D22">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" t="s">
-        <v>228</v>
-      </c>
-      <c r="C23" s="11">
-        <v>0.1</v>
-      </c>
-      <c r="D23">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="11"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E27" s="2">
-        <v>2019</v>
+        <v>155</v>
+      </c>
+      <c r="E27">
+        <v>2026</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>185</v>
       </c>
       <c r="G27" s="26">
-        <f>1+$C32</f>
+        <f>1+$C31</f>
         <v>1</v>
       </c>
       <c r="H27" s="16">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="I27" s="2">
         <v>3</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E28" s="2">
-        <v>2020</v>
+      <c r="D28" s="2"/>
+      <c r="E28">
+        <v>2027</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G28" s="26">
-        <f>1+$C33</f>
-        <v>1</v>
-      </c>
       <c r="H28" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E29">
-        <v>2026</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G29" s="26">
-        <f>1+$C33</f>
-        <v>1</v>
-      </c>
-      <c r="H29" s="16">
-        <v>1</v>
-      </c>
-      <c r="I29" s="2">
-        <v>3</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D30" s="2"/>
-      <c r="E30">
-        <v>2027</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="H30" s="16">
         <v>2</v>
       </c>
     </row>
@@ -6471,7 +6393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -6785,7 +6707,7 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f t="shared" ref="B11:B16" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A26,"MaxGrowth",B26)</f>
+        <f t="shared" ref="B11:B15" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A26,"MaxGrowth",B26)</f>
         <v>UC_RSD_MaxGrowth_Electricity</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -9664,6 +9586,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9874,22 +9811,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9906,21 +9845,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update DH max growth SRV
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E4E75F-EC08-4826-A30C-3BE84FFED2E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1251951-0FF7-4A4E-B860-60DA00F9E62E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="229">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -875,6 +875,9 @@
   </si>
   <si>
     <t>DH_SOL</t>
+  </si>
+  <si>
+    <t>DH_SOL*</t>
   </si>
 </sst>
 </file>
@@ -5815,10 +5818,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43B92B0C-7472-4C75-A119-CE0EE6C8A8E0}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:N28"/>
+  <dimension ref="A2:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5914,7 +5917,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f t="shared" ref="B6:B9" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
+        <f t="shared" ref="B6:B9" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -5930,21 +5933,21 @@
         <v>15</v>
       </c>
       <c r="G6" s="26">
-        <f t="shared" ref="G6:G9" si="1">1+$C14</f>
+        <f t="shared" ref="G6:G9" si="1">1+$C15</f>
         <v>1.02</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
       </c>
       <c r="I6" s="16">
-        <f t="shared" ref="I6:I11" si="2">-D14</f>
+        <f t="shared" ref="I6:I11" si="2">-D15</f>
         <v>-0.1</v>
       </c>
       <c r="J6" s="2">
         <v>5</v>
       </c>
       <c r="K6" s="2" t="str">
-        <f t="shared" ref="K6:K11" si="3">_xlfn.TEXTJOIN(" ",TRUE,A14, "maximum growth rate of",B14)</f>
+        <f t="shared" ref="K6:K11" si="3">_xlfn.TEXTJOIN(" ",TRUE,A15, "maximum growth rate of",B15)</f>
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
@@ -6058,7 +6061,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A19,"MaxGrowth",B19)</f>
         <v>UC_PWR_MaxGrowth_PV</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -6074,7 +6077,7 @@
         <v>15</v>
       </c>
       <c r="G10" s="26">
-        <f>1+$C18</f>
+        <f>1+$C19</f>
         <v>1.2</v>
       </c>
       <c r="H10" s="2">
@@ -6094,7 +6097,7 @@
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A19,"MaxGrowth",B19)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A20,"MaxGrowth",B20)</f>
         <v>UC_PWR_MaxGrowth_CSP</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -6110,7 +6113,7 @@
         <v>15</v>
       </c>
       <c r="G11" s="26">
-        <f>1+$C19</f>
+        <f>1+$C20</f>
         <v>1.2</v>
       </c>
       <c r="H11" s="2">
@@ -6128,26 +6131,48 @@
         <v>PWR maximum growth rate of CSP</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="str">
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
+        <v>UC_PWR_MaxGrowth_DH_SOL</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12">
+        <v>2018</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="26">
+        <f>1+$C22</f>
+        <v>1.05</v>
+      </c>
+      <c r="H12" s="2">
+        <v>1</v>
+      </c>
+      <c r="I12" s="16">
+        <f>-D22</f>
+        <v>-0.1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>6</v>
+      </c>
+      <c r="K12" s="2" t="str">
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A22, "maximum growth rate of",B22)</f>
+        <v>PWR maximum growth rate of DH_SOL</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
         <v>117</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>119</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>128</v>
-      </c>
-      <c r="B14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="50">
-        <v>0.02</v>
-      </c>
-      <c r="D14">
-        <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -6155,13 +6180,13 @@
         <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" s="11">
-        <v>0.2</v>
+        <v>124</v>
+      </c>
+      <c r="C15" s="50">
+        <v>0.02</v>
       </c>
       <c r="D15">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -6169,13 +6194,13 @@
         <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C16" s="11">
         <v>0.2</v>
       </c>
       <c r="D16">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -6183,13 +6208,13 @@
         <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>126</v>
       </c>
       <c r="C17" s="11">
         <v>0.2</v>
       </c>
       <c r="D17">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -6197,7 +6222,7 @@
         <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C18" s="11">
         <v>0.2</v>
@@ -6211,7 +6236,7 @@
         <v>128</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C19" s="11">
         <v>0.2</v>
@@ -6225,13 +6250,13 @@
         <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>226</v>
+        <v>157</v>
       </c>
       <c r="C20" s="11">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D20">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -6239,7 +6264,7 @@
         <v>128</v>
       </c>
       <c r="B21" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C21" s="11">
         <v>0.1</v>
@@ -6249,87 +6274,75 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="11"/>
+      <c r="A22" t="s">
+        <v>128</v>
+      </c>
+      <c r="B22" t="s">
+        <v>227</v>
+      </c>
+      <c r="C22" s="11">
+        <v>0.05</v>
+      </c>
+      <c r="D22">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2" t="s">
+      <c r="C23" s="11"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="4" t="s">
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E25" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G25" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H25" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I25" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="J24" s="4" t="s">
+      <c r="J25" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="E25" s="2">
-        <v>2019</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="G25" s="26">
-        <f>1+$C30</f>
-        <v>1</v>
-      </c>
-      <c r="H25" s="16">
-        <v>0.6</v>
-      </c>
-      <c r="I25" s="2">
-        <v>3</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
         <v>154</v>
       </c>
       <c r="E26" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>185</v>
@@ -6339,48 +6352,74 @@
         <v>1</v>
       </c>
       <c r="H26" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="I26" s="2">
+        <v>3</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>183</v>
+      </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>180</v>
-      </c>
+      <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="E27">
-        <v>2026</v>
+        <v>154</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2020</v>
       </c>
       <c r="F27" s="2" t="s">
         <v>185</v>
       </c>
       <c r="G27" s="26">
-        <f>1+$C31</f>
+        <f>1+$C32</f>
         <v>1</v>
       </c>
       <c r="H27" s="16">
-        <v>1</v>
-      </c>
-      <c r="I27" s="2">
-        <v>3</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>184</v>
-      </c>
+        <v>0.5</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D28" s="2"/>
+      <c r="B28" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="E28">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="F28" s="2" t="s">
         <v>185</v>
       </c>
+      <c r="G28" s="26">
+        <f>1+$C32</f>
+        <v>1</v>
+      </c>
       <c r="H28" s="16">
+        <v>1</v>
+      </c>
+      <c r="I28" s="2">
+        <v>3</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="2"/>
+      <c r="E29">
+        <v>2027</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="H29" s="16">
         <v>2</v>
       </c>
     </row>
@@ -6393,8 +6432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6827,7 +6866,7 @@
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A29,"MaxGrowth",B29)</f>
         <v>UC_RSD_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -7262,7 +7301,7 @@
   <dimension ref="A2:N28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7496,8 +7535,8 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_SRV_MaxGrowth_DistrictHeat</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"*UC",A20,"MaxGrowth",B20)</f>
+        <v>*UC_SRV_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>144</v>
@@ -9586,21 +9625,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9811,24 +9835,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9845,4 +9867,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Account for ELC dis cost
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04B751F4-7FFB-47B1-B040-D233F352CE6A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A0D6C7-723B-4AFD-B9BE-F34057EB76A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -5824,7 +5824,7 @@
   <dimension ref="A2:N30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6153,7 +6153,7 @@
       </c>
       <c r="G12" s="26">
         <f>1+$C22</f>
-        <v>1.05</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H12" s="2">
         <v>1</v>
@@ -6306,7 +6306,7 @@
         <v>226</v>
       </c>
       <c r="C22" s="11">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="D22">
         <v>0.1</v>
@@ -6471,7 +6471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -7339,8 +7339,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7653,7 +7653,7 @@
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
         <v>UC_SRV_MaxGrowth_Electricity</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -9664,6 +9664,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9874,22 +9889,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9906,21 +9923,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
No DH Tax RSD
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DAC265-9D8C-41B7-A733-1331FC66194D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5980210-411A-451A-B740-62369F4275F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -5823,7 +5823,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -6471,8 +6471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7318,11 +7318,10 @@
         <v>2018</v>
       </c>
       <c r="F37">
-        <v>2222</v>
+        <v>0</v>
       </c>
       <c r="G37">
-        <f>F37</f>
-        <v>2222</v>
+        <v>0</v>
       </c>
       <c r="H37" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F18)</f>
@@ -9664,6 +9663,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9874,22 +9888,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9906,21 +9922,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cd90 - DH 15% max g
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18585D04-D584-4537-8903-3EB0D6681D50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D216C5-6657-46F5-AB1A-58EC6C5E1793}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -7462,7 +7462,7 @@
   <dimension ref="A2:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7696,8 +7696,8 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"*UC",A20,"MaxGrowth",B20)</f>
-        <v>*UC_SRV_MaxGrowth_DistrictHeat</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A20,"MaxGrowth",B20)</f>
+        <v>UC_SRV_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>144</v>
@@ -8004,7 +8004,7 @@
         <v>191</v>
       </c>
       <c r="C20" s="50">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="D20">
         <v>0.3</v>
@@ -9785,21 +9785,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10010,24 +9995,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10044,4 +10027,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Over supply SRV AHT
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21F433B-55A2-4A41-ACB7-C23FB9C94FA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29A32CC-C4D2-446F-8CF4-181BA2451246}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="234">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -6592,10 +6592,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
-  <dimension ref="A2:N37"/>
+  <dimension ref="A2:N38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7451,6 +7451,24 @@
         <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDSOL,RSDSOL</v>
       </c>
     </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>217</v>
+      </c>
+      <c r="E38">
+        <v>2018</v>
+      </c>
+      <c r="F38">
+        <v>1E-3</v>
+      </c>
+      <c r="G38">
+        <v>1E-3</v>
+      </c>
+      <c r="H38" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6)</f>
+        <v>RSDAHT,RSDAHT2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7459,10 +7477,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F5F46D0-BFBE-459D-AD94-C3EBC85EC70F}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:N28"/>
+  <dimension ref="A2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D29" sqref="D29:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8113,6 +8131,24 @@
       <c r="H28" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F10)</f>
         <v>SRVBIO,SRVBGS,SRVAHT,SRVAHT2,SRVHET*,SRVGAS</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>217</v>
+      </c>
+      <c r="E29">
+        <v>2018</v>
+      </c>
+      <c r="F29">
+        <v>1E-3</v>
+      </c>
+      <c r="G29">
+        <v>1E-3</v>
+      </c>
+      <c r="H29" t="str">
+        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F8)</f>
+        <v>SRVAHT,SRVAHT2</v>
       </c>
     </row>
   </sheetData>
@@ -9785,21 +9821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10010,24 +10031,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10044,4 +10063,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cd 50 - 10%
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29A32CC-C4D2-446F-8CF4-181BA2451246}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADC6241-966C-45D2-A573-7CE7589AFA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -7480,7 +7480,7 @@
   <dimension ref="A2:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29:H29"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7714,8 +7714,8 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"*UC",A20,"MaxGrowth",B20)</f>
-        <v>*UC_SRV_MaxGrowth_DistrictHeat</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A20,"MaxGrowth",B20)</f>
+        <v>UC_SRV_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>144</v>
@@ -7741,7 +7741,7 @@
       </c>
       <c r="L9" s="16">
         <f t="shared" si="1"/>
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="M9" s="2">
         <v>5</v>
@@ -8025,7 +8025,7 @@
         <v>0.1</v>
       </c>
       <c r="D20">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -9821,6 +9821,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10031,22 +10046,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10063,21 +10080,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Still Service Oversupply of Ambient Heat
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{567AB6B1-8F1D-44E2-AEF8-F5FC8CA9DD59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF6620D-9BB3-4066-BCED-B06D052B86D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -6594,7 +6594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N38"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
@@ -7479,8 +7479,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7714,8 +7714,8 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"*UC",A20,"MaxGrowth",B20)</f>
-        <v>*UC_SRV_MaxGrowth_DistrictHeat</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A20,"MaxGrowth",B20)</f>
+        <v>UC_SRV_MaxGrowth_DistrictHeat</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>144</v>
@@ -8141,10 +8141,10 @@
         <v>2018</v>
       </c>
       <c r="F29">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="G29">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
       <c r="H29" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F8)</f>
@@ -9821,21 +9821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10046,24 +10031,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10080,4 +10063,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Gas Growth Linked to DH
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946649C1-730A-48BD-B096-1A41D501EA45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910AB6F8-FFF2-46DE-9FDA-8FFC4F82A07E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -6595,7 +6595,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6928,27 +6928,27 @@
         <v>15</v>
       </c>
       <c r="J11" s="29">
-        <f t="shared" ref="J11:J15" si="1">1+C26</f>
+        <f>1+C26</f>
         <v>1.3</v>
       </c>
       <c r="K11" s="2">
         <v>1</v>
       </c>
       <c r="L11" s="16">
-        <f t="shared" ref="L11:L16" si="2">-D26</f>
+        <f>-D26</f>
         <v>-0.1</v>
       </c>
       <c r="M11" s="2">
         <v>5</v>
       </c>
       <c r="N11" s="2" t="str">
-        <f t="shared" ref="N11:N15" si="3">_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A26, "maximum growth rate of",B26)</f>
         <v>RSD maximum growth rate of Electricity</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="str">
-        <f t="shared" ref="B12:B15" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A27,"MaxGrowth",B27)</f>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A27,"MaxGrowth",B27)</f>
         <v>UC_RSD_MaxGrowth_Ethanol</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -6968,28 +6968,28 @@
         <v>15</v>
       </c>
       <c r="J12" s="29">
-        <f t="shared" si="1"/>
+        <f>1+C27</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K12" s="2">
         <v>1</v>
       </c>
       <c r="L12" s="16">
-        <f t="shared" si="2"/>
+        <f>-D27</f>
         <v>0</v>
       </c>
       <c r="M12" s="2">
         <v>5</v>
       </c>
       <c r="N12" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A27, "maximum growth rate of",B27)</f>
         <v>RSD maximum growth rate of Ethanol</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>UC_RSD_MaxGrowth_Gas</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A28,"MinDeGrowth",B28)</f>
+        <v>UC_RSD_MinDeGrowth_Gas</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>144</v>
@@ -7005,18 +7005,18 @@
         <v>2021</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="J13" s="29">
         <f>1-C28</f>
-        <v>0.97</v>
+        <v>0.96</v>
       </c>
       <c r="K13" s="2">
         <v>1</v>
       </c>
       <c r="L13" s="16">
-        <f t="shared" si="2"/>
-        <v>-0.1</v>
+        <f t="shared" ref="L13:L16" si="1">-D28</f>
+        <v>0</v>
       </c>
       <c r="M13" s="2">
         <v>5</v>
@@ -7048,27 +7048,27 @@
         <v>15</v>
       </c>
       <c r="J14" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="J14:J15" si="2">1+C29</f>
         <v>1.1000000000000001</v>
       </c>
       <c r="K14" s="2">
         <v>1</v>
       </c>
       <c r="L14" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-0.1</v>
       </c>
       <c r="M14" s="2">
         <v>5</v>
       </c>
       <c r="N14" s="2" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="N14:N15" si="3">_xlfn.TEXTJOIN(" ",TRUE,A29, "maximum growth rate of",B29)</f>
         <v>RSD maximum growth rate of DistrictHeat</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="B13:B15" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A30,"MaxGrowth",B30)</f>
         <v>UC_RSD_MaxGrowth_LPG</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -7088,14 +7088,14 @@
         <v>15</v>
       </c>
       <c r="J15" s="29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.01</v>
       </c>
       <c r="K15" s="2">
         <v>1</v>
       </c>
       <c r="L15" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M15" s="2">
@@ -7135,7 +7135,7 @@
         <v>1</v>
       </c>
       <c r="L16" s="16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-0.1</v>
       </c>
       <c r="M16" s="2">
@@ -7340,10 +7340,10 @@
         <v>192</v>
       </c>
       <c r="C28" s="50">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="D28">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -9821,6 +9821,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10031,22 +10046,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10063,21 +10080,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Coal and HP UC Config
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20564EBA-5CF6-40B6-8659-33308E2CF9A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C94CF3-625A-4F10-BCE6-5E82D1C8C9F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -6595,7 +6595,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6828,8 +6828,8 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>UC_RSD_MaxGrowth_Coal</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A24,"MinDeGrowth",B24)</f>
+        <v>UC_RSD_MinDeGrowth_Coal</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>144</v>
@@ -6848,8 +6848,8 @@
         <v>15</v>
       </c>
       <c r="J9" s="29">
-        <f t="shared" si="1"/>
-        <v>1.01</v>
+        <f>1-C24</f>
+        <v>0.98</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
@@ -6889,7 +6889,7 @@
       </c>
       <c r="J10" s="29">
         <f t="shared" si="1"/>
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="K10" s="2">
         <v>1</v>
@@ -7108,8 +7108,8 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A31,"MaxDEGrowth",B31)</f>
-        <v>UC_RSD_MaxDEGrowth_Kerosene</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A31,"MinDEGrowth",B31)</f>
+        <v>UC_RSD_MinDEGrowth_Kerosene</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>144</v>
@@ -7284,7 +7284,7 @@
         <v>197</v>
       </c>
       <c r="C24" s="50">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -7298,7 +7298,7 @@
         <v>198</v>
       </c>
       <c r="C25" s="50">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -9821,6 +9821,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10031,22 +10046,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10063,21 +10080,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add HLI 2 - Result show small differences.
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C94CF3-625A-4F10-BCE6-5E82D1C8C9F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A66679D-AF4F-4DE7-AF21-DE4F9144AF4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -9821,21 +9821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10046,24 +10031,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10080,4 +10063,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update Max Ker degrowth
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73166E25-0AC8-461A-A359-6252F1A889A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC7CC1C-4C5B-40FB-9683-D3FC082CE3C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -6595,7 +6595,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7022,8 +7022,8 @@
         <v>5</v>
       </c>
       <c r="N13" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A28, "maximum degrowth rate of",B28)</f>
-        <v>RSD maximum degrowth rate of Gas</v>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A28, "minimum degrowth rate of",B28)</f>
+        <v>RSD minimum degrowth rate of Gas</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
@@ -7108,8 +7108,8 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A31,"MinDEGrowth",B31)</f>
-        <v>UC_RSD_MinDEGrowth_Kerosene</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A31,"MaxDEGrowth",B31)</f>
+        <v>UC_RSD_MaxDEGrowth_Kerosene</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>144</v>
@@ -7125,7 +7125,7 @@
         <v>2019</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>15</v>
+        <v>185</v>
       </c>
       <c r="J16" s="29">
         <f>1-C31</f>
@@ -9821,21 +9821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10046,24 +10031,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10080,4 +10063,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update after talk with Olex
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EDF753-2378-42AF-8361-08F94271B79B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B505B93-78AE-4A8B-BDF7-70F09CD11B09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -6595,7 +6595,7 @@
   <dimension ref="A2:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7005,7 +7005,7 @@
         <v>2019</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="J13" s="29">
         <f>1-C28</f>
@@ -7108,8 +7108,8 @@
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A31,"MinDEGrowth",B31)</f>
-        <v>UC_RSD_MinDEGrowth_Kerosene</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A31,"MaxGrowth",B31)</f>
+        <v>UC_RSD_MaxGrowth_Kerosene</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>144</v>
@@ -7125,7 +7125,7 @@
         <v>2019</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>185</v>
+        <v>15</v>
       </c>
       <c r="J16" s="29">
         <f>1-C31</f>
@@ -7142,8 +7142,8 @@
         <v>5</v>
       </c>
       <c r="N16" s="2" t="str">
-        <f>_xlfn.TEXTJOIN(" ",TRUE,A31, "minimum degrowth rate of",B31)</f>
-        <v>RSD minimum degrowth rate of Kerosene</v>
+        <f>_xlfn.TEXTJOIN(" ",TRUE,A31, "max growth rate of",B31)</f>
+        <v>RSD max growth rate of Kerosene</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -9821,21 +9821,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10046,24 +10031,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10080,4 +10063,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UC_HP_X changed HPN-AB to -1 and Max Growth rate increase AHT tax
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F9719A-A33C-4053-AB60-EE3FF15FD7D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA554D0D-3CC2-4BE7-BC11-F910415F63EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -171,7 +171,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="236">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -6598,10 +6598,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
-  <dimension ref="A2:N39"/>
+  <dimension ref="A2:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7235,8 +7235,8 @@
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A34,"MaxGrowth",B34)</f>
-        <v>UC_RSD_MaxGrowth_Immersion Elec</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"*UC",A34,"MaxGrowth",B34)</f>
+        <v>*UC_RSD_MaxGrowth_Immersion Elec</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>144</v>
@@ -7502,30 +7502,12 @@
         <v>2018</v>
       </c>
       <c r="F38">
+        <v>0.01</v>
+      </c>
+      <c r="G38">
         <v>1E-3</v>
       </c>
-      <c r="G38">
-        <v>0</v>
-      </c>
       <c r="H38" t="str">
-        <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F18)</f>
-        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDSOL,RSDSOL</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>217</v>
-      </c>
-      <c r="E39">
-        <v>2018</v>
-      </c>
-      <c r="F39">
-        <v>1E-3</v>
-      </c>
-      <c r="G39">
-        <v>1E-3</v>
-      </c>
-      <c r="H39" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6)</f>
         <v>RSDAHT,RSDAHT2</v>
       </c>
@@ -9882,21 +9864,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10107,24 +10074,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10141,4 +10106,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update after Olex talk - change Output Commodity and setup RSDAHT3
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{476F7FCA-0AF9-409D-825D-392D1DA898E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF25CE6-2000-4F68-8375-3B521C6D4E97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -853,9 +853,6 @@
     <t>SRVAHT,SRVAHT2</t>
   </si>
   <si>
-    <t>RSDAHT,RSDAHT2</t>
-  </si>
-  <si>
     <t>BIOGAS1G,BIOGAS2G</t>
   </si>
   <si>
@@ -902,6 +899,9 @@
   </si>
   <si>
     <t>R-WH*ELC_N1</t>
+  </si>
+  <si>
+    <t>RSDAHT,RSDAHT2,,RSDAHT3</t>
   </si>
 </sst>
 </file>
@@ -5865,7 +5865,7 @@
         <v>2222</v>
       </c>
       <c r="H17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -6198,7 +6198,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E12">
         <v>2018</v>
@@ -6234,7 +6234,7 @@
         <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E13">
         <v>2018</v>
@@ -6270,7 +6270,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E14">
         <v>2018</v>
@@ -6306,7 +6306,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E15">
         <v>2018</v>
@@ -6441,7 +6441,7 @@
         <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C25" s="11">
         <v>0.1</v>
@@ -6455,7 +6455,7 @@
         <v>128</v>
       </c>
       <c r="B26" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C26" s="11">
         <v>0.05</v>
@@ -6469,7 +6469,7 @@
         <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C27" s="11">
         <v>0.1</v>
@@ -6483,7 +6483,7 @@
         <v>128</v>
       </c>
       <c r="B28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C28" s="11">
         <v>0.1</v>
@@ -6638,7 +6638,7 @@
   <dimension ref="A2:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>142</v>
@@ -6792,7 +6792,7 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f t="shared" ref="B6:B11" si="2">_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
+        <f t="shared" ref="B7:B11" si="2">_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
         <v>UC_RSD_MaxGrowth_Biodiesel</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -7080,7 +7080,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="F14" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>142</v>
@@ -7283,7 +7283,7 @@
         <v>207</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H19" s="2">
         <v>2019</v>
@@ -7491,7 +7491,7 @@
         <v>194</v>
       </c>
       <c r="B34" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C34" s="50">
         <v>0.03</v>
@@ -7546,7 +7546,7 @@
       </c>
       <c r="H38" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F19)</f>
-        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDSOL,RSDSOL,RSDELC</v>
+        <v>RSDAHT,RSDAHT2,,RSDAHT3,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET*,RSDLPG,RSDKER,RSDSOL,RSDSOL,RSDELC</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
@@ -7564,7 +7564,7 @@
       </c>
       <c r="H39" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6)</f>
-        <v>RSDAHT,RSDAHT2</v>
+        <v>RSDAHT,RSDAHT2,,RSDAHT3</v>
       </c>
     </row>
   </sheetData>
@@ -7820,7 +7820,7 @@
       </c>
       <c r="D9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>142</v>
@@ -7899,7 +7899,7 @@
       </c>
       <c r="D11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>142</v>
@@ -7939,7 +7939,7 @@
       </c>
       <c r="D12" s="2"/>
       <c r="F12" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>142</v>
@@ -7979,7 +7979,7 @@
       </c>
       <c r="D13" s="2"/>
       <c r="F13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>142</v>
@@ -8019,7 +8019,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="F14" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>142</v>
@@ -9919,6 +9919,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10129,22 +10144,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10161,21 +10178,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Upfate COAL and Peat lower
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90FC3EB5-16FA-46CA-B744-5A5A1E0801BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD76C13-A777-48FC-80A4-7DBA3CC5951C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -6638,7 +6638,7 @@
   <dimension ref="A2:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6872,8 +6872,8 @@
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"*UC",A25,"MinDeGrowth",B25)</f>
-        <v>*UC_RSD_MinDeGrowth_Coal</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A25,"MinDeGrowth",B25)</f>
+        <v>UC_RSD_MinDeGrowth_Coal</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>144</v>
@@ -6893,7 +6893,7 @@
       </c>
       <c r="J9" s="29">
         <f>1-C25</f>
-        <v>0.98</v>
+        <v>0.94</v>
       </c>
       <c r="K9" s="2">
         <v>1</v>
@@ -6933,7 +6933,7 @@
       </c>
       <c r="J10" s="29">
         <f>1-C26</f>
-        <v>0.95</v>
+        <v>0.94</v>
       </c>
       <c r="K10" s="2">
         <v>1</v>
@@ -7368,7 +7368,7 @@
         <v>197</v>
       </c>
       <c r="C25" s="50">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -7382,7 +7382,7 @@
         <v>198</v>
       </c>
       <c r="C26" s="50">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -9919,6 +9919,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10129,22 +10144,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10161,21 +10178,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Edit - ELC, AHT, and BDL
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{534B47EA-F83C-4A56-A39D-7C7F497700C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3657F5A-A9D6-4FE8-8D41-1BB84E348BA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="237">
   <si>
     <t>~UC_Sets: T_E:</t>
   </si>
@@ -6641,7 +6641,7 @@
   <dimension ref="A2:N39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6795,8 +6795,8 @@
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"*UC",A23,"MaxGrowth",B23)</f>
-        <v>*UC_RSD_MaxGrowth_Biodiesel</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A23,"MaxGrowth",B23)</f>
+        <v>UC_RSD_MaxGrowth_Biodiesel</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>144</v>
@@ -6816,7 +6816,7 @@
       </c>
       <c r="J7" s="29">
         <f t="shared" si="0"/>
-        <v>1.03</v>
+        <v>1.05</v>
       </c>
       <c r="K7" s="2">
         <v>1</v>
@@ -6961,12 +6961,14 @@
       <c r="C11" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>236</v>
+      </c>
       <c r="F11" t="s">
         <v>207</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>236</v>
+        <v>142</v>
       </c>
       <c r="H11" s="2">
         <v>2019</v>
@@ -7343,7 +7345,7 @@
         <v>196</v>
       </c>
       <c r="C23" s="50">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="D23">
         <v>0.2</v>
@@ -9922,6 +9924,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10132,22 +10149,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10164,21 +10183,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
No AMB UC , UPDATE HP COST
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24F7C6C-EE88-4A78-9FF8-ED8649F15685}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21BD88FD-B7ED-4931-88CD-089F604CD197}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4350" yWindow="2340" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -6637,8 +6637,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6752,8 +6752,8 @@
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
-        <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
-        <v>UC_RSD_MaxGrowth_AmbientHeat</v>
+        <f>_xlfn.TEXTJOIN("_",TRUE,"*UC",A22,"MaxGrowth",B22)</f>
+        <v>*UC_RSD_MaxGrowth_AmbientHeat</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>144</v>
@@ -9919,6 +9919,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -10129,22 +10144,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10161,21 +10178,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated LED scenario file
LED scenario file have been updated to new structure in the residential buildings,
CB_400MT scenario file updated using TOTCO2 commodity
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\times-ireland-model-main\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\times-ireland-model-VAv2\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{973492E1-4AE2-46CF-98C8-EF4591B62932}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EEB40D7-E84B-4F9B-8964-C11C52566A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -1199,7 +1199,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1303,10 +1303,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2005,24 +2001,24 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:D20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26:D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="21.6640625" customWidth="1"/>
-    <col min="5" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
-    <col min="8" max="10" width="8.109375" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1"/>
-    <col min="12" max="12" width="8.109375" customWidth="1"/>
+    <col min="1" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="6" width="14.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="10" width="8.140625" customWidth="1"/>
+    <col min="11" max="11" width="9.7109375" customWidth="1"/>
+    <col min="12" max="12" width="8.140625" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="14" max="14" width="11.44140625" customWidth="1"/>
-    <col min="15" max="15" width="13.44140625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="30"/>
       <c r="B1" s="30"/>
       <c r="C1" s="30"/>
@@ -2050,7 +2046,7 @@
       <c r="Y1" s="31"/>
       <c r="Z1" s="31"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="30"/>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -2078,7 +2074,7 @@
       <c r="Y2" s="31"/>
       <c r="Z2" s="31"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="30"/>
       <c r="B3" s="30"/>
       <c r="C3" s="30"/>
@@ -2106,7 +2102,7 @@
       <c r="Y3" s="31"/>
       <c r="Z3" s="31"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="30"/>
       <c r="B4" s="30"/>
       <c r="C4" s="30"/>
@@ -2134,7 +2130,7 @@
       <c r="Y4" s="31"/>
       <c r="Z4" s="31"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="30"/>
       <c r="B5" s="30"/>
       <c r="C5" s="30"/>
@@ -2162,7 +2158,7 @@
       <c r="Y5" s="31"/>
       <c r="Z5" s="31"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="30"/>
       <c r="B6" s="30"/>
       <c r="C6" s="30"/>
@@ -2190,7 +2186,7 @@
       <c r="Y6" s="31"/>
       <c r="Z6" s="31"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
       <c r="B7" s="30"/>
       <c r="C7" s="30"/>
@@ -2218,7 +2214,7 @@
       <c r="Y7" s="31"/>
       <c r="Z7" s="31"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="30"/>
       <c r="B8" s="30"/>
       <c r="C8" s="30"/>
@@ -2246,7 +2242,7 @@
       <c r="Y8" s="31"/>
       <c r="Z8" s="31"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="30"/>
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
@@ -2274,7 +2270,7 @@
       <c r="Y9" s="31"/>
       <c r="Z9" s="31"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="30"/>
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
@@ -2302,7 +2298,7 @@
       <c r="Y10" s="31"/>
       <c r="Z10" s="31"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="30"/>
       <c r="B11" s="30"/>
       <c r="C11" s="30"/>
@@ -2330,7 +2326,7 @@
       <c r="Y11" s="31"/>
       <c r="Z11" s="31"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="30"/>
       <c r="B12" s="30"/>
       <c r="C12" s="30"/>
@@ -2358,7 +2354,7 @@
       <c r="Y12" s="31"/>
       <c r="Z12" s="31"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="30"/>
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
@@ -2386,7 +2382,7 @@
       <c r="Y13" s="31"/>
       <c r="Z13" s="31"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="30"/>
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
@@ -2414,7 +2410,7 @@
       <c r="Y14" s="31"/>
       <c r="Z14" s="31"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
       <c r="B15" s="30"/>
       <c r="C15" s="30"/>
@@ -2442,7 +2438,7 @@
       <c r="Y15" s="31"/>
       <c r="Z15" s="31"/>
     </row>
-    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="53" t="s">
         <v>161</v>
       </c>
@@ -2472,7 +2468,7 @@
       <c r="Y16" s="31"/>
       <c r="Z16" s="31"/>
     </row>
-    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
       <c r="B17" s="34"/>
       <c r="C17" s="34"/>
@@ -2500,7 +2496,7 @@
       <c r="Y17" s="31"/>
       <c r="Z17" s="31"/>
     </row>
-    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
       <c r="B18" s="34"/>
       <c r="C18" s="34"/>
@@ -2528,7 +2524,7 @@
       <c r="Y18" s="31"/>
       <c r="Z18" s="31"/>
     </row>
-    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
         <v>162</v>
       </c>
@@ -2560,7 +2556,7 @@
       <c r="Y19" s="31"/>
       <c r="Z19" s="31"/>
     </row>
-    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
         <v>163</v>
       </c>
@@ -2592,7 +2588,7 @@
       <c r="Y20" s="31"/>
       <c r="Z20" s="31"/>
     </row>
-    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
         <v>164</v>
       </c>
@@ -2624,7 +2620,7 @@
       <c r="Y21" s="31"/>
       <c r="Z21" s="31"/>
     </row>
-    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37"/>
       <c r="B22" s="40"/>
       <c r="C22" s="40"/>
@@ -2652,7 +2648,7 @@
       <c r="Y22" s="31"/>
       <c r="Z22" s="31"/>
     </row>
-    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
         <v>165</v>
       </c>
@@ -2684,7 +2680,7 @@
       <c r="Y23" s="31"/>
       <c r="Z23" s="31"/>
     </row>
-    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="37"/>
       <c r="B24" s="52" t="s">
         <v>174</v>
@@ -2714,7 +2710,7 @@
       <c r="Y24" s="31"/>
       <c r="Z24" s="31"/>
     </row>
-    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37"/>
       <c r="B25" s="40" t="s">
         <v>175</v>
@@ -2744,7 +2740,7 @@
       <c r="Y25" s="31"/>
       <c r="Z25" s="31"/>
     </row>
-    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>166</v>
       </c>
@@ -2776,7 +2772,7 @@
       <c r="Y26" s="31"/>
       <c r="Z26" s="31"/>
     </row>
-    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37"/>
       <c r="B27" s="40"/>
       <c r="C27" s="40"/>
@@ -2804,7 +2800,7 @@
       <c r="Y27" s="31"/>
       <c r="Z27" s="31"/>
     </row>
-    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37"/>
       <c r="B28" s="40"/>
       <c r="C28" s="40"/>
@@ -2832,7 +2828,7 @@
       <c r="Y28" s="31"/>
       <c r="Z28" s="31"/>
     </row>
-    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
         <v>167</v>
       </c>
@@ -2864,7 +2860,7 @@
       <c r="Y29" s="31"/>
       <c r="Z29" s="31"/>
     </row>
-    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
         <v>168</v>
       </c>
@@ -2896,7 +2892,7 @@
       <c r="Y30" s="31"/>
       <c r="Z30" s="31"/>
     </row>
-    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="37" t="s">
         <v>170</v>
       </c>
@@ -2928,7 +2924,7 @@
       <c r="Y31" s="31"/>
       <c r="Z31" s="31"/>
     </row>
-    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="43"/>
       <c r="B32" s="44" t="s">
         <v>172</v>
@@ -2958,7 +2954,7 @@
       <c r="Y32" s="31"/>
       <c r="Z32" s="31"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A33" s="30"/>
       <c r="B33" s="30"/>
       <c r="C33" s="30"/>
@@ -2986,7 +2982,7 @@
       <c r="Y33" s="31"/>
       <c r="Z33" s="31"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A34" s="30"/>
       <c r="B34" s="30"/>
       <c r="C34" s="30"/>
@@ -3014,7 +3010,7 @@
       <c r="Y34" s="31"/>
       <c r="Z34" s="31"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A35" s="30"/>
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
@@ -3042,7 +3038,7 @@
       <c r="Y35" s="31"/>
       <c r="Z35" s="31"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A36" s="30"/>
       <c r="B36" s="30"/>
       <c r="C36" s="30"/>
@@ -3070,7 +3066,7 @@
       <c r="Y36" s="31"/>
       <c r="Z36" s="31"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A37" s="30"/>
       <c r="B37" s="30"/>
       <c r="C37" s="30"/>
@@ -3098,7 +3094,7 @@
       <c r="Y37" s="31"/>
       <c r="Z37" s="31"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
       <c r="B38" s="30"/>
       <c r="C38" s="30"/>
@@ -3126,7 +3122,7 @@
       <c r="Y38" s="31"/>
       <c r="Z38" s="31"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
       <c r="B39" s="30"/>
       <c r="C39" s="30"/>
@@ -3154,7 +3150,7 @@
       <c r="Y39" s="31"/>
       <c r="Z39" s="31"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A40" s="30"/>
       <c r="B40" s="30"/>
       <c r="C40" s="30"/>
@@ -3182,7 +3178,7 @@
       <c r="Y40" s="31"/>
       <c r="Z40" s="31"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A41" s="30"/>
       <c r="B41" s="30"/>
       <c r="C41" s="30"/>
@@ -3210,7 +3206,7 @@
       <c r="Y41" s="31"/>
       <c r="Z41" s="31"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="30"/>
       <c r="C42" s="30"/>
@@ -3238,7 +3234,7 @@
       <c r="Y42" s="31"/>
       <c r="Z42" s="31"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A43" s="31"/>
       <c r="B43" s="31"/>
       <c r="C43" s="31"/>
@@ -3266,7 +3262,7 @@
       <c r="Y43" s="31"/>
       <c r="Z43" s="31"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A44" s="31"/>
       <c r="B44" s="31"/>
       <c r="C44" s="31"/>
@@ -3294,7 +3290,7 @@
       <c r="Y44" s="31"/>
       <c r="Z44" s="31"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A45" s="31"/>
       <c r="B45" s="31"/>
       <c r="C45" s="31"/>
@@ -3322,7 +3318,7 @@
       <c r="Y45" s="31"/>
       <c r="Z45" s="31"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A46" s="31"/>
       <c r="B46" s="31"/>
       <c r="C46" s="31"/>
@@ -3350,7 +3346,7 @@
       <c r="Y46" s="31"/>
       <c r="Z46" s="31"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A47" s="31"/>
       <c r="B47" s="31"/>
       <c r="C47" s="31"/>
@@ -3378,7 +3374,7 @@
       <c r="Y47" s="31"/>
       <c r="Z47" s="31"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A48" s="31"/>
       <c r="B48" s="31"/>
       <c r="C48" s="31"/>
@@ -3406,7 +3402,7 @@
       <c r="Y48" s="31"/>
       <c r="Z48" s="31"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="31"/>
       <c r="C49" s="31"/>
@@ -3434,7 +3430,7 @@
       <c r="Y49" s="31"/>
       <c r="Z49" s="31"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
       <c r="B50" s="31"/>
       <c r="C50" s="31"/>
@@ -3462,7 +3458,7 @@
       <c r="Y50" s="31"/>
       <c r="Z50" s="31"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A51" s="31"/>
       <c r="B51" s="31"/>
       <c r="C51" s="31"/>
@@ -3490,7 +3486,7 @@
       <c r="Y51" s="31"/>
       <c r="Z51" s="31"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A52" s="31"/>
       <c r="B52" s="31"/>
       <c r="C52" s="31"/>
@@ -3518,7 +3514,7 @@
       <c r="Y52" s="31"/>
       <c r="Z52" s="31"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A53" s="31"/>
       <c r="B53" s="31"/>
       <c r="C53" s="31"/>
@@ -3546,7 +3542,7 @@
       <c r="Y53" s="31"/>
       <c r="Z53" s="31"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A54" s="31"/>
       <c r="B54" s="31"/>
       <c r="C54" s="31"/>
@@ -3574,7 +3570,7 @@
       <c r="Y54" s="31"/>
       <c r="Z54" s="31"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A55" s="31"/>
       <c r="B55" s="31"/>
       <c r="C55" s="31"/>
@@ -3602,7 +3598,7 @@
       <c r="Y55" s="31"/>
       <c r="Z55" s="31"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A56" s="31"/>
       <c r="B56" s="31"/>
       <c r="C56" s="31"/>
@@ -3630,7 +3626,7 @@
       <c r="Y56" s="31"/>
       <c r="Z56" s="31"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A57" s="31"/>
       <c r="B57" s="31"/>
       <c r="C57" s="31"/>
@@ -3658,7 +3654,7 @@
       <c r="Y57" s="31"/>
       <c r="Z57" s="31"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A58" s="31"/>
       <c r="B58" s="31"/>
       <c r="C58" s="31"/>
@@ -3686,7 +3682,7 @@
       <c r="Y58" s="31"/>
       <c r="Z58" s="31"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A59" s="31"/>
       <c r="B59" s="31"/>
       <c r="C59" s="31"/>
@@ -3714,7 +3710,7 @@
       <c r="Y59" s="31"/>
       <c r="Z59" s="31"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A60" s="31"/>
       <c r="B60" s="31"/>
       <c r="C60" s="31"/>
@@ -3742,7 +3738,7 @@
       <c r="Y60" s="31"/>
       <c r="Z60" s="31"/>
     </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A61" s="31"/>
       <c r="B61" s="31"/>
       <c r="C61" s="31"/>
@@ -3770,7 +3766,7 @@
       <c r="Y61" s="31"/>
       <c r="Z61" s="31"/>
     </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A62" s="31"/>
       <c r="B62" s="31"/>
       <c r="C62" s="31"/>
@@ -3798,7 +3794,7 @@
       <c r="Y62" s="31"/>
       <c r="Z62" s="31"/>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A63" s="31"/>
       <c r="B63" s="31"/>
       <c r="C63" s="31"/>
@@ -3826,7 +3822,7 @@
       <c r="Y63" s="31"/>
       <c r="Z63" s="31"/>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A64" s="31"/>
       <c r="B64" s="31"/>
       <c r="C64" s="31"/>
@@ -3854,7 +3850,7 @@
       <c r="Y64" s="31"/>
       <c r="Z64" s="31"/>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A65" s="31"/>
       <c r="B65" s="31"/>
       <c r="C65" s="31"/>
@@ -3882,7 +3878,7 @@
       <c r="Y65" s="31"/>
       <c r="Z65" s="31"/>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A66" s="31"/>
       <c r="B66" s="31"/>
       <c r="C66" s="31"/>
@@ -3910,7 +3906,7 @@
       <c r="Y66" s="31"/>
       <c r="Z66" s="31"/>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A67" s="31"/>
       <c r="B67" s="31"/>
       <c r="C67" s="31"/>
@@ -3938,7 +3934,7 @@
       <c r="Y67" s="31"/>
       <c r="Z67" s="31"/>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A68" s="31"/>
       <c r="B68" s="31"/>
       <c r="C68" s="31"/>
@@ -3966,7 +3962,7 @@
       <c r="Y68" s="31"/>
       <c r="Z68" s="31"/>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A69" s="31"/>
       <c r="B69" s="31"/>
       <c r="C69" s="31"/>
@@ -3994,7 +3990,7 @@
       <c r="Y69" s="31"/>
       <c r="Z69" s="31"/>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A70" s="31"/>
       <c r="B70" s="31"/>
       <c r="C70" s="31"/>
@@ -4022,7 +4018,7 @@
       <c r="Y70" s="31"/>
       <c r="Z70" s="31"/>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A71" s="31"/>
       <c r="B71" s="31"/>
       <c r="C71" s="31"/>
@@ -4050,7 +4046,7 @@
       <c r="Y71" s="31"/>
       <c r="Z71" s="31"/>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A72" s="31"/>
       <c r="B72" s="31"/>
       <c r="C72" s="31"/>
@@ -4078,7 +4074,7 @@
       <c r="Y72" s="31"/>
       <c r="Z72" s="31"/>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A73" s="31"/>
       <c r="B73" s="31"/>
       <c r="C73" s="31"/>
@@ -4106,7 +4102,7 @@
       <c r="Y73" s="31"/>
       <c r="Z73" s="31"/>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A74" s="31"/>
       <c r="B74" s="31"/>
       <c r="C74" s="31"/>
@@ -4134,7 +4130,7 @@
       <c r="Y74" s="31"/>
       <c r="Z74" s="31"/>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A75" s="31"/>
       <c r="B75" s="31"/>
       <c r="C75" s="31"/>
@@ -4162,7 +4158,7 @@
       <c r="Y75" s="31"/>
       <c r="Z75" s="31"/>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A76" s="31"/>
       <c r="B76" s="31"/>
       <c r="C76" s="31"/>
@@ -4190,7 +4186,7 @@
       <c r="Y76" s="31"/>
       <c r="Z76" s="31"/>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A77" s="31"/>
       <c r="B77" s="31"/>
       <c r="C77" s="31"/>
@@ -4218,7 +4214,7 @@
       <c r="Y77" s="31"/>
       <c r="Z77" s="31"/>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A78" s="31"/>
       <c r="B78" s="31"/>
       <c r="C78" s="31"/>
@@ -4246,7 +4242,7 @@
       <c r="Y78" s="31"/>
       <c r="Z78" s="31"/>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A79" s="31"/>
       <c r="B79" s="31"/>
       <c r="C79" s="31"/>
@@ -4274,7 +4270,7 @@
       <c r="Y79" s="31"/>
       <c r="Z79" s="31"/>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A80" s="31"/>
       <c r="B80" s="31"/>
       <c r="C80" s="31"/>
@@ -4302,7 +4298,7 @@
       <c r="Y80" s="31"/>
       <c r="Z80" s="31"/>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A81" s="31"/>
       <c r="B81" s="31"/>
       <c r="C81" s="31"/>
@@ -4330,7 +4326,7 @@
       <c r="Y81" s="31"/>
       <c r="Z81" s="31"/>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A82" s="31"/>
       <c r="B82" s="31"/>
       <c r="C82" s="31"/>
@@ -4358,7 +4354,7 @@
       <c r="Y82" s="31"/>
       <c r="Z82" s="31"/>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A83" s="31"/>
       <c r="B83" s="31"/>
       <c r="C83" s="31"/>
@@ -4386,7 +4382,7 @@
       <c r="Y83" s="31"/>
       <c r="Z83" s="31"/>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A84" s="31"/>
       <c r="B84" s="31"/>
       <c r="C84" s="31"/>
@@ -4414,7 +4410,7 @@
       <c r="Y84" s="31"/>
       <c r="Z84" s="31"/>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A85" s="31"/>
       <c r="B85" s="31"/>
       <c r="C85" s="31"/>
@@ -4442,7 +4438,7 @@
       <c r="Y85" s="31"/>
       <c r="Z85" s="31"/>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A86" s="31"/>
       <c r="B86" s="31"/>
       <c r="C86" s="31"/>
@@ -4470,7 +4466,7 @@
       <c r="Y86" s="31"/>
       <c r="Z86" s="31"/>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A87" s="31"/>
       <c r="B87" s="31"/>
       <c r="C87" s="31"/>
@@ -4498,7 +4494,7 @@
       <c r="Y87" s="31"/>
       <c r="Z87" s="31"/>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A88" s="31"/>
       <c r="B88" s="31"/>
       <c r="C88" s="31"/>
@@ -4526,7 +4522,7 @@
       <c r="Y88" s="31"/>
       <c r="Z88" s="31"/>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A89" s="31"/>
       <c r="B89" s="31"/>
       <c r="C89" s="31"/>
@@ -4554,7 +4550,7 @@
       <c r="Y89" s="31"/>
       <c r="Z89" s="31"/>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A90" s="31"/>
       <c r="B90" s="31"/>
       <c r="C90" s="31"/>
@@ -4582,7 +4578,7 @@
       <c r="Y90" s="31"/>
       <c r="Z90" s="31"/>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A91" s="31"/>
       <c r="B91" s="31"/>
       <c r="C91" s="31"/>
@@ -4610,7 +4606,7 @@
       <c r="Y91" s="31"/>
       <c r="Z91" s="31"/>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A92" s="31"/>
       <c r="B92" s="31"/>
       <c r="C92" s="31"/>
@@ -4638,7 +4634,7 @@
       <c r="Y92" s="31"/>
       <c r="Z92" s="31"/>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A93" s="31"/>
       <c r="B93" s="31"/>
       <c r="C93" s="31"/>
@@ -4666,7 +4662,7 @@
       <c r="Y93" s="31"/>
       <c r="Z93" s="31"/>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A94" s="31"/>
       <c r="B94" s="31"/>
       <c r="C94" s="31"/>
@@ -4694,7 +4690,7 @@
       <c r="Y94" s="31"/>
       <c r="Z94" s="31"/>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A95" s="31"/>
       <c r="B95" s="31"/>
       <c r="C95" s="31"/>
@@ -4722,7 +4718,7 @@
       <c r="Y95" s="31"/>
       <c r="Z95" s="31"/>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A96" s="31"/>
       <c r="B96" s="31"/>
       <c r="C96" s="31"/>
@@ -4750,7 +4746,7 @@
       <c r="Y96" s="31"/>
       <c r="Z96" s="31"/>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A97" s="31"/>
       <c r="B97" s="31"/>
       <c r="C97" s="31"/>
@@ -4778,7 +4774,7 @@
       <c r="Y97" s="31"/>
       <c r="Z97" s="31"/>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A98" s="31"/>
       <c r="B98" s="31"/>
       <c r="C98" s="31"/>
@@ -4806,7 +4802,7 @@
       <c r="Y98" s="31"/>
       <c r="Z98" s="31"/>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A99" s="31"/>
       <c r="B99" s="31"/>
       <c r="C99" s="31"/>
@@ -4864,39 +4860,39 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" customWidth="1"/>
-    <col min="3" max="3" width="3.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.5546875" customWidth="1"/>
-    <col min="25" max="25" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+    <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.5703125" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="6" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="C3" s="20" t="str" cm="1">
         <f t="array" ref="C3">IF(LEFT(INDEX(C5:C7,$A$4),1)&lt;&gt;"*",INDEX(C5:C7,$A$4),"")</f>
         <v>IE</v>
@@ -5010,12 +5006,12 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -5130,7 +5126,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -5247,7 +5243,7 @@
         <v>*IE-MN</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -5364,7 +5360,7 @@
         <v>IE-MN</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="22" t="s">
         <v>56</v>
       </c>
@@ -5372,7 +5368,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>58</v>
       </c>
@@ -5380,7 +5376,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="24" t="s">
         <v>60</v>
       </c>
@@ -5388,7 +5384,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="24" t="s">
         <v>62</v>
       </c>
@@ -5396,7 +5392,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>64</v>
       </c>
@@ -5404,7 +5400,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>66</v>
       </c>
@@ -5412,7 +5408,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="24" t="s">
         <v>68</v>
       </c>
@@ -5420,7 +5416,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>70</v>
       </c>
@@ -5428,7 +5424,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>72</v>
       </c>
@@ -5436,7 +5432,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>74</v>
       </c>
@@ -5444,7 +5440,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>76</v>
       </c>
@@ -5452,7 +5448,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>78</v>
       </c>
@@ -5460,7 +5456,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>80</v>
       </c>
@@ -5468,7 +5464,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>82</v>
       </c>
@@ -5476,7 +5472,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>84</v>
       </c>
@@ -5484,7 +5480,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
         <v>86</v>
       </c>
@@ -5492,7 +5488,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>88</v>
       </c>
@@ -5500,7 +5496,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>90</v>
       </c>
@@ -5508,7 +5504,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>92</v>
       </c>
@@ -5516,7 +5512,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>94</v>
       </c>
@@ -5524,7 +5520,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
         <v>96</v>
       </c>
@@ -5532,7 +5528,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>98</v>
       </c>
@@ -5540,7 +5536,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>100</v>
       </c>
@@ -5548,7 +5544,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
         <v>102</v>
       </c>
@@ -5556,7 +5552,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="24" t="s">
         <v>104</v>
       </c>
@@ -5564,7 +5560,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
         <v>106</v>
       </c>
@@ -5572,7 +5568,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
         <v>108</v>
       </c>
@@ -5580,7 +5576,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>110</v>
       </c>
@@ -5628,17 +5624,17 @@
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -5656,7 +5652,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -5673,7 +5669,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -5687,7 +5683,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -5719,7 +5715,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A12,"MaxGrowth",B12)</f>
         <v>UC_SUP_MaxGrowth_BIOGAS</v>
@@ -5755,7 +5751,7 @@
         <v>SUP maximum growth rate of BIOGAS</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
         <f t="shared" ref="B7:B8" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A13,"MaxGrowth",B13)</f>
         <v>UC_SUP_MaxGrowth_BIODST</v>
@@ -5791,7 +5787,7 @@
         <v>SUP maximum growth rate of BIODST</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
         <f t="shared" si="4"/>
         <v>UC_SUP_MaxGrowth_BIOETH</v>
@@ -5827,7 +5823,7 @@
         <v>SUP maximum growth rate of BIOETH</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -5839,7 +5835,7 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>117</v>
       </c>
@@ -5847,7 +5843,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>186</v>
       </c>
@@ -5861,7 +5857,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>186</v>
       </c>
@@ -5875,7 +5871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>186</v>
       </c>
@@ -5889,18 +5885,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
       <c r="F15" s="2"/>
       <c r="H15" s="16"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="45" t="s">
         <v>215</v>
       </c>
       <c r="H17" s="46"/>
     </row>
-    <row r="18" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="47" t="s">
         <v>216</v>
       </c>
@@ -5925,7 +5921,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
         <v>219</v>
       </c>
@@ -5953,21 +5949,21 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A2:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="33.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -5985,7 +5981,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -6002,7 +5998,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -6016,7 +6012,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -6048,7 +6044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6:B9" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
         <v>UC_PWR_MaxGrowth_CCS</v>
@@ -6084,7 +6080,7 @@
         <v>PWR maximum growth rate of CCS</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_Wave</v>
@@ -6120,7 +6116,7 @@
         <v>PWR maximum growth rate of Wave</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_Tidal</v>
@@ -6156,7 +6152,7 @@
         <v>PWR maximum growth rate of Tidal</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_PWR_MaxGrowth_H2GT</v>
@@ -6192,7 +6188,7 @@
         <v>PWR maximum growth rate of H2GT</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
         <f t="shared" ref="B10:B11" si="4">_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_PWR_MaxGrowth_PV</v>
@@ -6228,7 +6224,7 @@
         <v>PWR maximum growth rate of PV</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
         <f t="shared" si="4"/>
         <v>UC_PWR_MaxGrowth_CSP</v>
@@ -6264,7 +6260,7 @@
         <v>PWR maximum growth rate of CSP</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>117</v>
       </c>
@@ -6272,7 +6268,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>128</v>
       </c>
@@ -6286,7 +6282,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>128</v>
       </c>
@@ -6300,7 +6296,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -6314,7 +6310,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>128</v>
       </c>
@@ -6328,7 +6324,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>128</v>
       </c>
@@ -6342,7 +6338,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>128</v>
       </c>
@@ -6356,7 +6352,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -6370,7 +6366,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>1</v>
       </c>
@@ -6399,7 +6395,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>179</v>
       </c>
@@ -6427,7 +6423,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
@@ -6449,7 +6445,7 @@
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
@@ -6470,24 +6466,24 @@
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="57" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57" t="s">
+      <c r="C27" s="2"/>
+      <c r="D27" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E27" s="56">
+      <c r="E27">
         <v>2026</v>
       </c>
-      <c r="F27" s="57" t="s">
+      <c r="F27" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G27" s="59">
+      <c r="G27" s="26">
         <v>1</v>
       </c>
-      <c r="H27" s="58">
+      <c r="H27" s="16">
         <v>0.8</v>
       </c>
       <c r="I27" s="2">
@@ -6497,79 +6493,71 @@
         <v>184</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="57" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D28" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E28" s="56">
+      <c r="E28">
         <v>2027</v>
       </c>
-      <c r="F28" s="57" t="s">
+      <c r="F28" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G28" s="59">
+      <c r="G28" s="26">
         <v>1</v>
       </c>
-      <c r="H28" s="58">
+      <c r="H28" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="56"/>
-      <c r="C29" s="56"/>
-      <c r="D29" s="57" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D29" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E29" s="56">
+      <c r="E29">
         <v>2028</v>
       </c>
-      <c r="F29" s="57" t="s">
+      <c r="F29" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G29" s="59">
+      <c r="G29" s="26">
         <v>1</v>
       </c>
-      <c r="H29" s="58">
+      <c r="H29" s="16">
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="57" t="s">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D30" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E30" s="56">
+      <c r="E30">
         <v>2029</v>
       </c>
-      <c r="F30" s="57" t="s">
+      <c r="F30" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G30" s="59">
+      <c r="G30" s="26">
         <v>1</v>
       </c>
-      <c r="H30" s="58">
+      <c r="H30" s="16">
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="57" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D31" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E31" s="56">
+      <c r="E31">
         <v>2030</v>
       </c>
-      <c r="F31" s="57" t="s">
+      <c r="F31" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G31" s="59">
+      <c r="G31" s="26">
         <v>1</v>
       </c>
-      <c r="H31" s="58">
+      <c r="H31" s="16">
         <v>2</v>
       </c>
     </row>
@@ -6583,25 +6571,25 @@
   <dimension ref="A2:N37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -6619,7 +6607,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -6636,7 +6624,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -6653,7 +6641,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -6694,7 +6682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A21,"MaxGrowth",B21)</f>
         <v>UC_RSD_MaxGrowth_AmbientHeat</v>
@@ -6734,7 +6722,7 @@
         <v>RSD maximum growth rate of AmbientHeat</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
         <f t="shared" ref="B7:B17" si="0">_xlfn.TEXTJOIN("_",TRUE,"UC",A22,"MaxGrowth",B22)</f>
         <v>UC_RSD_MaxGrowth_Biodiesel</v>
@@ -6774,7 +6762,7 @@
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Biomass</v>
@@ -6814,7 +6802,7 @@
         <v>RSD maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Coal</v>
@@ -6854,7 +6842,7 @@
         <v>RSD maximum growth rate of Coal</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Peat</v>
@@ -6894,7 +6882,7 @@
         <v>RSD maximum growth rate of Peat</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Electricity</v>
@@ -6934,7 +6922,7 @@
         <v>RSD maximum growth rate of Electricity</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Ethanol</v>
@@ -6974,7 +6962,7 @@
         <v>RSD maximum growth rate of Ethanol</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Gas</v>
@@ -7014,7 +7002,7 @@
         <v>RSD maximum growth rate of Gas</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_DistrictHeat</v>
@@ -7054,7 +7042,7 @@
         <v>RSD maximum growth rate of DistrictHeat</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_LPG</v>
@@ -7094,7 +7082,7 @@
         <v>RSD maximum growth rate of LPG</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Kerosene</v>
@@ -7134,7 +7122,7 @@
         <v>RSD maximum growth rate of Kerosene</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC_RSD_MaxGrowth_Solar</v>
@@ -7174,7 +7162,7 @@
         <v>RSD maximum growth rate of Solar</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -7187,7 +7175,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
         <v>117</v>
       </c>
@@ -7195,7 +7183,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>195</v>
       </c>
@@ -7209,7 +7197,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>195</v>
       </c>
@@ -7223,7 +7211,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>195</v>
       </c>
@@ -7237,7 +7225,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>195</v>
       </c>
@@ -7251,7 +7239,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>195</v>
       </c>
@@ -7265,7 +7253,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>195</v>
       </c>
@@ -7279,7 +7267,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>195</v>
       </c>
@@ -7293,7 +7281,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>195</v>
       </c>
@@ -7307,7 +7295,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>195</v>
       </c>
@@ -7321,7 +7309,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>195</v>
       </c>
@@ -7335,7 +7323,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>195</v>
       </c>
@@ -7349,7 +7337,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>195</v>
       </c>
@@ -7363,13 +7351,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="45" t="s">
         <v>215</v>
       </c>
       <c r="H35" s="46"/>
     </row>
-    <row r="36" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="47" t="s">
         <v>216</v>
       </c>
@@ -7394,7 +7382,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>219</v>
       </c>
@@ -7423,27 +7411,27 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A2:N24"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -7461,7 +7449,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7478,7 +7466,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7495,7 +7483,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -7536,7 +7524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A14,"MaxGrowth",B14)</f>
         <v>UC_SRV_MaxGrowth_Biomass</v>
@@ -7576,7 +7564,7 @@
         <v>SRV maximum growth rate of Biomass</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A15,"MaxGrowth",B15)</f>
         <v>UC_SRV_MaxGrowth_Biogas</v>
@@ -7616,7 +7604,7 @@
         <v>SRV maximum growth rate of Biogas</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A16,"MaxGrowth",B16)</f>
         <v>UC_SRV_MaxGrowth_AmbientHeat</v>
@@ -7646,7 +7634,7 @@
       </c>
       <c r="L8" s="16">
         <f>-D16</f>
-        <v>-0.3</v>
+        <v>-0.8</v>
       </c>
       <c r="M8" s="2">
         <v>5</v>
@@ -7656,7 +7644,7 @@
         <v>SRV maximum growth rate of AmbientHeat</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A17,"MaxGrowth",B17)</f>
         <v>UC_SRV_MaxGrowth_DistrictHeat</v>
@@ -7696,7 +7684,7 @@
         <v>SRV maximum growth rate of DistrictHeat</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A18,"MaxGrowth",B18)</f>
         <v>UC_SRV_MaxGrowth_Gas</v>
@@ -7736,7 +7724,7 @@
         <v>SRV maximum growth rate of Gas</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -7750,7 +7738,7 @@
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>117</v>
       </c>
@@ -7758,7 +7746,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>139</v>
       </c>
@@ -7772,7 +7760,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>139</v>
       </c>
@@ -7786,7 +7774,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>139</v>
       </c>
@@ -7797,10 +7785,10 @@
         <v>0.05</v>
       </c>
       <c r="D16">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>139</v>
       </c>
@@ -7814,7 +7802,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -7828,13 +7816,13 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="45" t="s">
         <v>215</v>
       </c>
       <c r="H22" s="46"/>
     </row>
-    <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="47" t="s">
         <v>216</v>
       </c>
@@ -7859,7 +7847,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D24" t="s">
         <v>219</v>
       </c>
@@ -7891,22 +7879,22 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" customWidth="1"/>
-    <col min="9" max="9" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3:D3)</f>
         <v>~UC_Sets: R_E: IE,National</v>
@@ -7924,7 +7912,7 @@
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -7941,7 +7929,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -7958,7 +7946,7 @@
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -7999,7 +7987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
         <f>_xlfn.TEXTJOIN("_",TRUE,"UC",A10,"MaxGrowth",B10)</f>
         <v>UC_RSD_MaxGrowth_Retrofits</v>
@@ -8037,7 +8025,7 @@
         <v>RSD maximum growth rate of retrofits</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>226</v>
       </c>
@@ -8067,7 +8055,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>117</v>
       </c>
@@ -8075,7 +8063,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>195</v>
       </c>
@@ -8103,23 +8091,23 @@
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5546875" customWidth="1"/>
-    <col min="14" max="14" width="13.5546875" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" customWidth="1"/>
-    <col min="16" max="16" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="str">
         <f>"~UC_Sets: R_E: " &amp; _xlfn.TEXTJOIN(",",TRUE,Regions!C3,Regions!E3:AD3)</f>
         <v>~UC_Sets: R_E: IE,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
@@ -8138,7 +8126,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -8156,7 +8144,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
     </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -8174,7 +8162,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
     </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -8215,7 +8203,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="str">
         <f t="shared" ref="B6:B23" si="0">IF(H27="*","*",_xlfn.TEXTJOIN("",TRUE,"UC-",I27,"_MaxGrowth",J27))</f>
         <v>UC-CAR_MaxGrowthBEV</v>
@@ -8256,7 +8244,7 @@
         <v>CARs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthPHEV</v>
@@ -8297,7 +8285,7 @@
         <v>CARs maximum growth rate of PHEVs</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthNG-ICE</v>
@@ -8338,7 +8326,7 @@
         <v>CARs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-CAR_MaxGrowthFCV</v>
@@ -8379,7 +8367,7 @@
         <v>CARs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthBEV</v>
@@ -8420,7 +8408,7 @@
         <v>LGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthPHEV</v>
@@ -8461,7 +8449,7 @@
         <v>LGTs maximum growth rate of PHEVs</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthNG-ICE</v>
@@ -8502,7 +8490,7 @@
         <v>LGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-LGT_MaxGrowthFCV</v>
@@ -8543,7 +8531,7 @@
         <v>LGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthBEV</v>
@@ -8584,7 +8572,7 @@
         <v>MGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthNG-ICE</v>
@@ -8625,7 +8613,7 @@
         <v>MGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthLNG-ICE</v>
@@ -8666,7 +8654,7 @@
         <v>MGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthHEV</v>
@@ -8707,7 +8695,7 @@
         <v>MGTs maximum growth rate of HEVs</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-MGT_MaxGrowthFCV</v>
@@ -8748,7 +8736,7 @@
         <v>MGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthBEV</v>
@@ -8789,7 +8777,7 @@
         <v>HGTs maximum growth rate of BEVs</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthNG-ICE</v>
@@ -8830,7 +8818,7 @@
         <v>HGTs maximum growth rate of NG-ICEs</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthLNG-ICE</v>
@@ -8871,7 +8859,7 @@
         <v>HGTs maximum growth rate of LNG-ICEs</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthHEV</v>
@@ -8913,7 +8901,7 @@
       </c>
       <c r="O22" s="2"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B23" s="18" t="str">
         <f t="shared" si="0"/>
         <v>UC-HGT_MaxGrowthFCV</v>
@@ -8954,7 +8942,7 @@
         <v>HGTs maximum growth rate of FCVs</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="H26" t="s">
         <v>152</v>
       </c>
@@ -8971,7 +8959,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I27" t="s">
         <v>147</v>
       </c>
@@ -8985,7 +8973,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>29</v>
       </c>
@@ -9002,7 +8990,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8" t="s">
@@ -9027,7 +9015,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="55" t="s">
         <v>27</v>
       </c>
@@ -9057,7 +9045,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="55"/>
       <c r="B31" t="s">
         <v>25</v>
@@ -9085,7 +9073,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="55"/>
       <c r="B32" t="s">
         <v>24</v>
@@ -9113,7 +9101,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="55"/>
       <c r="B33" t="s">
         <v>23</v>
@@ -9141,7 +9129,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="55"/>
       <c r="B34" t="s">
         <v>22</v>
@@ -9169,7 +9157,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="55"/>
       <c r="B35" t="s">
         <v>21</v>
@@ -9197,7 +9185,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>20</v>
       </c>
@@ -9224,7 +9212,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>19</v>
       </c>
@@ -9251,7 +9239,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>18</v>
       </c>
@@ -9278,7 +9266,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="5" t="s">
         <v>17</v>
@@ -9306,7 +9294,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -9323,7 +9311,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I41" t="s">
         <v>135</v>
       </c>
@@ -9337,7 +9325,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I42" t="s">
         <v>135</v>
       </c>
@@ -9351,7 +9339,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I43" t="s">
         <v>135</v>
       </c>
@@ -9365,7 +9353,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
         <v>135</v>
       </c>
@@ -9379,12 +9367,12 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>33</v>
       </c>
@@ -9392,7 +9380,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B47" s="11">
         <v>0.5</v>
       </c>
@@ -9400,7 +9388,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C48">
         <v>2018</v>
       </c>
@@ -9444,7 +9432,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>34</v>
       </c>
@@ -9488,7 +9476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>35</v>
       </c>
@@ -9553,7 +9541,7 @@
         <v>22797</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>36</v>
       </c>
@@ -9618,7 +9606,7 @@
         <v>11207</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -9683,7 +9671,7 @@
         <v>328695</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>38</v>
       </c>
@@ -9768,12 +9756,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087B74FDAF7A4FB4D876E5EA45926113E" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c45a71fd69a7f965f9452dfe567e395">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a32fc56-8470-4d77-ad86-bef2a7229878" xmlns:ns3="af10b6eb-1b35-481e-9f8a-8ff8d968e3bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e11456b9df302c9cdeb068d2abd9c51d" ns2:_="" ns3:_="">
     <xsd:import namespace="3a32fc56-8470-4d77-ad86-bef2a7229878"/>
@@ -9984,6 +9966,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
@@ -9993,15 +9981,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{00FA9C21-6103-4373-B43A-A6097DCED766}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10018,4 +9997,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>